<commit_message>
1st updated file - Assignment 2
</commit_message>
<xml_diff>
--- a/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
+++ b/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
@@ -4,47 +4,66 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Assignment 2" sheetId="4" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignment 1'!$A$17:$X$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Assignment 2'!$A$17:$X$17</definedName>
     <definedName name="abc" localSheetId="0">#REF!</definedName>
+    <definedName name="abc" localSheetId="1">#REF!</definedName>
     <definedName name="abc">#REF!</definedName>
     <definedName name="Check_inputed_mail_address" localSheetId="0">#REF!</definedName>
+    <definedName name="Check_inputed_mail_address" localSheetId="1">#REF!</definedName>
     <definedName name="Check_inputed_mail_address">#REF!</definedName>
     <definedName name="CS_IT_1.1_001" localSheetId="0">#REF!</definedName>
+    <definedName name="CS_IT_1.1_001" localSheetId="1">#REF!</definedName>
     <definedName name="CS_IT_1.1_001">#REF!</definedName>
     <definedName name="CS_IT_1.1_002" localSheetId="0">#REF!</definedName>
+    <definedName name="CS_IT_1.1_002" localSheetId="1">#REF!</definedName>
     <definedName name="CS_IT_1.1_002">#REF!</definedName>
     <definedName name="CS_IT_1.1_003" localSheetId="0">#REF!</definedName>
+    <definedName name="CS_IT_1.1_003" localSheetId="1">#REF!</definedName>
     <definedName name="CS_IT_1.1_003">#REF!</definedName>
     <definedName name="CS_IT_1.1_004" localSheetId="0">#REF!</definedName>
+    <definedName name="CS_IT_1.1_004" localSheetId="1">#REF!</definedName>
     <definedName name="CS_IT_1.1_004">#REF!</definedName>
     <definedName name="Evaluation" localSheetId="0">#REF!</definedName>
+    <definedName name="Evaluation" localSheetId="1">#REF!</definedName>
     <definedName name="Evaluation">#REF!</definedName>
     <definedName name="JaEnNickname" localSheetId="0">#REF!</definedName>
+    <definedName name="JaEnNickname" localSheetId="1">#REF!</definedName>
     <definedName name="JaEnNickname">#REF!</definedName>
     <definedName name="Mail_Magazine" localSheetId="0">#REF!</definedName>
+    <definedName name="Mail_Magazine" localSheetId="1">#REF!</definedName>
     <definedName name="Mail_Magazine">#REF!</definedName>
     <definedName name="project_code" localSheetId="0">#REF!</definedName>
+    <definedName name="project_code" localSheetId="1">#REF!</definedName>
     <definedName name="project_code">#REF!</definedName>
     <definedName name="ProjectName" localSheetId="0">'[1]Version 1'!#REF!</definedName>
+    <definedName name="ProjectName" localSheetId="1">'[1]Version 1'!#REF!</definedName>
     <definedName name="ProjectName">'[1]Version 1'!#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_001" localSheetId="0">#REF!</definedName>
+    <definedName name="Result_CS_IT_1.1_001" localSheetId="1">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_001">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_002" localSheetId="0">#REF!</definedName>
+    <definedName name="Result_CS_IT_1.1_002" localSheetId="1">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_002">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_003" localSheetId="0">#REF!</definedName>
+    <definedName name="Result_CS_IT_1.1_003" localSheetId="1">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_003">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_004" localSheetId="0">#REF!</definedName>
+    <definedName name="Result_CS_IT_1.1_004" localSheetId="1">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_004">#REF!</definedName>
     <definedName name="safa" localSheetId="0">#REF!</definedName>
+    <definedName name="safa" localSheetId="1">#REF!</definedName>
     <definedName name="safa">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -168,8 +187,96 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="F17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pass
+Fail
+Untested
+N/A
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pass
+Fail
+Untested
+N/A
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pass
+Fail
+Untested
+N/A
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F167" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Bug ID: 13057</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="241">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -665,6 +772,313 @@
   </si>
   <si>
     <t>Verify that the big photo frame switch from the last photo to the close-to-last photo</t>
+  </si>
+  <si>
+    <t>1. Check fields of Sign up with Email function</t>
+  </si>
+  <si>
+    <t>Check Email</t>
+  </si>
+  <si>
+    <t>When Email is in default status</t>
+  </si>
+  <si>
+    <t>When the user enters alphabetic characters into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters special characters into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters numeric characters into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters space in the middle of a valid characters
+string into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters space at the beginning and the end of a valid characters
+string into the Email box</t>
+  </si>
+  <si>
+    <t>When the user doesn't enter any character
+into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters a string of spaces into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters less than 10 valid characters into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters 10 valid characters into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters greater than 10 valid characters into the Email box</t>
+  </si>
+  <si>
+    <t>Check SMS Verification Code</t>
+  </si>
+  <si>
+    <t>When SMS Verification Code is in default status</t>
+  </si>
+  <si>
+    <t>When the user enters alphabetic characters into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user enters special characters into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user enters numeric characters into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user enters space in the middle of a valid characters
+string into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user enters space at the beginning and the end of a valid characters
+string into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user doesn't enter any character
+into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user enters a string of spaces into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user enters less than 6 valid characters into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user enters 6 valid characters into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user enters greater than 6 valid characters into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>Check Password</t>
+  </si>
+  <si>
+    <t>When Password is in default status</t>
+  </si>
+  <si>
+    <t>When the user enters alphabetic characters into the Password box</t>
+  </si>
+  <si>
+    <t>When the user enters special characters into the Password box</t>
+  </si>
+  <si>
+    <t>When the user enters numeric characters into the Password box</t>
+  </si>
+  <si>
+    <t>When the user enters a string that contains alphabetic and numeric characters into the Password box</t>
+  </si>
+  <si>
+    <t>When the user enters space in the middle of a valid characters string into the Password box</t>
+  </si>
+  <si>
+    <t>When the user enters space at the beginning and the end of a valid characters string into the Password box</t>
+  </si>
+  <si>
+    <t>When the user doesn't enter any character
+into the Password box</t>
+  </si>
+  <si>
+    <t>When the user enters a string of spaces into the Password box</t>
+  </si>
+  <si>
+    <t>When the user enters less than 6 valid characters into the Password box</t>
+  </si>
+  <si>
+    <t>When the user enters 6 valid characters into the Password box</t>
+  </si>
+  <si>
+    <t>When the user enters 50 valid characters into the Password box</t>
+  </si>
+  <si>
+    <t>When the user enters greater than 50 valid characters into the Password box</t>
+  </si>
+  <si>
+    <t>Check Eye icon in default status</t>
+  </si>
+  <si>
+    <t>When the user clicks on the Eye icon to show the password</t>
+  </si>
+  <si>
+    <t>When the user clicks on the Eye icon to hide the password</t>
+  </si>
+  <si>
+    <t>Check Birthday</t>
+  </si>
+  <si>
+    <t>When Birthday is in default status</t>
+  </si>
+  <si>
+    <t>When the user doesn't enter data</t>
+  </si>
+  <si>
+    <t>When the user enters valid date</t>
+  </si>
+  <si>
+    <t>When the user enters invalid date</t>
+  </si>
+  <si>
+    <t>Check Gender</t>
+  </si>
+  <si>
+    <t>When Gender is in default status</t>
+  </si>
+  <si>
+    <t>When the user enters valid value</t>
+  </si>
+  <si>
+    <t>Check Full Name</t>
+  </si>
+  <si>
+    <t>When Full Name is in default status</t>
+  </si>
+  <si>
+    <t>When the user enters alphabetic characters into the Full Name box</t>
+  </si>
+  <si>
+    <t>When the user enters special characters into the Full Name box</t>
+  </si>
+  <si>
+    <t>When the user enters numeric characters into the Full Name box</t>
+  </si>
+  <si>
+    <t>When the user enters space in the middle of a numeric characters
+string into the Full Name box</t>
+  </si>
+  <si>
+    <t>When the user enters space at the beginning and the end of a valid characters string into the Full Name box</t>
+  </si>
+  <si>
+    <t>When the user doesn't enter any character
+into the Full Name box</t>
+  </si>
+  <si>
+    <t>When the user enters a string of spaces into the Full Name box</t>
+  </si>
+  <si>
+    <t>When the user enters less than 6 valid characters into the Full Name box</t>
+  </si>
+  <si>
+    <t>When the user enters 6 valid characters into the Full Name box</t>
+  </si>
+  <si>
+    <t>When the user enters 50 valid characters into the Full Name box</t>
+  </si>
+  <si>
+    <t>When the user enters greater than 50 valid characters into the Full Name box</t>
+  </si>
+  <si>
+    <t>Check Checkbox</t>
+  </si>
+  <si>
+    <t>When Check box is in default status</t>
+  </si>
+  <si>
+    <t>When Check box is unchecked</t>
+  </si>
+  <si>
+    <t>When Check box is checked</t>
+  </si>
+  <si>
+    <t>2. Check fields of Sign up with Email function</t>
+  </si>
+  <si>
+    <t>When the user enters correct email format into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters incorrect email format into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters space in the middle of a valid characters string into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters space at the beginning and the end of a valid characters string into the Email box</t>
+  </si>
+  <si>
+    <t>When the user doesn't enter any character into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters less than 6 valid characters into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters 6 valid characters into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters 60 valid characters into the Email box</t>
+  </si>
+  <si>
+    <t>When the user enters greater than 60 valid characters into the Email box</t>
+  </si>
+  <si>
+    <t>Check Email Code</t>
+  </si>
+  <si>
+    <t>When Email Code is in default status</t>
+  </si>
+  <si>
+    <t>When the user enters alphabetic characters into the Email Code box</t>
+  </si>
+  <si>
+    <t>When the user enters special characters into the Email Code box</t>
+  </si>
+  <si>
+    <t>When the user enters numeric characters into the Email Code box</t>
+  </si>
+  <si>
+    <t>When the user enters space in the middle of a valid characters string into the Email Code box</t>
+  </si>
+  <si>
+    <t>When the user enters space at the beginning and the end of a valid characters string into the Email Code box</t>
+  </si>
+  <si>
+    <t>When the user doesn't enter any character
+into the Email Code box</t>
+  </si>
+  <si>
+    <t>When the user enters a string of spaces into the Email Code box</t>
+  </si>
+  <si>
+    <t>When the user enters less than 6 valid characters into the Email Code box</t>
+  </si>
+  <si>
+    <t>When the user enters 6 valid characters into the Email Code box</t>
+  </si>
+  <si>
+    <t>When the user enters greater than 6 valid characters into the Email Code box</t>
+  </si>
+  <si>
+    <t>3. Check Sign up function</t>
+  </si>
+  <si>
+    <t>Check Sign up with Email</t>
+  </si>
+  <si>
+    <t>When all fields are enters valid data</t>
+  </si>
+  <si>
+    <t>When the user enters a registered Email</t>
+  </si>
+  <si>
+    <t>When the user enters any invalid fields</t>
+  </si>
+  <si>
+    <t>When the user clicks on ‘Sign up with Email’ button</t>
+  </si>
+  <si>
+    <t>Check Sign up with Facebook</t>
+  </si>
+  <si>
+    <t>When the user clicks on ‘Facebook’ button</t>
+  </si>
+  <si>
+    <t>Check Sign up with Google</t>
+  </si>
+  <si>
+    <t>When the user clicks on ‘Google’ button</t>
   </si>
 </sst>
 </file>
@@ -964,7 +1378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1143,6 +1557,66 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1183,6 +1657,21 @@
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Assignment 1"/>
+      <sheetName val="Assignment 2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1453,7 +1942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
@@ -18983,4 +19472,2690 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X167"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="12" style="36" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="37" customWidth="1"/>
+    <col min="3" max="4" width="35.140625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" style="37" customWidth="1"/>
+    <col min="6" max="8" width="9.7109375" style="37" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="37" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="4" customFormat="1" ht="14.25">
+      <c r="A1" s="60"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:24" s="4" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A2" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:24" s="4" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:24" s="9" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A4" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="X4" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="9" customFormat="1" ht="144.75" customHeight="1">
+      <c r="A5" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="X5" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" s="9" customFormat="1" ht="25.5">
+      <c r="A6" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:24" s="9" customFormat="1">
+      <c r="A7" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="8"/>
+      <c r="X7" s="11"/>
+    </row>
+    <row r="8" spans="1:24" s="12" customFormat="1">
+      <c r="A8" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+    </row>
+    <row r="9" spans="1:24" s="12" customFormat="1">
+      <c r="A9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="13" t="str">
+        <f>F17</f>
+        <v>Internal Build 03112011</v>
+      </c>
+      <c r="C9" s="13" t="str">
+        <f>G17</f>
+        <v>Internal build 14112011</v>
+      </c>
+      <c r="D9" s="13" t="str">
+        <f>H17</f>
+        <v>External build 16112011</v>
+      </c>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+    </row>
+    <row r="10" spans="1:24" s="12" customFormat="1">
+      <c r="A10" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="14">
+        <f>SUM(B11:B14)</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="14">
+        <f>SUM(C11:C14)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="14">
+        <f>SUM(D11:D14)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+    </row>
+    <row r="11" spans="1:24" s="12" customFormat="1">
+      <c r="A11" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="15">
+        <f>COUNTIF($F$18:$F$167,"*Passed")</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
+        <f>COUNTIF($G$18:$G$167,"*Passed")</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="15">
+        <f>COUNTIF($H$18:$H$167,"*Passed")</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+    </row>
+    <row r="12" spans="1:24" s="12" customFormat="1">
+      <c r="A12" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="15">
+        <f>COUNTIF($F$18:$F$167,"*Failed*")</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="15">
+        <f>COUNTIF($G$18:$G$167,"*Failed*")</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="15">
+        <f>COUNTIF($H$18:$H$167,"*Failed*")</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+    </row>
+    <row r="13" spans="1:24" s="12" customFormat="1">
+      <c r="A13" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="15">
+        <f>COUNTIF($F$18:$F$167,"*Not Run*")</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="15">
+        <f>COUNTIF($G$18:$G$167,"*Not Run*")</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="15">
+        <f>COUNTIF($H$18:$H$167,"*Not Run*")</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:24" s="12" customFormat="1">
+      <c r="A14" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="15">
+        <f>COUNTIF($F$18:$F$167,"*NA*")</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="15">
+        <f>COUNTIF($G$18:$G$167,"*NA*")</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="15">
+        <f>COUNTIF($H$18:$H$167,"*NA*")</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:24" s="12" customFormat="1" ht="38.25">
+      <c r="A15" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="15">
+        <f>COUNTIF($F$18:$F$167,"*Passed in previous build*")</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="15">
+        <f>COUNTIF($G$18:$G$167,"*Passed in previous build*")</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="15">
+        <f>COUNTIF($H$18:$H$167,"*Passed in previous build*")</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:24" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="69"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="1:9" s="21" customFormat="1" ht="38.25">
+      <c r="A17" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A18" s="71"/>
+      <c r="B18" s="72" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="73"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="71"/>
+    </row>
+    <row r="19" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A19" s="43"/>
+      <c r="B19" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" s="76"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="78"/>
+    </row>
+    <row r="20" spans="1:9" s="27" customFormat="1">
+      <c r="A20" s="80">
+        <f t="shared" ref="A20:A83" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A21" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A22" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A23" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B23" s="81" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A24" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="26"/>
+    </row>
+    <row r="25" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A25" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="26"/>
+    </row>
+    <row r="26" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A26" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="82"/>
+    </row>
+    <row r="27" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A27" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="26"/>
+    </row>
+    <row r="28" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A28" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="82"/>
+    </row>
+    <row r="29" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A29" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="82"/>
+    </row>
+    <row r="30" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A30" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="82"/>
+    </row>
+    <row r="31" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A31" s="43"/>
+      <c r="B31" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="78"/>
+    </row>
+    <row r="32" spans="1:9" s="27" customFormat="1">
+      <c r="A32" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="26"/>
+    </row>
+    <row r="33" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A33" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" s="24"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="26"/>
+    </row>
+    <row r="34" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A34" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="26"/>
+    </row>
+    <row r="35" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A35" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B35" s="81" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="26"/>
+    </row>
+    <row r="36" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A36" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="26"/>
+    </row>
+    <row r="37" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A37" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="26"/>
+    </row>
+    <row r="38" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A38" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="26"/>
+    </row>
+    <row r="39" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A39" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="82"/>
+    </row>
+    <row r="40" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A40" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="82"/>
+    </row>
+    <row r="41" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A41" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="82"/>
+    </row>
+    <row r="42" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A42" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="82"/>
+    </row>
+    <row r="43" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A43" s="43"/>
+      <c r="B43" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="76"/>
+      <c r="D43" s="77"/>
+      <c r="E43" s="78"/>
+      <c r="F43" s="79"/>
+      <c r="G43" s="79"/>
+      <c r="H43" s="79"/>
+      <c r="I43" s="78"/>
+    </row>
+    <row r="44" spans="1:9" s="27" customFormat="1">
+      <c r="A44" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="26"/>
+    </row>
+    <row r="45" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A45" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="26"/>
+    </row>
+    <row r="46" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A46" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="24"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="26"/>
+    </row>
+    <row r="47" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A47" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="26"/>
+    </row>
+    <row r="48" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A48" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="26"/>
+    </row>
+    <row r="49" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A49" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="26"/>
+    </row>
+    <row r="50" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A50" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="26"/>
+    </row>
+    <row r="51" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A51" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="26"/>
+    </row>
+    <row r="52" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A52" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="82"/>
+    </row>
+    <row r="53" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A53" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="82"/>
+    </row>
+    <row r="54" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A54" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="82"/>
+    </row>
+    <row r="55" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A55" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="82"/>
+    </row>
+    <row r="56" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A56" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="82"/>
+    </row>
+    <row r="57" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A57" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="82"/>
+    </row>
+    <row r="58" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A58" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="82"/>
+    </row>
+    <row r="59" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A59" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="82"/>
+    </row>
+    <row r="60" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A60" s="43"/>
+      <c r="B60" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="C60" s="76"/>
+      <c r="D60" s="77"/>
+      <c r="E60" s="78"/>
+      <c r="F60" s="79"/>
+      <c r="G60" s="79"/>
+      <c r="H60" s="79"/>
+      <c r="I60" s="78"/>
+    </row>
+    <row r="61" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A61" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="82"/>
+    </row>
+    <row r="62" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A62" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="82"/>
+    </row>
+    <row r="63" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A63" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="82"/>
+    </row>
+    <row r="64" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A64" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="82"/>
+    </row>
+    <row r="65" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A65" s="43"/>
+      <c r="B65" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="C65" s="76"/>
+      <c r="D65" s="77"/>
+      <c r="E65" s="78"/>
+      <c r="F65" s="79"/>
+      <c r="G65" s="79"/>
+      <c r="H65" s="79"/>
+      <c r="I65" s="78"/>
+    </row>
+    <row r="66" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A66" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="82"/>
+    </row>
+    <row r="67" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A67" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="82"/>
+    </row>
+    <row r="68" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A68" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="82"/>
+    </row>
+    <row r="69" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A69" s="43"/>
+      <c r="B69" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" s="76"/>
+      <c r="D69" s="77"/>
+      <c r="E69" s="78"/>
+      <c r="F69" s="79"/>
+      <c r="G69" s="79"/>
+      <c r="H69" s="79"/>
+      <c r="I69" s="78"/>
+    </row>
+    <row r="70" spans="1:9" s="27" customFormat="1">
+      <c r="A70" s="80">
+        <f t="shared" ref="A70:A81" ca="1" si="1">IF(OFFSET(A70,-1,0) ="",OFFSET(A70,-2,0)+1,OFFSET(A70,-1,0)+1 )</f>
+        <v>46</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="26"/>
+    </row>
+    <row r="71" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A71" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D71" s="24"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="26"/>
+    </row>
+    <row r="72" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A72" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="26"/>
+    </row>
+    <row r="73" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A73" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B73" s="81" t="s">
+        <v>196</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="25"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="26"/>
+    </row>
+    <row r="74" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A74" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="25"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="26"/>
+    </row>
+    <row r="75" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A75" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="25"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="26"/>
+    </row>
+    <row r="76" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A76" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="25"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="82"/>
+    </row>
+    <row r="77" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A77" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="25"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="26"/>
+    </row>
+    <row r="78" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A78" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="25"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="82"/>
+    </row>
+    <row r="79" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A79" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="82"/>
+    </row>
+    <row r="80" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A80" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="82"/>
+    </row>
+    <row r="81" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A81" s="80">
+        <f t="shared" ca="1" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="82"/>
+    </row>
+    <row r="82" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A82" s="43"/>
+      <c r="B82" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="C82" s="76"/>
+      <c r="D82" s="77"/>
+      <c r="E82" s="78"/>
+      <c r="F82" s="79"/>
+      <c r="G82" s="79"/>
+      <c r="H82" s="79"/>
+      <c r="I82" s="78"/>
+    </row>
+    <row r="83" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A83" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="25"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="82"/>
+    </row>
+    <row r="84" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A84" s="80">
+        <f t="shared" ref="A84:A192" ca="1" si="2">IF(OFFSET(A84,-1,0) ="",OFFSET(A84,-2,0)+1,OFFSET(A84,-1,0)+1 )</f>
+        <v>59</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="25"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="82"/>
+    </row>
+    <row r="85" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A85" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="82"/>
+    </row>
+    <row r="86" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A86" s="71"/>
+      <c r="B86" s="72" t="s">
+        <v>209</v>
+      </c>
+      <c r="C86" s="73"/>
+      <c r="D86" s="74"/>
+      <c r="E86" s="71"/>
+      <c r="F86" s="75"/>
+      <c r="G86" s="75"/>
+      <c r="H86" s="75"/>
+      <c r="I86" s="71"/>
+    </row>
+    <row r="87" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A87" s="43"/>
+      <c r="B87" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C87" s="76"/>
+      <c r="D87" s="77"/>
+      <c r="E87" s="78"/>
+      <c r="F87" s="79"/>
+      <c r="G87" s="79"/>
+      <c r="H87" s="79"/>
+      <c r="I87" s="78"/>
+    </row>
+    <row r="88" spans="1:9" s="27" customFormat="1">
+      <c r="A88" s="80">
+        <f ca="1">A85+1</f>
+        <v>61</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C88" s="1"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="26"/>
+    </row>
+    <row r="89" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A89" s="80">
+        <f t="shared" ref="A88:A124" ca="1" si="3">IF(OFFSET(A89,-1,0) ="",OFFSET(A89,-2,0)+1,OFFSET(A89,-1,0)+1 )</f>
+        <v>62</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D89" s="24"/>
+      <c r="E89" s="25"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="26"/>
+    </row>
+    <row r="90" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A90" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="25"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="26"/>
+    </row>
+    <row r="91" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A91" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="25"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="26"/>
+    </row>
+    <row r="92" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A92" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="25"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="26"/>
+    </row>
+    <row r="93" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A93" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C93" s="1"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="25"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="82"/>
+    </row>
+    <row r="94" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A94" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C94" s="1"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="26"/>
+    </row>
+    <row r="95" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A95" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C95" s="1"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="25"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="82"/>
+    </row>
+    <row r="96" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A96" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="24"/>
+      <c r="E96" s="25"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="82"/>
+    </row>
+    <row r="97" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A97" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C97" s="1"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="25"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="82"/>
+    </row>
+    <row r="98" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A98" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C98" s="1"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="25"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="82"/>
+    </row>
+    <row r="99" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A99" s="43"/>
+      <c r="B99" s="53" t="s">
+        <v>219</v>
+      </c>
+      <c r="C99" s="76"/>
+      <c r="D99" s="77"/>
+      <c r="E99" s="78"/>
+      <c r="F99" s="79"/>
+      <c r="G99" s="79"/>
+      <c r="H99" s="79"/>
+      <c r="I99" s="78"/>
+    </row>
+    <row r="100" spans="1:9" s="27" customFormat="1">
+      <c r="A100" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C100" s="1"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="26"/>
+    </row>
+    <row r="101" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A101" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D101" s="24"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="26"/>
+    </row>
+    <row r="102" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A102" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="D102" s="24"/>
+      <c r="E102" s="25"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="26"/>
+    </row>
+    <row r="103" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A103" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="B103" s="81" t="s">
+        <v>223</v>
+      </c>
+      <c r="C103" s="1"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="25"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="26"/>
+    </row>
+    <row r="104" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A104" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>76</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C104" s="1"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="26"/>
+    </row>
+    <row r="105" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A105" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C105" s="1"/>
+      <c r="D105" s="24"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="26"/>
+    </row>
+    <row r="106" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A106" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C106" s="1"/>
+      <c r="D106" s="24"/>
+      <c r="E106" s="25"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="26"/>
+    </row>
+    <row r="107" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A107" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C107" s="1"/>
+      <c r="D107" s="24"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="82"/>
+    </row>
+    <row r="108" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A108" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="24"/>
+      <c r="E108" s="25"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="82"/>
+    </row>
+    <row r="109" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A109" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C109" s="1"/>
+      <c r="D109" s="24"/>
+      <c r="E109" s="25"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="82"/>
+    </row>
+    <row r="110" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A110" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C110" s="1"/>
+      <c r="D110" s="24"/>
+      <c r="E110" s="25"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="82"/>
+    </row>
+    <row r="111" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A111" s="43"/>
+      <c r="B111" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C111" s="76"/>
+      <c r="D111" s="77"/>
+      <c r="E111" s="78"/>
+      <c r="F111" s="79"/>
+      <c r="G111" s="79"/>
+      <c r="H111" s="79"/>
+      <c r="I111" s="78"/>
+    </row>
+    <row r="112" spans="1:9" s="27" customFormat="1">
+      <c r="A112" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C112" s="1"/>
+      <c r="D112" s="24"/>
+      <c r="E112" s="25"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="26"/>
+    </row>
+    <row r="113" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A113" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C113" s="1"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="25"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="26"/>
+    </row>
+    <row r="114" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A114" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D114" s="24"/>
+      <c r="E114" s="25"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="26"/>
+    </row>
+    <row r="115" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A115" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>86</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C115" s="1"/>
+      <c r="D115" s="24"/>
+      <c r="E115" s="25"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="26"/>
+    </row>
+    <row r="116" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A116" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C116" s="1"/>
+      <c r="D116" s="24"/>
+      <c r="E116" s="25"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="26"/>
+    </row>
+    <row r="117" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A117" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C117" s="1"/>
+      <c r="D117" s="24"/>
+      <c r="E117" s="25"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="26"/>
+    </row>
+    <row r="118" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A118" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C118" s="1"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="25"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="26"/>
+    </row>
+    <row r="119" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A119" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C119" s="1"/>
+      <c r="D119" s="24"/>
+      <c r="E119" s="25"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="26"/>
+    </row>
+    <row r="120" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A120" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C120" s="1"/>
+      <c r="D120" s="24"/>
+      <c r="E120" s="25"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="82"/>
+    </row>
+    <row r="121" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A121" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>92</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C121" s="1"/>
+      <c r="D121" s="24"/>
+      <c r="E121" s="25"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="82"/>
+    </row>
+    <row r="122" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A122" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C122" s="1"/>
+      <c r="D122" s="24"/>
+      <c r="E122" s="25"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="82"/>
+    </row>
+    <row r="123" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A123" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>94</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C123" s="1"/>
+      <c r="D123" s="24"/>
+      <c r="E123" s="25"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="82"/>
+    </row>
+    <row r="124" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A124" s="80">
+        <f t="shared" ca="1" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C124" s="1"/>
+      <c r="D124" s="24"/>
+      <c r="E124" s="25"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="82"/>
+    </row>
+    <row r="125" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A125" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C125" s="1"/>
+      <c r="D125" s="24"/>
+      <c r="E125" s="25"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="82"/>
+    </row>
+    <row r="126" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A126" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C126" s="1"/>
+      <c r="D126" s="24"/>
+      <c r="E126" s="25"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="82"/>
+    </row>
+    <row r="127" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A127" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C127" s="1"/>
+      <c r="D127" s="24"/>
+      <c r="E127" s="25"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="82"/>
+    </row>
+    <row r="128" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A128" s="43"/>
+      <c r="B128" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="C128" s="76"/>
+      <c r="D128" s="77"/>
+      <c r="E128" s="78"/>
+      <c r="F128" s="79"/>
+      <c r="G128" s="79"/>
+      <c r="H128" s="79"/>
+      <c r="I128" s="78"/>
+    </row>
+    <row r="129" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A129" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C129" s="1"/>
+      <c r="D129" s="24"/>
+      <c r="E129" s="25"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+      <c r="I129" s="82"/>
+    </row>
+    <row r="130" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A130" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C130" s="1"/>
+      <c r="D130" s="24"/>
+      <c r="E130" s="25"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="82"/>
+    </row>
+    <row r="131" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A131" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C131" s="1"/>
+      <c r="D131" s="24"/>
+      <c r="E131" s="25"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="82"/>
+    </row>
+    <row r="132" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A132" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C132" s="1"/>
+      <c r="D132" s="24"/>
+      <c r="E132" s="25"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="82"/>
+    </row>
+    <row r="133" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A133" s="43"/>
+      <c r="B133" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="C133" s="76"/>
+      <c r="D133" s="77"/>
+      <c r="E133" s="78"/>
+      <c r="F133" s="79"/>
+      <c r="G133" s="79"/>
+      <c r="H133" s="79"/>
+      <c r="I133" s="78"/>
+    </row>
+    <row r="134" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A134" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C134" s="1"/>
+      <c r="D134" s="24"/>
+      <c r="E134" s="25"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="82"/>
+    </row>
+    <row r="135" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A135" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C135" s="1"/>
+      <c r="D135" s="24"/>
+      <c r="E135" s="25"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="82"/>
+    </row>
+    <row r="136" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A136" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C136" s="1"/>
+      <c r="D136" s="24"/>
+      <c r="E136" s="25"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="1"/>
+      <c r="H136" s="1"/>
+      <c r="I136" s="82"/>
+    </row>
+    <row r="137" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A137" s="43"/>
+      <c r="B137" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="C137" s="76"/>
+      <c r="D137" s="77"/>
+      <c r="E137" s="78"/>
+      <c r="F137" s="79"/>
+      <c r="G137" s="79"/>
+      <c r="H137" s="79"/>
+      <c r="I137" s="78"/>
+    </row>
+    <row r="138" spans="1:9" s="27" customFormat="1">
+      <c r="A138" s="80">
+        <f t="shared" ref="A138:A149" ca="1" si="4">IF(OFFSET(A138,-1,0) ="",OFFSET(A138,-2,0)+1,OFFSET(A138,-1,0)+1 )</f>
+        <v>106</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C138" s="1"/>
+      <c r="D138" s="24"/>
+      <c r="E138" s="25"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="26"/>
+    </row>
+    <row r="139" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A139" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>107</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D139" s="24"/>
+      <c r="E139" s="25"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+      <c r="I139" s="26"/>
+    </row>
+    <row r="140" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A140" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>108</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C140" s="1"/>
+      <c r="D140" s="24"/>
+      <c r="E140" s="25"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
+      <c r="I140" s="26"/>
+    </row>
+    <row r="141" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A141" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>109</v>
+      </c>
+      <c r="B141" s="81" t="s">
+        <v>196</v>
+      </c>
+      <c r="C141" s="1"/>
+      <c r="D141" s="24"/>
+      <c r="E141" s="25"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+      <c r="I141" s="26"/>
+    </row>
+    <row r="142" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A142" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>110</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C142" s="1"/>
+      <c r="D142" s="24"/>
+      <c r="E142" s="25"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+      <c r="I142" s="26"/>
+    </row>
+    <row r="143" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A143" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>111</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C143" s="1"/>
+      <c r="D143" s="24"/>
+      <c r="E143" s="25"/>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+      <c r="I143" s="26"/>
+    </row>
+    <row r="144" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A144" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>112</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C144" s="1"/>
+      <c r="D144" s="24"/>
+      <c r="E144" s="25"/>
+      <c r="F144" s="1"/>
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
+      <c r="I144" s="82"/>
+    </row>
+    <row r="145" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A145" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>113</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C145" s="1"/>
+      <c r="D145" s="24"/>
+      <c r="E145" s="25"/>
+      <c r="F145" s="1"/>
+      <c r="G145" s="1"/>
+      <c r="H145" s="1"/>
+      <c r="I145" s="26"/>
+    </row>
+    <row r="146" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A146" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>114</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C146" s="1"/>
+      <c r="D146" s="24"/>
+      <c r="E146" s="25"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+      <c r="I146" s="82"/>
+    </row>
+    <row r="147" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A147" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>115</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C147" s="1"/>
+      <c r="D147" s="24"/>
+      <c r="E147" s="25"/>
+      <c r="F147" s="1"/>
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
+      <c r="I147" s="82"/>
+    </row>
+    <row r="148" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A148" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>116</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C148" s="1"/>
+      <c r="D148" s="24"/>
+      <c r="E148" s="25"/>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
+      <c r="I148" s="82"/>
+    </row>
+    <row r="149" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A149" s="80">
+        <f t="shared" ca="1" si="4"/>
+        <v>117</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C149" s="1"/>
+      <c r="D149" s="24"/>
+      <c r="E149" s="25"/>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
+      <c r="I149" s="82"/>
+    </row>
+    <row r="150" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A150" s="43"/>
+      <c r="B150" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="C150" s="76"/>
+      <c r="D150" s="77"/>
+      <c r="E150" s="78"/>
+      <c r="F150" s="79"/>
+      <c r="G150" s="79"/>
+      <c r="H150" s="79"/>
+      <c r="I150" s="78"/>
+    </row>
+    <row r="151" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A151" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C151" s="1"/>
+      <c r="D151" s="24"/>
+      <c r="E151" s="25"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="82"/>
+    </row>
+    <row r="152" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A152" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C152" s="1"/>
+      <c r="D152" s="24"/>
+      <c r="E152" s="25"/>
+      <c r="F152" s="1"/>
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
+      <c r="I152" s="82"/>
+    </row>
+    <row r="153" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A153" s="80">
+        <f t="shared" ca="1" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C153" s="1"/>
+      <c r="D153" s="24"/>
+      <c r="E153" s="25"/>
+      <c r="F153" s="1"/>
+      <c r="G153" s="1"/>
+      <c r="H153" s="1"/>
+      <c r="I153" s="82"/>
+    </row>
+    <row r="154" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A154" s="83"/>
+      <c r="B154" s="72" t="s">
+        <v>231</v>
+      </c>
+      <c r="C154" s="73"/>
+      <c r="D154" s="74"/>
+      <c r="E154" s="84"/>
+      <c r="F154" s="32"/>
+      <c r="G154" s="32"/>
+      <c r="H154" s="32"/>
+      <c r="I154" s="84"/>
+    </row>
+    <row r="155" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A155" s="43"/>
+      <c r="B155" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="C155" s="76"/>
+      <c r="D155" s="77"/>
+      <c r="E155" s="78"/>
+      <c r="F155" s="79"/>
+      <c r="G155" s="79"/>
+      <c r="H155" s="79"/>
+      <c r="I155" s="78"/>
+    </row>
+    <row r="156" spans="1:9" s="27" customFormat="1">
+      <c r="A156" s="80">
+        <f ca="1">A153+1</f>
+        <v>121</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C156" s="1"/>
+      <c r="D156" s="24"/>
+      <c r="E156" s="25"/>
+      <c r="F156" s="1"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="26"/>
+    </row>
+    <row r="157" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A157" s="80">
+        <f ca="1">IF(OFFSET(A157,-1,0) ="",OFFSET(A157,-2,0)+1,OFFSET(A157,-1,0)+1 )</f>
+        <v>122</v>
+      </c>
+      <c r="B157" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="C157" s="1"/>
+      <c r="D157" s="85"/>
+      <c r="E157" s="25"/>
+      <c r="F157" s="1"/>
+      <c r="G157" s="1"/>
+      <c r="H157" s="1"/>
+      <c r="I157" s="82"/>
+    </row>
+    <row r="158" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A158" s="80">
+        <f ca="1">IF(OFFSET(A158,-1,0) ="",OFFSET(A158,-2,0)+1,OFFSET(A158,-1,0)+1 )</f>
+        <v>123</v>
+      </c>
+      <c r="B158" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="C158" s="86"/>
+      <c r="D158" s="85"/>
+      <c r="E158" s="25"/>
+      <c r="F158" s="1"/>
+      <c r="G158" s="1"/>
+      <c r="H158" s="1"/>
+      <c r="I158" s="82"/>
+    </row>
+    <row r="159" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A159" s="43"/>
+      <c r="B159" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="C159" s="76"/>
+      <c r="D159" s="77"/>
+      <c r="E159" s="78"/>
+      <c r="F159" s="79"/>
+      <c r="G159" s="79"/>
+      <c r="H159" s="79"/>
+      <c r="I159" s="78"/>
+    </row>
+    <row r="160" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A160" s="80">
+        <f t="shared" ref="A160:A163" ca="1" si="5">IF(OFFSET(A160,-1,0) ="",OFFSET(A160,-2,0)+1,OFFSET(A160,-1,0)+1 )</f>
+        <v>124</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C160" s="1"/>
+      <c r="D160" s="24"/>
+      <c r="E160" s="25"/>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
+      <c r="I160" s="82"/>
+    </row>
+    <row r="161" spans="1:9" s="27" customFormat="1">
+      <c r="A161" s="80">
+        <f t="shared" ca="1" si="5"/>
+        <v>125</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C161" s="1"/>
+      <c r="D161" s="24"/>
+      <c r="E161" s="25"/>
+      <c r="F161" s="1"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1"/>
+      <c r="I161" s="26"/>
+    </row>
+    <row r="162" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A162" s="80">
+        <f t="shared" ca="1" si="5"/>
+        <v>126</v>
+      </c>
+      <c r="B162" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="C162" s="1"/>
+      <c r="D162" s="85"/>
+      <c r="E162" s="25"/>
+      <c r="F162" s="1"/>
+      <c r="G162" s="1"/>
+      <c r="H162" s="1"/>
+      <c r="I162" s="82"/>
+    </row>
+    <row r="163" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A163" s="80">
+        <f t="shared" ca="1" si="5"/>
+        <v>127</v>
+      </c>
+      <c r="B163" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="C163" s="86"/>
+      <c r="D163" s="85"/>
+      <c r="E163" s="25"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="1"/>
+      <c r="H163" s="1"/>
+      <c r="I163" s="82"/>
+    </row>
+    <row r="164" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A164" s="43"/>
+      <c r="B164" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="C164" s="76"/>
+      <c r="D164" s="77"/>
+      <c r="E164" s="78"/>
+      <c r="F164" s="79"/>
+      <c r="G164" s="79"/>
+      <c r="H164" s="79"/>
+      <c r="I164" s="78"/>
+    </row>
+    <row r="165" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A165" s="87">
+        <f t="shared" ca="1" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C165" s="1"/>
+      <c r="D165" s="24"/>
+      <c r="E165" s="25"/>
+      <c r="F165" s="25"/>
+      <c r="G165" s="1"/>
+      <c r="H165" s="1"/>
+      <c r="I165" s="87"/>
+    </row>
+    <row r="166" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A166" s="43"/>
+      <c r="B166" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="C166" s="76"/>
+      <c r="D166" s="77"/>
+      <c r="E166" s="78"/>
+      <c r="F166" s="79"/>
+      <c r="G166" s="79"/>
+      <c r="H166" s="79"/>
+      <c r="I166" s="78"/>
+    </row>
+    <row r="167" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A167" s="87">
+        <f t="shared" ref="A167" ca="1" si="6">IF(OFFSET(A167,-1,0) ="",OFFSET(A167,-2,0)+1,OFFSET(A167,-1,0)+1 )</f>
+        <v>129</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C167" s="1"/>
+      <c r="D167" s="24"/>
+      <c r="E167" s="25"/>
+      <c r="F167" s="25"/>
+      <c r="G167" s="1"/>
+      <c r="H167" s="1"/>
+      <c r="I167" s="87"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B154:D154"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F60:H60 F18:H19 F166:H166 F65:H65 F82:H82 F31:H31 F43:H43 F155:H155 F159:H159 F164:H164 F69:H69 F128:H128 F86:H87 F133:H133 F150:H150 F99:H99 F111:H111 F137:H137"/>
+    <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
+    <dataValidation type="list" allowBlank="1" sqref="F61:H64 F66:H68 F44:H59 F32:H42 F70:H81 F165:H165 F167:H167 F156:H158 F20:H30 F83:H85 F151:H154 F129:H132 F134:H136 F112:H127 F100:H110 F138:H149 F160:H163 F88:H98">
+      <formula1>$A$11:$A$15</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2rd updated file - Assignment 2
</commit_message>
<xml_diff>
--- a/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
+++ b/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
@@ -12,7 +12,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
-    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignment 1'!$A$17:$X$17</definedName>
@@ -247,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F167" authorId="0" shapeId="0">
+    <comment ref="F96" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -276,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="220">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -774,48 +773,6 @@
     <t>Verify that the big photo frame switch from the last photo to the close-to-last photo</t>
   </si>
   <si>
-    <t>1. Check fields of Sign up with Email function</t>
-  </si>
-  <si>
-    <t>Check Email</t>
-  </si>
-  <si>
-    <t>When Email is in default status</t>
-  </si>
-  <si>
-    <t>When the user enters alphabetic characters into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters special characters into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters numeric characters into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters space in the middle of a valid characters
-string into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters space at the beginning and the end of a valid characters
-string into the Email box</t>
-  </si>
-  <si>
-    <t>When the user doesn't enter any character
-into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters a string of spaces into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters less than 10 valid characters into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters 10 valid characters into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters greater than 10 valid characters into the Email box</t>
-  </si>
-  <si>
     <t>Check SMS Verification Code</t>
   </si>
   <si>
@@ -829,14 +786,6 @@
   </si>
   <si>
     <t>When the user enters numeric characters into the SMS Verification Code box</t>
-  </si>
-  <si>
-    <t>When the user enters space in the middle of a valid characters
-string into the SMS Verification Code box</t>
-  </si>
-  <si>
-    <t>When the user enters space at the beginning and the end of a valid characters
-string into the SMS Verification Code box</t>
   </si>
   <si>
     <t>When the user doesn't enter any character
@@ -984,85 +933,12 @@
     <t>When Check box is checked</t>
   </si>
   <si>
-    <t>2. Check fields of Sign up with Email function</t>
-  </si>
-  <si>
-    <t>When the user enters correct email format into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters incorrect email format into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters space in the middle of a valid characters string into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters space at the beginning and the end of a valid characters string into the Email box</t>
-  </si>
-  <si>
-    <t>When the user doesn't enter any character into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters less than 6 valid characters into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters 6 valid characters into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters 60 valid characters into the Email box</t>
-  </si>
-  <si>
-    <t>When the user enters greater than 60 valid characters into the Email box</t>
-  </si>
-  <si>
-    <t>Check Email Code</t>
-  </si>
-  <si>
-    <t>When Email Code is in default status</t>
-  </si>
-  <si>
-    <t>When the user enters alphabetic characters into the Email Code box</t>
-  </si>
-  <si>
-    <t>When the user enters special characters into the Email Code box</t>
-  </si>
-  <si>
-    <t>When the user enters numeric characters into the Email Code box</t>
-  </si>
-  <si>
-    <t>When the user enters space in the middle of a valid characters string into the Email Code box</t>
-  </si>
-  <si>
-    <t>When the user enters space at the beginning and the end of a valid characters string into the Email Code box</t>
-  </si>
-  <si>
-    <t>When the user doesn't enter any character
-into the Email Code box</t>
-  </si>
-  <si>
-    <t>When the user enters a string of spaces into the Email Code box</t>
-  </si>
-  <si>
-    <t>When the user enters less than 6 valid characters into the Email Code box</t>
-  </si>
-  <si>
-    <t>When the user enters 6 valid characters into the Email Code box</t>
-  </si>
-  <si>
-    <t>When the user enters greater than 6 valid characters into the Email Code box</t>
-  </si>
-  <si>
-    <t>3. Check Sign up function</t>
-  </si>
-  <si>
     <t>Check Sign up with Email</t>
   </si>
   <si>
     <t>When all fields are enters valid data</t>
   </si>
   <si>
-    <t>When the user enters a registered Email</t>
-  </si>
-  <si>
     <t>When the user enters any invalid fields</t>
   </si>
   <si>
@@ -1079,6 +955,60 @@
   </si>
   <si>
     <t>When the user clicks on ‘Google’ button</t>
+  </si>
+  <si>
+    <t>1. Check fields of Sign up with Phone number function</t>
+  </si>
+  <si>
+    <t>2. Check Sign up function</t>
+  </si>
+  <si>
+    <t>Check Phone Number</t>
+  </si>
+  <si>
+    <t>When Phone number is in default status</t>
+  </si>
+  <si>
+    <t>When the user enters alphabetic characters into the Phone number box</t>
+  </si>
+  <si>
+    <t>When the user enters special characters into the Phone number box</t>
+  </si>
+  <si>
+    <t>When the user enters numeric characters into the Phone number box</t>
+  </si>
+  <si>
+    <t>When the user enters a string of spaces into the Phone number box</t>
+  </si>
+  <si>
+    <t>When the user enters less than 10 valid characters into the Phone number box</t>
+  </si>
+  <si>
+    <t>When the user enters 10 valid characters into the Phone number box</t>
+  </si>
+  <si>
+    <t>When the user enters greater than 10 valid characters into the Phone number box</t>
+  </si>
+  <si>
+    <t>When the user enters space in the middle of a valid characters string into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user enters space at the beginning and the end of a valid characters string into the SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>When the user enters space in the middle of a valid characters string into the Phone number box</t>
+  </si>
+  <si>
+    <t>When the user enters space at the beginning and the end of a valid characters string into the Phone number box</t>
+  </si>
+  <si>
+    <t>When the user doesn't enter any character into the Phone number box</t>
+  </si>
+  <si>
+    <t>Check Sign up with Phone Number</t>
+  </si>
+  <si>
+    <t>When the user enters a registered Phone Number</t>
   </si>
 </sst>
 </file>
@@ -1521,42 +1451,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1568,15 +1462,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1616,6 +1501,51 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1657,21 +1587,6 @@
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Assignment 1"/>
-      <sheetName val="Assignment 2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1958,10 +1873,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" ht="14.25">
-      <c r="A1" s="60"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1970,13 +1885,13 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:24" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="62"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -1985,9 +1900,9 @@
     </row>
     <row r="3" spans="1:24" s="4" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="62"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="79"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -1998,11 +1913,11 @@
       <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -2016,9 +1931,9 @@
       <c r="A5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -2032,9 +1947,9 @@
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -2045,11 +1960,11 @@
       <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -2061,9 +1976,9 @@
       <c r="A8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:24" s="12" customFormat="1">
@@ -2206,11 +2121,11 @@
       <c r="C16" s="17"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
-      <c r="F16" s="56" t="s">
+      <c r="F16" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
       <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:16384" s="21" customFormat="1" ht="38.25">
@@ -2244,11 +2159,11 @@
     </row>
     <row r="18" spans="1:16384" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="22"/>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="76"/>
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
@@ -19097,11 +19012,11 @@
     </row>
     <row r="43" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A43" s="30"/>
-      <c r="B43" s="57" t="s">
+      <c r="B43" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="58"/>
-      <c r="D43" s="59"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="76"/>
       <c r="E43" s="31"/>
       <c r="F43" s="32"/>
       <c r="G43" s="32"/>
@@ -19476,16 +19391,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X167"/>
+  <dimension ref="A1:X96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A157" sqref="A157"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="12" style="36" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="37" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" style="37" customWidth="1"/>
     <col min="3" max="4" width="35.140625" style="37" customWidth="1"/>
     <col min="5" max="5" width="32.140625" style="37" customWidth="1"/>
     <col min="6" max="8" width="9.7109375" style="37" customWidth="1"/>
@@ -19494,10 +19409,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" ht="14.25">
-      <c r="A1" s="60"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -19506,13 +19421,13 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:24" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="62"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -19521,9 +19436,9 @@
     </row>
     <row r="3" spans="1:24" s="4" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="62"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="79"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -19534,11 +19449,11 @@
       <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -19552,9 +19467,9 @@
       <c r="A5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -19568,9 +19483,9 @@
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -19581,11 +19496,11 @@
       <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -19597,14 +19512,14 @@
       <c r="A8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
     </row>
     <row r="9" spans="1:24" s="12" customFormat="1">
       <c r="A9" s="39" t="s">
@@ -19622,11 +19537,11 @@
         <f>H17</f>
         <v>External build 16112011</v>
       </c>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
     </row>
     <row r="10" spans="1:24" s="12" customFormat="1">
       <c r="A10" s="40" t="s">
@@ -19644,70 +19559,70 @@
         <f>SUM(D11:D14)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
     </row>
     <row r="11" spans="1:24" s="12" customFormat="1">
       <c r="A11" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="15">
-        <f>COUNTIF($F$18:$F$167,"*Passed")</f>
+        <f>COUNTIF($F$18:$F$96,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="C11" s="15">
-        <f>COUNTIF($G$18:$G$167,"*Passed")</f>
+        <f>COUNTIF($G$18:$G$96,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="D11" s="15">
-        <f>COUNTIF($H$18:$H$167,"*Passed")</f>
+        <f>COUNTIF($H$18:$H$96,"*Passed")</f>
         <v>0</v>
       </c>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
     </row>
     <row r="12" spans="1:24" s="12" customFormat="1">
       <c r="A12" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="15">
-        <f>COUNTIF($F$18:$F$167,"*Failed*")</f>
+        <f>COUNTIF($F$18:$F$96,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="C12" s="15">
-        <f>COUNTIF($G$18:$G$167,"*Failed*")</f>
+        <f>COUNTIF($G$18:$G$96,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="D12" s="15">
-        <f>COUNTIF($H$18:$H$167,"*Failed*")</f>
+        <f>COUNTIF($H$18:$H$96,"*Failed*")</f>
         <v>0</v>
       </c>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
     </row>
     <row r="13" spans="1:24" s="12" customFormat="1">
       <c r="A13" s="40" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="15">
-        <f>COUNTIF($F$18:$F$167,"*Not Run*")</f>
+        <f>COUNTIF($F$18:$F$96,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="C13" s="15">
-        <f>COUNTIF($G$18:$G$167,"*Not Run*")</f>
+        <f>COUNTIF($G$18:$G$96,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="D13" s="15">
-        <f>COUNTIF($H$18:$H$167,"*Not Run*")</f>
+        <f>COUNTIF($H$18:$H$96,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="E13" s="8"/>
@@ -19721,15 +19636,15 @@
         <v>16</v>
       </c>
       <c r="B14" s="15">
-        <f>COUNTIF($F$18:$F$167,"*NA*")</f>
+        <f>COUNTIF($F$18:$F$96,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="C14" s="15">
-        <f>COUNTIF($G$18:$G$167,"*NA*")</f>
+        <f>COUNTIF($G$18:$G$96,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="D14" s="15">
-        <f>COUNTIF($H$18:$H$167,"*NA*")</f>
+        <f>COUNTIF($H$18:$H$96,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="E14" s="8"/>
@@ -19743,15 +19658,15 @@
         <v>17</v>
       </c>
       <c r="B15" s="15">
-        <f>COUNTIF($F$18:$F$167,"*Passed in previous build*")</f>
+        <f>COUNTIF($F$18:$F$96,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="C15" s="15">
-        <f>COUNTIF($G$18:$G$167,"*Passed in previous build*")</f>
+        <f>COUNTIF($G$18:$G$96,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="D15" s="15">
-        <f>COUNTIF($H$18:$H$167,"*Passed in previous build*")</f>
+        <f>COUNTIF($H$18:$H$96,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="E15" s="8"/>
@@ -19761,16 +19676,16 @@
       <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:24" s="21" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="69"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
-      <c r="F16" s="56" t="s">
+      <c r="F16" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
       <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" s="21" customFormat="1" ht="38.25">
@@ -19803,38 +19718,38 @@
       </c>
     </row>
     <row r="18" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A18" s="71"/>
-      <c r="B18" s="72" t="s">
-        <v>142</v>
-      </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="71"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="85" t="s">
+        <v>202</v>
+      </c>
+      <c r="C18" s="86"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="59"/>
     </row>
     <row r="19" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="43"/>
       <c r="B19" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="C19" s="76"/>
-      <c r="D19" s="77"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="78"/>
+        <v>204</v>
+      </c>
+      <c r="C19" s="61"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="63"/>
     </row>
     <row r="20" spans="1:9" s="27" customFormat="1">
-      <c r="A20" s="80">
+      <c r="A20" s="65">
         <f t="shared" ref="A20:A83" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>144</v>
+        <v>205</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="24"/>
@@ -19845,12 +19760,12 @@
       <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A21" s="80">
+      <c r="A21" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>145</v>
+        <v>206</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="25"/>
@@ -19860,12 +19775,12 @@
       <c r="I21" s="26"/>
     </row>
     <row r="22" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A22" s="80">
+      <c r="A22" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>146</v>
+        <v>207</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="24"/>
@@ -19876,12 +19791,12 @@
       <c r="I22" s="26"/>
     </row>
     <row r="23" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A23" s="80">
+      <c r="A23" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="B23" s="81" t="s">
-        <v>147</v>
+      <c r="B23" s="66" t="s">
+        <v>208</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="24"/>
@@ -19891,13 +19806,13 @@
       <c r="H23" s="1"/>
       <c r="I23" s="26"/>
     </row>
-    <row r="24" spans="1:9" s="27" customFormat="1" ht="38.25">
-      <c r="A24" s="80">
+    <row r="24" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A24" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>148</v>
+        <v>215</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="24"/>
@@ -19907,13 +19822,13 @@
       <c r="H24" s="1"/>
       <c r="I24" s="26"/>
     </row>
-    <row r="25" spans="1:9" s="27" customFormat="1" ht="38.25">
-      <c r="A25" s="80">
+    <row r="25" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A25" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>149</v>
+        <v>216</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="24"/>
@@ -19924,12 +19839,12 @@
       <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A26" s="80">
+      <c r="A26" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>150</v>
+        <v>217</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="24"/>
@@ -19937,15 +19852,15 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="82"/>
+      <c r="I26" s="67"/>
     </row>
     <row r="27" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A27" s="80">
+      <c r="A27" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>151</v>
+        <v>209</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="24"/>
@@ -19956,12 +19871,12 @@
       <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A28" s="80">
+      <c r="A28" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>152</v>
+        <v>210</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="24"/>
@@ -19969,15 +19884,15 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="82"/>
+      <c r="I28" s="67"/>
     </row>
     <row r="29" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A29" s="80">
+      <c r="A29" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>153</v>
+        <v>211</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="24"/>
@@ -19985,15 +19900,15 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="82"/>
+      <c r="I29" s="67"/>
     </row>
     <row r="30" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A30" s="80">
+      <c r="A30" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>154</v>
+        <v>212</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="24"/>
@@ -20001,28 +19916,28 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="82"/>
+      <c r="I30" s="67"/>
     </row>
     <row r="31" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="43"/>
       <c r="B31" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="C31" s="76"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="78"/>
+        <v>142</v>
+      </c>
+      <c r="C31" s="61"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="63"/>
     </row>
     <row r="32" spans="1:9" s="27" customFormat="1">
-      <c r="A32" s="80">
+      <c r="A32" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="24"/>
@@ -20033,12 +19948,12 @@
       <c r="I32" s="26"/>
     </row>
     <row r="33" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A33" s="80">
+      <c r="A33" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D33" s="24"/>
       <c r="E33" s="25"/>
@@ -20048,12 +19963,12 @@
       <c r="I33" s="26"/>
     </row>
     <row r="34" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A34" s="80">
+      <c r="A34" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>14</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="24"/>
@@ -20064,12 +19979,12 @@
       <c r="I34" s="26"/>
     </row>
     <row r="35" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A35" s="80">
+      <c r="A35" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
-      <c r="B35" s="81" t="s">
-        <v>159</v>
+      <c r="B35" s="66" t="s">
+        <v>146</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="24"/>
@@ -20079,13 +19994,13 @@
       <c r="H35" s="1"/>
       <c r="I35" s="26"/>
     </row>
-    <row r="36" spans="1:9" s="27" customFormat="1" ht="38.25">
-      <c r="A36" s="80">
+    <row r="36" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A36" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>160</v>
+        <v>213</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="24"/>
@@ -20095,13 +20010,13 @@
       <c r="H36" s="1"/>
       <c r="I36" s="26"/>
     </row>
-    <row r="37" spans="1:9" s="27" customFormat="1" ht="38.25">
-      <c r="A37" s="80">
+    <row r="37" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A37" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>17</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>161</v>
+        <v>214</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="24"/>
@@ -20112,12 +20027,12 @@
       <c r="I37" s="26"/>
     </row>
     <row r="38" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A38" s="80">
+      <c r="A38" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>18</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="24"/>
@@ -20128,12 +20043,12 @@
       <c r="I38" s="26"/>
     </row>
     <row r="39" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A39" s="80">
+      <c r="A39" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="24"/>
@@ -20141,15 +20056,15 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="82"/>
+      <c r="I39" s="67"/>
     </row>
     <row r="40" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A40" s="80">
+      <c r="A40" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="24"/>
@@ -20157,15 +20072,15 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="82"/>
+      <c r="I40" s="67"/>
     </row>
     <row r="41" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A41" s="80">
+      <c r="A41" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>21</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="24"/>
@@ -20173,15 +20088,15 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="82"/>
+      <c r="I41" s="67"/>
     </row>
     <row r="42" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A42" s="80">
+      <c r="A42" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="24"/>
@@ -20189,28 +20104,28 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="82"/>
+      <c r="I42" s="67"/>
     </row>
     <row r="43" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A43" s="43"/>
       <c r="B43" s="53" t="s">
-        <v>167</v>
-      </c>
-      <c r="C43" s="76"/>
-      <c r="D43" s="77"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="78"/>
+        <v>152</v>
+      </c>
+      <c r="C43" s="61"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="64"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="63"/>
     </row>
     <row r="44" spans="1:9" s="27" customFormat="1">
-      <c r="A44" s="80">
+      <c r="A44" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>23</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="24"/>
@@ -20221,12 +20136,12 @@
       <c r="I44" s="26"/>
     </row>
     <row r="45" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A45" s="80">
+      <c r="A45" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>24</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="24"/>
@@ -20237,12 +20152,12 @@
       <c r="I45" s="26"/>
     </row>
     <row r="46" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A46" s="80">
+      <c r="A46" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>25</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D46" s="24"/>
       <c r="E46" s="25"/>
@@ -20252,12 +20167,12 @@
       <c r="I46" s="26"/>
     </row>
     <row r="47" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A47" s="80">
+      <c r="A47" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>26</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="24"/>
@@ -20268,12 +20183,12 @@
       <c r="I47" s="26"/>
     </row>
     <row r="48" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A48" s="80">
+      <c r="A48" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>27</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="24"/>
@@ -20284,12 +20199,12 @@
       <c r="I48" s="26"/>
     </row>
     <row r="49" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A49" s="80">
+      <c r="A49" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="24"/>
@@ -20300,12 +20215,12 @@
       <c r="I49" s="26"/>
     </row>
     <row r="50" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A50" s="80">
+      <c r="A50" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>29</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="24"/>
@@ -20316,12 +20231,12 @@
       <c r="I50" s="26"/>
     </row>
     <row r="51" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A51" s="80">
+      <c r="A51" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="24"/>
@@ -20332,12 +20247,12 @@
       <c r="I51" s="26"/>
     </row>
     <row r="52" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A52" s="80">
+      <c r="A52" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>31</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="24"/>
@@ -20345,15 +20260,15 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
-      <c r="I52" s="82"/>
+      <c r="I52" s="67"/>
     </row>
     <row r="53" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A53" s="80">
+      <c r="A53" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>32</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="24"/>
@@ -20361,15 +20276,15 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-      <c r="I53" s="82"/>
+      <c r="I53" s="67"/>
     </row>
     <row r="54" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A54" s="80">
+      <c r="A54" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>33</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="24"/>
@@ -20377,15 +20292,15 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
-      <c r="I54" s="82"/>
+      <c r="I54" s="67"/>
     </row>
     <row r="55" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A55" s="80">
+      <c r="A55" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>34</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="24"/>
@@ -20393,15 +20308,15 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
-      <c r="I55" s="82"/>
+      <c r="I55" s="67"/>
     </row>
     <row r="56" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A56" s="80">
+      <c r="A56" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="24"/>
@@ -20409,15 +20324,15 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
-      <c r="I56" s="82"/>
+      <c r="I56" s="67"/>
     </row>
     <row r="57" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A57" s="80">
+      <c r="A57" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>36</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="24"/>
@@ -20425,15 +20340,15 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
-      <c r="I57" s="82"/>
+      <c r="I57" s="67"/>
     </row>
     <row r="58" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A58" s="80">
+      <c r="A58" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>37</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="24"/>
@@ -20441,15 +20356,15 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
-      <c r="I58" s="82"/>
+      <c r="I58" s="67"/>
     </row>
     <row r="59" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A59" s="80">
+      <c r="A59" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>38</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="24"/>
@@ -20457,28 +20372,28 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="82"/>
+      <c r="I59" s="67"/>
     </row>
     <row r="60" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="43"/>
       <c r="B60" s="53" t="s">
-        <v>184</v>
-      </c>
-      <c r="C60" s="76"/>
-      <c r="D60" s="77"/>
-      <c r="E60" s="78"/>
-      <c r="F60" s="79"/>
-      <c r="G60" s="79"/>
-      <c r="H60" s="79"/>
-      <c r="I60" s="78"/>
+        <v>169</v>
+      </c>
+      <c r="C60" s="61"/>
+      <c r="D60" s="62"/>
+      <c r="E60" s="63"/>
+      <c r="F60" s="64"/>
+      <c r="G60" s="64"/>
+      <c r="H60" s="64"/>
+      <c r="I60" s="63"/>
     </row>
     <row r="61" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A61" s="80">
+      <c r="A61" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>39</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="24"/>
@@ -20486,15 +20401,15 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="82"/>
+      <c r="I61" s="67"/>
     </row>
     <row r="62" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A62" s="80">
+      <c r="A62" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>40</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="24"/>
@@ -20502,15 +20417,15 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="82"/>
+      <c r="I62" s="67"/>
     </row>
     <row r="63" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A63" s="80">
+      <c r="A63" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>41</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="24"/>
@@ -20518,15 +20433,15 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="82"/>
+      <c r="I63" s="67"/>
     </row>
     <row r="64" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A64" s="80">
+      <c r="A64" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>42</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="24"/>
@@ -20534,28 +20449,28 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
-      <c r="I64" s="82"/>
+      <c r="I64" s="67"/>
     </row>
     <row r="65" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A65" s="43"/>
       <c r="B65" s="53" t="s">
-        <v>189</v>
-      </c>
-      <c r="C65" s="76"/>
-      <c r="D65" s="77"/>
-      <c r="E65" s="78"/>
-      <c r="F65" s="79"/>
-      <c r="G65" s="79"/>
-      <c r="H65" s="79"/>
-      <c r="I65" s="78"/>
+        <v>174</v>
+      </c>
+      <c r="C65" s="61"/>
+      <c r="D65" s="62"/>
+      <c r="E65" s="63"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="64"/>
+      <c r="H65" s="64"/>
+      <c r="I65" s="63"/>
     </row>
     <row r="66" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A66" s="80">
+      <c r="A66" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>43</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="24"/>
@@ -20563,15 +20478,15 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
-      <c r="I66" s="82"/>
+      <c r="I66" s="67"/>
     </row>
     <row r="67" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A67" s="80">
+      <c r="A67" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>44</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="24"/>
@@ -20579,15 +20494,15 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
-      <c r="I67" s="82"/>
+      <c r="I67" s="67"/>
     </row>
     <row r="68" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A68" s="80">
+      <c r="A68" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>45</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="24"/>
@@ -20595,28 +20510,28 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
-      <c r="I68" s="82"/>
+      <c r="I68" s="67"/>
     </row>
     <row r="69" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A69" s="43"/>
       <c r="B69" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="C69" s="76"/>
-      <c r="D69" s="77"/>
-      <c r="E69" s="78"/>
-      <c r="F69" s="79"/>
-      <c r="G69" s="79"/>
-      <c r="H69" s="79"/>
-      <c r="I69" s="78"/>
+        <v>177</v>
+      </c>
+      <c r="C69" s="61"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="63"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="64"/>
+      <c r="H69" s="64"/>
+      <c r="I69" s="63"/>
     </row>
     <row r="70" spans="1:9" s="27" customFormat="1">
-      <c r="A70" s="80">
+      <c r="A70" s="65">
         <f t="shared" ref="A70:A81" ca="1" si="1">IF(OFFSET(A70,-1,0) ="",OFFSET(A70,-2,0)+1,OFFSET(A70,-1,0)+1 )</f>
         <v>46</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="24"/>
@@ -20627,12 +20542,12 @@
       <c r="I70" s="26"/>
     </row>
     <row r="71" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A71" s="80">
+      <c r="A71" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>47</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D71" s="24"/>
       <c r="E71" s="25"/>
@@ -20642,12 +20557,12 @@
       <c r="I71" s="26"/>
     </row>
     <row r="72" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A72" s="80">
+      <c r="A72" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>48</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="24"/>
@@ -20658,12 +20573,12 @@
       <c r="I72" s="26"/>
     </row>
     <row r="73" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A73" s="80">
+      <c r="A73" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>49</v>
       </c>
-      <c r="B73" s="81" t="s">
-        <v>196</v>
+      <c r="B73" s="66" t="s">
+        <v>181</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="24"/>
@@ -20674,12 +20589,12 @@
       <c r="I73" s="26"/>
     </row>
     <row r="74" spans="1:9" s="27" customFormat="1" ht="38.25">
-      <c r="A74" s="80">
+      <c r="A74" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>50</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="24"/>
@@ -20690,12 +20605,12 @@
       <c r="I74" s="26"/>
     </row>
     <row r="75" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A75" s="80">
+      <c r="A75" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>51</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="24"/>
@@ -20706,12 +20621,12 @@
       <c r="I75" s="26"/>
     </row>
     <row r="76" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A76" s="80">
+      <c r="A76" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>52</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="24"/>
@@ -20719,15 +20634,15 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
-      <c r="I76" s="82"/>
+      <c r="I76" s="67"/>
     </row>
     <row r="77" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A77" s="80">
+      <c r="A77" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>53</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="24"/>
@@ -20738,12 +20653,12 @@
       <c r="I77" s="26"/>
     </row>
     <row r="78" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A78" s="80">
+      <c r="A78" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>54</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="24"/>
@@ -20751,15 +20666,15 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
-      <c r="I78" s="82"/>
+      <c r="I78" s="67"/>
     </row>
     <row r="79" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A79" s="80">
+      <c r="A79" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>55</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="24"/>
@@ -20767,15 +20682,15 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-      <c r="I79" s="82"/>
+      <c r="I79" s="67"/>
     </row>
     <row r="80" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A80" s="80">
+      <c r="A80" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>56</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="24"/>
@@ -20783,15 +20698,15 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
-      <c r="I80" s="82"/>
+      <c r="I80" s="67"/>
     </row>
     <row r="81" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A81" s="80">
+      <c r="A81" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>57</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="24"/>
@@ -20799,28 +20714,28 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
-      <c r="I81" s="82"/>
+      <c r="I81" s="67"/>
     </row>
     <row r="82" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A82" s="43"/>
       <c r="B82" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="C82" s="76"/>
-      <c r="D82" s="77"/>
-      <c r="E82" s="78"/>
-      <c r="F82" s="79"/>
-      <c r="G82" s="79"/>
-      <c r="H82" s="79"/>
-      <c r="I82" s="78"/>
+        <v>190</v>
+      </c>
+      <c r="C82" s="61"/>
+      <c r="D82" s="62"/>
+      <c r="E82" s="63"/>
+      <c r="F82" s="64"/>
+      <c r="G82" s="64"/>
+      <c r="H82" s="64"/>
+      <c r="I82" s="63"/>
     </row>
     <row r="83" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A83" s="80">
+      <c r="A83" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>58</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="24"/>
@@ -20828,15 +20743,15 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
-      <c r="I83" s="82"/>
+      <c r="I83" s="67"/>
     </row>
     <row r="84" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A84" s="80">
-        <f t="shared" ref="A84:A192" ca="1" si="2">IF(OFFSET(A84,-1,0) ="",OFFSET(A84,-2,0)+1,OFFSET(A84,-1,0)+1 )</f>
+      <c r="A84" s="65">
+        <f t="shared" ref="A84:A94" ca="1" si="2">IF(OFFSET(A84,-1,0) ="",OFFSET(A84,-2,0)+1,OFFSET(A84,-1,0)+1 )</f>
         <v>59</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="24"/>
@@ -20844,15 +20759,15 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
-      <c r="I84" s="82"/>
+      <c r="I84" s="67"/>
     </row>
     <row r="85" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A85" s="80">
+      <c r="A85" s="65">
         <f t="shared" ca="1" si="2"/>
         <v>60</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="24"/>
@@ -20860,41 +20775,41 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
-      <c r="I85" s="82"/>
+      <c r="I85" s="67"/>
     </row>
-    <row r="86" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A86" s="71"/>
-      <c r="B86" s="72" t="s">
-        <v>209</v>
-      </c>
-      <c r="C86" s="73"/>
-      <c r="D86" s="74"/>
-      <c r="E86" s="71"/>
-      <c r="F86" s="75"/>
-      <c r="G86" s="75"/>
-      <c r="H86" s="75"/>
-      <c r="I86" s="71"/>
+    <row r="86" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A86" s="68"/>
+      <c r="B86" s="85" t="s">
+        <v>203</v>
+      </c>
+      <c r="C86" s="86"/>
+      <c r="D86" s="87"/>
+      <c r="E86" s="69"/>
+      <c r="F86" s="32"/>
+      <c r="G86" s="32"/>
+      <c r="H86" s="32"/>
+      <c r="I86" s="69"/>
     </row>
     <row r="87" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A87" s="43"/>
       <c r="B87" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="C87" s="76"/>
-      <c r="D87" s="77"/>
-      <c r="E87" s="78"/>
-      <c r="F87" s="79"/>
-      <c r="G87" s="79"/>
-      <c r="H87" s="79"/>
-      <c r="I87" s="78"/>
+        <v>218</v>
+      </c>
+      <c r="C87" s="61"/>
+      <c r="D87" s="62"/>
+      <c r="E87" s="63"/>
+      <c r="F87" s="64"/>
+      <c r="G87" s="64"/>
+      <c r="H87" s="64"/>
+      <c r="I87" s="63"/>
     </row>
     <row r="88" spans="1:9" s="27" customFormat="1">
-      <c r="A88" s="80">
+      <c r="A88" s="65">
         <f ca="1">A85+1</f>
         <v>61</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="24"/>
@@ -20904,60 +20819,58 @@
       <c r="H88" s="1"/>
       <c r="I88" s="26"/>
     </row>
-    <row r="89" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A89" s="80">
-        <f t="shared" ref="A88:A124" ca="1" si="3">IF(OFFSET(A89,-1,0) ="",OFFSET(A89,-2,0)+1,OFFSET(A89,-1,0)+1 )</f>
+    <row r="89" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A89" s="65">
+        <f ca="1">IF(OFFSET(A89,-1,0) ="",OFFSET(A89,-2,0)+1,OFFSET(A89,-1,0)+1 )</f>
         <v>62</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D89" s="24"/>
+      <c r="B89" s="54" t="s">
+        <v>219</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="70"/>
       <c r="E89" s="25"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
-      <c r="I89" s="26"/>
+      <c r="I89" s="67"/>
     </row>
-    <row r="90" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A90" s="80">
-        <f t="shared" ca="1" si="3"/>
+    <row r="90" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A90" s="65">
+        <f ca="1">IF(OFFSET(A90,-1,0) ="",OFFSET(A90,-2,0)+1,OFFSET(A90,-1,0)+1 )</f>
         <v>63</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C90" s="1"/>
-      <c r="D90" s="24"/>
+      <c r="B90" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="C90" s="71"/>
+      <c r="D90" s="70"/>
       <c r="E90" s="25"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
-      <c r="I90" s="26"/>
+      <c r="I90" s="67"/>
     </row>
-    <row r="91" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A91" s="80">
-        <f t="shared" ca="1" si="3"/>
+    <row r="91" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A91" s="43"/>
+      <c r="B91" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="C91" s="61"/>
+      <c r="D91" s="62"/>
+      <c r="E91" s="63"/>
+      <c r="F91" s="64"/>
+      <c r="G91" s="64"/>
+      <c r="H91" s="64"/>
+      <c r="I91" s="63"/>
+    </row>
+    <row r="92" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A92" s="65">
+        <f t="shared" ref="A92" ca="1" si="3">IF(OFFSET(A92,-1,0) ="",OFFSET(A92,-2,0)+1,OFFSET(A92,-1,0)+1 )</f>
         <v>64</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C91" s="1"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="26"/>
-    </row>
-    <row r="92" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A92" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>65</v>
-      </c>
       <c r="B92" s="1" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="24"/>
@@ -20965,1192 +20878,85 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
-      <c r="I92" s="26"/>
+      <c r="I92" s="67"/>
     </row>
-    <row r="93" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A93" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>66</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C93" s="1"/>
-      <c r="D93" s="24"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="82"/>
+    <row r="93" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A93" s="43"/>
+      <c r="B93" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="C93" s="61"/>
+      <c r="D93" s="62"/>
+      <c r="E93" s="63"/>
+      <c r="F93" s="64"/>
+      <c r="G93" s="64"/>
+      <c r="H93" s="64"/>
+      <c r="I93" s="63"/>
     </row>
-    <row r="94" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A94" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+    <row r="94" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A94" s="72">
+        <f t="shared" ca="1" si="2"/>
+        <v>65</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>151</v>
+        <v>199</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="24"/>
       <c r="E94" s="25"/>
-      <c r="F94" s="1"/>
+      <c r="F94" s="25"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
-      <c r="I94" s="26"/>
+      <c r="I94" s="72"/>
     </row>
-    <row r="95" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A95" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>68</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C95" s="1"/>
-      <c r="D95" s="24"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="82"/>
+    <row r="95" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A95" s="43"/>
+      <c r="B95" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="C95" s="61"/>
+      <c r="D95" s="62"/>
+      <c r="E95" s="63"/>
+      <c r="F95" s="64"/>
+      <c r="G95" s="64"/>
+      <c r="H95" s="64"/>
+      <c r="I95" s="63"/>
     </row>
-    <row r="96" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A96" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+    <row r="96" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A96" s="72">
+        <f t="shared" ref="A96" ca="1" si="4">IF(OFFSET(A96,-1,0) ="",OFFSET(A96,-2,0)+1,OFFSET(A96,-1,0)+1 )</f>
+        <v>66</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="24"/>
       <c r="E96" s="25"/>
-      <c r="F96" s="1"/>
+      <c r="F96" s="25"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
-      <c r="I96" s="82"/>
-    </row>
-    <row r="97" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A97" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C97" s="1"/>
-      <c r="D97" s="24"/>
-      <c r="E97" s="25"/>
-      <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="82"/>
-    </row>
-    <row r="98" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A98" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>71</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C98" s="1"/>
-      <c r="D98" s="24"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
-      <c r="I98" s="82"/>
-    </row>
-    <row r="99" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A99" s="43"/>
-      <c r="B99" s="53" t="s">
-        <v>219</v>
-      </c>
-      <c r="C99" s="76"/>
-      <c r="D99" s="77"/>
-      <c r="E99" s="78"/>
-      <c r="F99" s="79"/>
-      <c r="G99" s="79"/>
-      <c r="H99" s="79"/>
-      <c r="I99" s="78"/>
-    </row>
-    <row r="100" spans="1:9" s="27" customFormat="1">
-      <c r="A100" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>72</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C100" s="1"/>
-      <c r="D100" s="24"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="26"/>
-    </row>
-    <row r="101" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A101" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>73</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D101" s="24"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="26"/>
-    </row>
-    <row r="102" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A102" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>74</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C102" s="1"/>
-      <c r="D102" s="24"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="26"/>
-    </row>
-    <row r="103" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A103" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>75</v>
-      </c>
-      <c r="B103" s="81" t="s">
-        <v>223</v>
-      </c>
-      <c r="C103" s="1"/>
-      <c r="D103" s="24"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="I103" s="26"/>
-    </row>
-    <row r="104" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A104" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>76</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C104" s="1"/>
-      <c r="D104" s="24"/>
-      <c r="E104" s="25"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="26"/>
-    </row>
-    <row r="105" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A105" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>77</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C105" s="1"/>
-      <c r="D105" s="24"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
-      <c r="I105" s="26"/>
-    </row>
-    <row r="106" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A106" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>78</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C106" s="1"/>
-      <c r="D106" s="24"/>
-      <c r="E106" s="25"/>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
-      <c r="H106" s="1"/>
-      <c r="I106" s="26"/>
-    </row>
-    <row r="107" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A107" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>79</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C107" s="1"/>
-      <c r="D107" s="24"/>
-      <c r="E107" s="25"/>
-      <c r="F107" s="1"/>
-      <c r="G107" s="1"/>
-      <c r="H107" s="1"/>
-      <c r="I107" s="82"/>
-    </row>
-    <row r="108" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A108" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>80</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C108" s="1"/>
-      <c r="D108" s="24"/>
-      <c r="E108" s="25"/>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
-      <c r="H108" s="1"/>
-      <c r="I108" s="82"/>
-    </row>
-    <row r="109" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A109" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>81</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C109" s="1"/>
-      <c r="D109" s="24"/>
-      <c r="E109" s="25"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="I109" s="82"/>
-    </row>
-    <row r="110" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A110" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>82</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C110" s="1"/>
-      <c r="D110" s="24"/>
-      <c r="E110" s="25"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-      <c r="I110" s="82"/>
-    </row>
-    <row r="111" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A111" s="43"/>
-      <c r="B111" s="53" t="s">
-        <v>167</v>
-      </c>
-      <c r="C111" s="76"/>
-      <c r="D111" s="77"/>
-      <c r="E111" s="78"/>
-      <c r="F111" s="79"/>
-      <c r="G111" s="79"/>
-      <c r="H111" s="79"/>
-      <c r="I111" s="78"/>
-    </row>
-    <row r="112" spans="1:9" s="27" customFormat="1">
-      <c r="A112" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>83</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C112" s="1"/>
-      <c r="D112" s="24"/>
-      <c r="E112" s="25"/>
-      <c r="F112" s="1"/>
-      <c r="G112" s="1"/>
-      <c r="H112" s="1"/>
-      <c r="I112" s="26"/>
-    </row>
-    <row r="113" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A113" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>84</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C113" s="1"/>
-      <c r="D113" s="24"/>
-      <c r="E113" s="25"/>
-      <c r="F113" s="1"/>
-      <c r="G113" s="1"/>
-      <c r="H113" s="1"/>
-      <c r="I113" s="26"/>
-    </row>
-    <row r="114" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A114" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>85</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D114" s="24"/>
-      <c r="E114" s="25"/>
-      <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
-      <c r="H114" s="1"/>
-      <c r="I114" s="26"/>
-    </row>
-    <row r="115" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A115" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>86</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C115" s="1"/>
-      <c r="D115" s="24"/>
-      <c r="E115" s="25"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="26"/>
-    </row>
-    <row r="116" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A116" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>87</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C116" s="1"/>
-      <c r="D116" s="24"/>
-      <c r="E116" s="25"/>
-      <c r="F116" s="1"/>
-      <c r="G116" s="1"/>
-      <c r="H116" s="1"/>
-      <c r="I116" s="26"/>
-    </row>
-    <row r="117" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A117" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>88</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C117" s="1"/>
-      <c r="D117" s="24"/>
-      <c r="E117" s="25"/>
-      <c r="F117" s="1"/>
-      <c r="G117" s="1"/>
-      <c r="H117" s="1"/>
-      <c r="I117" s="26"/>
-    </row>
-    <row r="118" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A118" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>89</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C118" s="1"/>
-      <c r="D118" s="24"/>
-      <c r="E118" s="25"/>
-      <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-      <c r="I118" s="26"/>
-    </row>
-    <row r="119" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A119" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>90</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C119" s="1"/>
-      <c r="D119" s="24"/>
-      <c r="E119" s="25"/>
-      <c r="F119" s="1"/>
-      <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
-      <c r="I119" s="26"/>
-    </row>
-    <row r="120" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A120" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>91</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C120" s="1"/>
-      <c r="D120" s="24"/>
-      <c r="E120" s="25"/>
-      <c r="F120" s="1"/>
-      <c r="G120" s="1"/>
-      <c r="H120" s="1"/>
-      <c r="I120" s="82"/>
-    </row>
-    <row r="121" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A121" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>92</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C121" s="1"/>
-      <c r="D121" s="24"/>
-      <c r="E121" s="25"/>
-      <c r="F121" s="1"/>
-      <c r="G121" s="1"/>
-      <c r="H121" s="1"/>
-      <c r="I121" s="82"/>
-    </row>
-    <row r="122" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A122" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>93</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C122" s="1"/>
-      <c r="D122" s="24"/>
-      <c r="E122" s="25"/>
-      <c r="F122" s="1"/>
-      <c r="G122" s="1"/>
-      <c r="H122" s="1"/>
-      <c r="I122" s="82"/>
-    </row>
-    <row r="123" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A123" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>94</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C123" s="1"/>
-      <c r="D123" s="24"/>
-      <c r="E123" s="25"/>
-      <c r="F123" s="1"/>
-      <c r="G123" s="1"/>
-      <c r="H123" s="1"/>
-      <c r="I123" s="82"/>
-    </row>
-    <row r="124" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A124" s="80">
-        <f t="shared" ca="1" si="3"/>
-        <v>95</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C124" s="1"/>
-      <c r="D124" s="24"/>
-      <c r="E124" s="25"/>
-      <c r="F124" s="1"/>
-      <c r="G124" s="1"/>
-      <c r="H124" s="1"/>
-      <c r="I124" s="82"/>
-    </row>
-    <row r="125" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A125" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>96</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C125" s="1"/>
-      <c r="D125" s="24"/>
-      <c r="E125" s="25"/>
-      <c r="F125" s="1"/>
-      <c r="G125" s="1"/>
-      <c r="H125" s="1"/>
-      <c r="I125" s="82"/>
-    </row>
-    <row r="126" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A126" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>97</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C126" s="1"/>
-      <c r="D126" s="24"/>
-      <c r="E126" s="25"/>
-      <c r="F126" s="1"/>
-      <c r="G126" s="1"/>
-      <c r="H126" s="1"/>
-      <c r="I126" s="82"/>
-    </row>
-    <row r="127" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A127" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>98</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C127" s="1"/>
-      <c r="D127" s="24"/>
-      <c r="E127" s="25"/>
-      <c r="F127" s="1"/>
-      <c r="G127" s="1"/>
-      <c r="H127" s="1"/>
-      <c r="I127" s="82"/>
-    </row>
-    <row r="128" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A128" s="43"/>
-      <c r="B128" s="53" t="s">
-        <v>184</v>
-      </c>
-      <c r="C128" s="76"/>
-      <c r="D128" s="77"/>
-      <c r="E128" s="78"/>
-      <c r="F128" s="79"/>
-      <c r="G128" s="79"/>
-      <c r="H128" s="79"/>
-      <c r="I128" s="78"/>
-    </row>
-    <row r="129" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A129" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>99</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C129" s="1"/>
-      <c r="D129" s="24"/>
-      <c r="E129" s="25"/>
-      <c r="F129" s="1"/>
-      <c r="G129" s="1"/>
-      <c r="H129" s="1"/>
-      <c r="I129" s="82"/>
-    </row>
-    <row r="130" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A130" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C130" s="1"/>
-      <c r="D130" s="24"/>
-      <c r="E130" s="25"/>
-      <c r="F130" s="1"/>
-      <c r="G130" s="1"/>
-      <c r="H130" s="1"/>
-      <c r="I130" s="82"/>
-    </row>
-    <row r="131" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A131" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>101</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C131" s="1"/>
-      <c r="D131" s="24"/>
-      <c r="E131" s="25"/>
-      <c r="F131" s="1"/>
-      <c r="G131" s="1"/>
-      <c r="H131" s="1"/>
-      <c r="I131" s="82"/>
-    </row>
-    <row r="132" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A132" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>102</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C132" s="1"/>
-      <c r="D132" s="24"/>
-      <c r="E132" s="25"/>
-      <c r="F132" s="1"/>
-      <c r="G132" s="1"/>
-      <c r="H132" s="1"/>
-      <c r="I132" s="82"/>
-    </row>
-    <row r="133" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A133" s="43"/>
-      <c r="B133" s="53" t="s">
-        <v>189</v>
-      </c>
-      <c r="C133" s="76"/>
-      <c r="D133" s="77"/>
-      <c r="E133" s="78"/>
-      <c r="F133" s="79"/>
-      <c r="G133" s="79"/>
-      <c r="H133" s="79"/>
-      <c r="I133" s="78"/>
-    </row>
-    <row r="134" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A134" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>103</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C134" s="1"/>
-      <c r="D134" s="24"/>
-      <c r="E134" s="25"/>
-      <c r="F134" s="1"/>
-      <c r="G134" s="1"/>
-      <c r="H134" s="1"/>
-      <c r="I134" s="82"/>
-    </row>
-    <row r="135" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A135" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>104</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C135" s="1"/>
-      <c r="D135" s="24"/>
-      <c r="E135" s="25"/>
-      <c r="F135" s="1"/>
-      <c r="G135" s="1"/>
-      <c r="H135" s="1"/>
-      <c r="I135" s="82"/>
-    </row>
-    <row r="136" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A136" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C136" s="1"/>
-      <c r="D136" s="24"/>
-      <c r="E136" s="25"/>
-      <c r="F136" s="1"/>
-      <c r="G136" s="1"/>
-      <c r="H136" s="1"/>
-      <c r="I136" s="82"/>
-    </row>
-    <row r="137" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A137" s="43"/>
-      <c r="B137" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="C137" s="76"/>
-      <c r="D137" s="77"/>
-      <c r="E137" s="78"/>
-      <c r="F137" s="79"/>
-      <c r="G137" s="79"/>
-      <c r="H137" s="79"/>
-      <c r="I137" s="78"/>
-    </row>
-    <row r="138" spans="1:9" s="27" customFormat="1">
-      <c r="A138" s="80">
-        <f t="shared" ref="A138:A149" ca="1" si="4">IF(OFFSET(A138,-1,0) ="",OFFSET(A138,-2,0)+1,OFFSET(A138,-1,0)+1 )</f>
-        <v>106</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C138" s="1"/>
-      <c r="D138" s="24"/>
-      <c r="E138" s="25"/>
-      <c r="F138" s="1"/>
-      <c r="G138" s="1"/>
-      <c r="H138" s="1"/>
-      <c r="I138" s="26"/>
-    </row>
-    <row r="139" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A139" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>107</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D139" s="24"/>
-      <c r="E139" s="25"/>
-      <c r="F139" s="1"/>
-      <c r="G139" s="1"/>
-      <c r="H139" s="1"/>
-      <c r="I139" s="26"/>
-    </row>
-    <row r="140" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A140" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>108</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C140" s="1"/>
-      <c r="D140" s="24"/>
-      <c r="E140" s="25"/>
-      <c r="F140" s="1"/>
-      <c r="G140" s="1"/>
-      <c r="H140" s="1"/>
-      <c r="I140" s="26"/>
-    </row>
-    <row r="141" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A141" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>109</v>
-      </c>
-      <c r="B141" s="81" t="s">
-        <v>196</v>
-      </c>
-      <c r="C141" s="1"/>
-      <c r="D141" s="24"/>
-      <c r="E141" s="25"/>
-      <c r="F141" s="1"/>
-      <c r="G141" s="1"/>
-      <c r="H141" s="1"/>
-      <c r="I141" s="26"/>
-    </row>
-    <row r="142" spans="1:9" s="27" customFormat="1" ht="38.25">
-      <c r="A142" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>110</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C142" s="1"/>
-      <c r="D142" s="24"/>
-      <c r="E142" s="25"/>
-      <c r="F142" s="1"/>
-      <c r="G142" s="1"/>
-      <c r="H142" s="1"/>
-      <c r="I142" s="26"/>
-    </row>
-    <row r="143" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A143" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>111</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C143" s="1"/>
-      <c r="D143" s="24"/>
-      <c r="E143" s="25"/>
-      <c r="F143" s="1"/>
-      <c r="G143" s="1"/>
-      <c r="H143" s="1"/>
-      <c r="I143" s="26"/>
-    </row>
-    <row r="144" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A144" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>112</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C144" s="1"/>
-      <c r="D144" s="24"/>
-      <c r="E144" s="25"/>
-      <c r="F144" s="1"/>
-      <c r="G144" s="1"/>
-      <c r="H144" s="1"/>
-      <c r="I144" s="82"/>
-    </row>
-    <row r="145" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A145" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>113</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C145" s="1"/>
-      <c r="D145" s="24"/>
-      <c r="E145" s="25"/>
-      <c r="F145" s="1"/>
-      <c r="G145" s="1"/>
-      <c r="H145" s="1"/>
-      <c r="I145" s="26"/>
-    </row>
-    <row r="146" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A146" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>114</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C146" s="1"/>
-      <c r="D146" s="24"/>
-      <c r="E146" s="25"/>
-      <c r="F146" s="1"/>
-      <c r="G146" s="1"/>
-      <c r="H146" s="1"/>
-      <c r="I146" s="82"/>
-    </row>
-    <row r="147" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A147" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>115</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C147" s="1"/>
-      <c r="D147" s="24"/>
-      <c r="E147" s="25"/>
-      <c r="F147" s="1"/>
-      <c r="G147" s="1"/>
-      <c r="H147" s="1"/>
-      <c r="I147" s="82"/>
-    </row>
-    <row r="148" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A148" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>116</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C148" s="1"/>
-      <c r="D148" s="24"/>
-      <c r="E148" s="25"/>
-      <c r="F148" s="1"/>
-      <c r="G148" s="1"/>
-      <c r="H148" s="1"/>
-      <c r="I148" s="82"/>
-    </row>
-    <row r="149" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A149" s="80">
-        <f t="shared" ca="1" si="4"/>
-        <v>117</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C149" s="1"/>
-      <c r="D149" s="24"/>
-      <c r="E149" s="25"/>
-      <c r="F149" s="1"/>
-      <c r="G149" s="1"/>
-      <c r="H149" s="1"/>
-      <c r="I149" s="82"/>
-    </row>
-    <row r="150" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A150" s="43"/>
-      <c r="B150" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="C150" s="76"/>
-      <c r="D150" s="77"/>
-      <c r="E150" s="78"/>
-      <c r="F150" s="79"/>
-      <c r="G150" s="79"/>
-      <c r="H150" s="79"/>
-      <c r="I150" s="78"/>
-    </row>
-    <row r="151" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A151" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C151" s="1"/>
-      <c r="D151" s="24"/>
-      <c r="E151" s="25"/>
-      <c r="F151" s="1"/>
-      <c r="G151" s="1"/>
-      <c r="H151" s="1"/>
-      <c r="I151" s="82"/>
-    </row>
-    <row r="152" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A152" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>119</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C152" s="1"/>
-      <c r="D152" s="24"/>
-      <c r="E152" s="25"/>
-      <c r="F152" s="1"/>
-      <c r="G152" s="1"/>
-      <c r="H152" s="1"/>
-      <c r="I152" s="82"/>
-    </row>
-    <row r="153" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A153" s="80">
-        <f t="shared" ca="1" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C153" s="1"/>
-      <c r="D153" s="24"/>
-      <c r="E153" s="25"/>
-      <c r="F153" s="1"/>
-      <c r="G153" s="1"/>
-      <c r="H153" s="1"/>
-      <c r="I153" s="82"/>
-    </row>
-    <row r="154" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A154" s="83"/>
-      <c r="B154" s="72" t="s">
-        <v>231</v>
-      </c>
-      <c r="C154" s="73"/>
-      <c r="D154" s="74"/>
-      <c r="E154" s="84"/>
-      <c r="F154" s="32"/>
-      <c r="G154" s="32"/>
-      <c r="H154" s="32"/>
-      <c r="I154" s="84"/>
-    </row>
-    <row r="155" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A155" s="43"/>
-      <c r="B155" s="53" t="s">
-        <v>232</v>
-      </c>
-      <c r="C155" s="76"/>
-      <c r="D155" s="77"/>
-      <c r="E155" s="78"/>
-      <c r="F155" s="79"/>
-      <c r="G155" s="79"/>
-      <c r="H155" s="79"/>
-      <c r="I155" s="78"/>
-    </row>
-    <row r="156" spans="1:9" s="27" customFormat="1">
-      <c r="A156" s="80">
-        <f ca="1">A153+1</f>
-        <v>121</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C156" s="1"/>
-      <c r="D156" s="24"/>
-      <c r="E156" s="25"/>
-      <c r="F156" s="1"/>
-      <c r="G156" s="1"/>
-      <c r="H156" s="1"/>
-      <c r="I156" s="26"/>
-    </row>
-    <row r="157" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A157" s="80">
-        <f ca="1">IF(OFFSET(A157,-1,0) ="",OFFSET(A157,-2,0)+1,OFFSET(A157,-1,0)+1 )</f>
-        <v>122</v>
-      </c>
-      <c r="B157" s="54" t="s">
-        <v>234</v>
-      </c>
-      <c r="C157" s="1"/>
-      <c r="D157" s="85"/>
-      <c r="E157" s="25"/>
-      <c r="F157" s="1"/>
-      <c r="G157" s="1"/>
-      <c r="H157" s="1"/>
-      <c r="I157" s="82"/>
-    </row>
-    <row r="158" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A158" s="80">
-        <f ca="1">IF(OFFSET(A158,-1,0) ="",OFFSET(A158,-2,0)+1,OFFSET(A158,-1,0)+1 )</f>
-        <v>123</v>
-      </c>
-      <c r="B158" s="54" t="s">
-        <v>235</v>
-      </c>
-      <c r="C158" s="86"/>
-      <c r="D158" s="85"/>
-      <c r="E158" s="25"/>
-      <c r="F158" s="1"/>
-      <c r="G158" s="1"/>
-      <c r="H158" s="1"/>
-      <c r="I158" s="82"/>
-    </row>
-    <row r="159" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A159" s="43"/>
-      <c r="B159" s="53" t="s">
-        <v>232</v>
-      </c>
-      <c r="C159" s="76"/>
-      <c r="D159" s="77"/>
-      <c r="E159" s="78"/>
-      <c r="F159" s="79"/>
-      <c r="G159" s="79"/>
-      <c r="H159" s="79"/>
-      <c r="I159" s="78"/>
-    </row>
-    <row r="160" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A160" s="80">
-        <f t="shared" ref="A160:A163" ca="1" si="5">IF(OFFSET(A160,-1,0) ="",OFFSET(A160,-2,0)+1,OFFSET(A160,-1,0)+1 )</f>
-        <v>124</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C160" s="1"/>
-      <c r="D160" s="24"/>
-      <c r="E160" s="25"/>
-      <c r="F160" s="1"/>
-      <c r="G160" s="1"/>
-      <c r="H160" s="1"/>
-      <c r="I160" s="82"/>
-    </row>
-    <row r="161" spans="1:9" s="27" customFormat="1">
-      <c r="A161" s="80">
-        <f t="shared" ca="1" si="5"/>
-        <v>125</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C161" s="1"/>
-      <c r="D161" s="24"/>
-      <c r="E161" s="25"/>
-      <c r="F161" s="1"/>
-      <c r="G161" s="1"/>
-      <c r="H161" s="1"/>
-      <c r="I161" s="26"/>
-    </row>
-    <row r="162" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A162" s="80">
-        <f t="shared" ca="1" si="5"/>
-        <v>126</v>
-      </c>
-      <c r="B162" s="54" t="s">
-        <v>234</v>
-      </c>
-      <c r="C162" s="1"/>
-      <c r="D162" s="85"/>
-      <c r="E162" s="25"/>
-      <c r="F162" s="1"/>
-      <c r="G162" s="1"/>
-      <c r="H162" s="1"/>
-      <c r="I162" s="82"/>
-    </row>
-    <row r="163" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A163" s="80">
-        <f t="shared" ca="1" si="5"/>
-        <v>127</v>
-      </c>
-      <c r="B163" s="54" t="s">
-        <v>235</v>
-      </c>
-      <c r="C163" s="86"/>
-      <c r="D163" s="85"/>
-      <c r="E163" s="25"/>
-      <c r="F163" s="1"/>
-      <c r="G163" s="1"/>
-      <c r="H163" s="1"/>
-      <c r="I163" s="82"/>
-    </row>
-    <row r="164" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A164" s="43"/>
-      <c r="B164" s="53" t="s">
-        <v>237</v>
-      </c>
-      <c r="C164" s="76"/>
-      <c r="D164" s="77"/>
-      <c r="E164" s="78"/>
-      <c r="F164" s="79"/>
-      <c r="G164" s="79"/>
-      <c r="H164" s="79"/>
-      <c r="I164" s="78"/>
-    </row>
-    <row r="165" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A165" s="87">
-        <f t="shared" ca="1" si="2"/>
-        <v>128</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C165" s="1"/>
-      <c r="D165" s="24"/>
-      <c r="E165" s="25"/>
-      <c r="F165" s="25"/>
-      <c r="G165" s="1"/>
-      <c r="H165" s="1"/>
-      <c r="I165" s="87"/>
-    </row>
-    <row r="166" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A166" s="43"/>
-      <c r="B166" s="53" t="s">
-        <v>239</v>
-      </c>
-      <c r="C166" s="76"/>
-      <c r="D166" s="77"/>
-      <c r="E166" s="78"/>
-      <c r="F166" s="79"/>
-      <c r="G166" s="79"/>
-      <c r="H166" s="79"/>
-      <c r="I166" s="78"/>
-    </row>
-    <row r="167" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A167" s="87">
-        <f t="shared" ref="A167" ca="1" si="6">IF(OFFSET(A167,-1,0) ="",OFFSET(A167,-2,0)+1,OFFSET(A167,-1,0)+1 )</f>
-        <v>129</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C167" s="1"/>
-      <c r="D167" s="24"/>
-      <c r="E167" s="25"/>
-      <c r="F167" s="25"/>
-      <c r="G167" s="1"/>
-      <c r="H167" s="1"/>
-      <c r="I167" s="87"/>
+      <c r="I96" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B154:D154"/>
+  <mergeCells count="12">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B86:D86"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F60:H60 F18:H19 F166:H166 F65:H65 F82:H82 F31:H31 F43:H43 F155:H155 F159:H159 F164:H164 F69:H69 F128:H128 F86:H87 F133:H133 F150:H150 F99:H99 F111:H111 F137:H137"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F60:H60 F18:H19 F95:H95 F65:H65 F82:H82 F31:H31 F43:H43 F87:H87 F91:H91 F93:H93 F69:H69"/>
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
-    <dataValidation type="list" allowBlank="1" sqref="F61:H64 F66:H68 F44:H59 F32:H42 F70:H81 F165:H165 F167:H167 F156:H158 F20:H30 F83:H85 F151:H154 F129:H132 F134:H136 F112:H127 F100:H110 F138:H149 F160:H163 F88:H98">
+    <dataValidation type="list" allowBlank="1" sqref="F61:H64 F66:H68 F44:H59 F32:H42 F70:H81 F94:H94 F96:H96 F88:H90 F20:H30 F92:H92 F83:H86">
       <formula1>$A$11:$A$15</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated file on 23/10 (2) - Assignment 2,3
</commit_message>
<xml_diff>
--- a/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
+++ b/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 1" sheetId="3" r:id="rId1"/>
@@ -264,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F120" authorId="0" shapeId="0">
+    <comment ref="F118" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -453,7 +453,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="389">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -1068,9 +1068,6 @@
     <t>When the user enters lower password</t>
   </si>
   <si>
-    <t>When the user enters password that meets the policy</t>
-  </si>
-  <si>
     <t>When the user doesn't select anything</t>
   </si>
   <si>
@@ -1120,9 +1117,6 @@
   </si>
   <si>
     <t>When the user selects future date</t>
-  </si>
-  <si>
-    <t>Check scroll bar</t>
   </si>
   <si>
     <t>Check dropdown list</t>
@@ -1456,24 +1450,7 @@
     <t xml:space="preserve">When the user enters greater than 6 numeric characters  </t>
   </si>
   <si>
-    <t>1. Open Lazada registration page
-2. Enter valid phone number
-3. Slide to get SMS code
-4. Enter less than 10 numeric characters in SMS Verification Code box</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter valid phone number
-3. Slide to get SMS code
-4. Enter more than 10 numeric characters in SMS Verification Code box</t>
-  </si>
-  <si>
     <t>System will show error message “Please enter a valid SMS Verification Code"</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter more than 10 numeric characters
-3. Slide to get SMS code</t>
   </si>
   <si>
     <t>1. Open Lazada registration page
@@ -1509,11 +1486,6 @@
   <si>
     <t>1. Open Lazada registration page
 2. Don't enter character
-3. Slide to get SMS code</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter less than 10 numeric characters
 3. Slide to get SMS code</t>
   </si>
   <si>
@@ -1580,6 +1552,297 @@
 2. Enter valid phone number
 3. Slide to get SMS code
 4. Enter space into SMS Verification Code</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Observe the display of the Password</t>
+  </si>
+  <si>
+    <t>Password is blank 
+The placeholder is "Minimum 6 characters with a number and a letter"
+There is a symbol * marks Password as a mandatory field</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Don't enter character
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>System will show error message “Please enter Password”</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter only alphabetic characters</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter only special characters</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter only numberic characters</t>
+  </si>
+  <si>
+    <t>System will show error message "Password should contain alphabetic and numeric characters"</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter numeric and special characters</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter alphabetic and special characters</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter alphabetic and numeric characters
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter numeric, alphabetic and special characters
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Copy/Paste password</t>
+  </si>
+  <si>
+    <t>Do not allow copy/paste password</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter space at the beginning and the end of the password
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>Spaces are removed
+Sign up successfully, return to login screen</t>
+  </si>
+  <si>
+    <t>System will show error message "The length of Password should be 6-50 characters"</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 6 characters (valid password)
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 10 characters (valid password) 
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 50 characters (valid password) 
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 5 characters</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter valid phone number
+3. Slide to get SMS code
+4. Enter 5 numeric characters in SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter valid phone number
+3. Slide to get SMS code
+4. Enter 17 numeric characters in SMS Verification Code box</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 11 numeric characters
+3. Slide to get SMS code</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 9 numeric characters
+3. Slide to get SMS code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Lazada registration page
+2. Enter 51 characters
+</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter a valid password where all letters are uppercase
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter a valid password where all letters are lowercase
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>Password is shown</t>
+  </si>
+  <si>
+    <t>Password is hided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Lazada registration page
+2. Observe the display of the Eye icon
+3. Enter any character </t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on the Eye icon to show the password</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on the Eye icon to hide the password</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+4. Enter characters
+3. Click on close (x) button</t>
+  </si>
+  <si>
+    <t>Month is blank, the placeholder is "Month"
+Day is blank, the placeholder is "Day"
+Year is blank, the placeholder is "Year"</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Don't select birthday
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Month
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Day
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Year
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Month and Day
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Month and Year
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Year and Day
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select valid date
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select invalid date
+3. Other fields are valid
+4. Click Sign up button</t>
+  </si>
+  <si>
+    <t>System will show error message “Please select the correct birthday"</t>
+  </si>
+  <si>
+    <t>System will show error message  “Please select the correct birthday"</t>
+  </si>
+  <si>
+    <t>System will show error message “Wrong birthday format"</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select future date</t>
+  </si>
+  <si>
+    <t>There is a scrollbar when the list of Months exceeds the display frame</t>
+  </si>
+  <si>
+    <t>There is a scrollbar when the list of Days exceeds the display frame</t>
+  </si>
+  <si>
+    <t>There is a scrollbar when the list of Years exceeds the display frame</t>
+  </si>
+  <si>
+    <t>The months are fully displayed in the dropdown list and sorted in ascending order</t>
+  </si>
+  <si>
+    <t>Do not allow enter from keyboard</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Observe the display of the Birthday</t>
+  </si>
+  <si>
+    <t>Gender is blank
+The placeholder is "Select"</t>
+  </si>
+  <si>
+    <t>The days are fully displayed in the dropdown list and sorted in ascending order</t>
+  </si>
+  <si>
+    <t>List of years starting from 1990 to 2022 and sorted in descending order</t>
+  </si>
+  <si>
+    <t>There are 2 values: Female and male</t>
+  </si>
+  <si>
+    <t>srollbar maybe not need</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on Month</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on Day</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on Year</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on Gender</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter characters from keyboard</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Don't select Gender
+3. Other fields are valid
+4. Click Sign up button</t>
   </si>
 </sst>
 </file>
@@ -19993,10 +20256,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I130"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -20163,15 +20426,15 @@
         <v>13</v>
       </c>
       <c r="B11" s="15">
-        <f>COUNTIF($F$18:$F$128,"*Passed")</f>
+        <f>COUNTIF($F$18:$F$126,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="C11" s="15">
-        <f>COUNTIF($G$18:$G$128,"*Passed")</f>
+        <f>COUNTIF($G$18:$G$126,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="D11" s="15">
-        <f>COUNTIF($H$18:$H$128,"*Passed")</f>
+        <f>COUNTIF($H$18:$H$126,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="E11" s="56"/>
@@ -20185,15 +20448,15 @@
         <v>14</v>
       </c>
       <c r="B12" s="15">
-        <f>COUNTIF($F$18:$F$128,"*Failed*")</f>
+        <f>COUNTIF($F$18:$F$126,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="C12" s="15">
-        <f>COUNTIF($G$18:$G$128,"*Failed*")</f>
+        <f>COUNTIF($G$18:$G$126,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="D12" s="15">
-        <f>COUNTIF($H$18:$H$128,"*Failed*")</f>
+        <f>COUNTIF($H$18:$H$126,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="E12" s="56"/>
@@ -20207,15 +20470,15 @@
         <v>15</v>
       </c>
       <c r="B13" s="15">
-        <f>COUNTIF($F$18:$F$128,"*Not Run*")</f>
+        <f>COUNTIF($F$18:$F$126,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="C13" s="15">
-        <f>COUNTIF($G$18:$G$128,"*Not Run*")</f>
+        <f>COUNTIF($G$18:$G$126,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="D13" s="15">
-        <f>COUNTIF($H$18:$H$128,"*Not Run*")</f>
+        <f>COUNTIF($H$18:$H$126,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="E13" s="8"/>
@@ -20229,15 +20492,15 @@
         <v>16</v>
       </c>
       <c r="B14" s="15">
-        <f>COUNTIF($F$18:$F$128,"*NA*")</f>
+        <f>COUNTIF($F$18:$F$126,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="C14" s="15">
-        <f>COUNTIF($G$18:$G$128,"*NA*")</f>
+        <f>COUNTIF($G$18:$G$126,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="D14" s="15">
-        <f>COUNTIF($H$18:$H$128,"*NA*")</f>
+        <f>COUNTIF($H$18:$H$126,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="E14" s="8"/>
@@ -20251,15 +20514,15 @@
         <v>17</v>
       </c>
       <c r="B15" s="15">
-        <f>COUNTIF($F$18:$F$128,"*Passed in previous build*")</f>
+        <f>COUNTIF($F$18:$F$126,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="C15" s="15">
-        <f>COUNTIF($G$18:$G$128,"*Passed in previous build*")</f>
+        <f>COUNTIF($G$18:$G$126,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="D15" s="15">
-        <f>COUNTIF($H$18:$H$128,"*Passed in previous build*")</f>
+        <f>COUNTIF($H$18:$H$126,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="E15" s="8"/>
@@ -20338,17 +20601,17 @@
     </row>
     <row r="20" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A20" s="65">
-        <f t="shared" ref="A20:A114" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
+        <f t="shared" ref="A20:A112" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>281</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>283</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="1"/>
@@ -20365,10 +20628,10 @@
         <v>166</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="1"/>
@@ -20385,10 +20648,10 @@
         <v>163</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="1"/>
@@ -20405,10 +20668,10 @@
         <v>164</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="1"/>
@@ -20425,10 +20688,10 @@
         <v>165</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E24" s="25"/>
       <c r="F24" s="1"/>
@@ -20445,10 +20708,10 @@
         <v>170</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E25" s="25"/>
       <c r="F25" s="1"/>
@@ -20465,10 +20728,10 @@
         <v>169</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E26" s="25"/>
       <c r="F26" s="1"/>
@@ -20482,13 +20745,13 @@
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>319</v>
+        <v>348</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E27" s="25"/>
       <c r="F27" s="1"/>
@@ -20502,13 +20765,13 @@
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E28" s="25"/>
       <c r="F28" s="1"/>
@@ -20522,13 +20785,13 @@
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>310</v>
+        <v>347</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -20542,13 +20805,13 @@
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -20565,10 +20828,10 @@
         <v>160</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D31" s="70" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="1"/>
@@ -20598,10 +20861,10 @@
         <v>168</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E33" s="25"/>
       <c r="F33" s="1"/>
@@ -20618,10 +20881,10 @@
         <v>173</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E34" s="25"/>
       <c r="F34" s="1"/>
@@ -20638,10 +20901,10 @@
         <v>163</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E35" s="25"/>
       <c r="F35" s="1"/>
@@ -20658,10 +20921,10 @@
         <v>164</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E36" s="25"/>
       <c r="F36" s="1"/>
@@ -20678,10 +20941,10 @@
         <v>165</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E37" s="25"/>
       <c r="F37" s="1"/>
@@ -20695,13 +20958,13 @@
         <v>18</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E38" s="25"/>
       <c r="F38" s="1"/>
@@ -20718,10 +20981,10 @@
         <v>169</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E39" s="25"/>
       <c r="F39" s="1"/>
@@ -20735,13 +20998,13 @@
         <v>20</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>307</v>
+        <v>345</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E40" s="25"/>
       <c r="F40" s="1"/>
@@ -20755,13 +21018,13 @@
         <v>21</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E41" s="25"/>
       <c r="F41" s="1"/>
@@ -20775,13 +21038,13 @@
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>308</v>
+        <v>346</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E42" s="25"/>
       <c r="F42" s="1"/>
@@ -20795,13 +21058,13 @@
         <v>23</v>
       </c>
       <c r="B43" s="54" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -20818,10 +21081,10 @@
         <v>160</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D44" s="70" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E44" s="25"/>
       <c r="F44" s="1"/>
@@ -20842,7 +21105,7 @@
       <c r="H45" s="64"/>
       <c r="I45" s="63"/>
     </row>
-    <row r="46" spans="1:9" s="27" customFormat="1">
+    <row r="46" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A46" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>25</v>
@@ -20851,16 +21114,18 @@
         <v>168</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D46" s="24"/>
+        <v>324</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>325</v>
+      </c>
       <c r="E46" s="25"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="26"/>
     </row>
-    <row r="47" spans="1:9" s="27" customFormat="1">
+    <row r="47" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A47" s="65">
         <f ca="1">IF(OFFSET(A47,-1,0) ="",OFFSET(A47,-2,0)+1,OFFSET(A47,-1,0)+1 )</f>
         <v>26</v>
@@ -20869,70 +21134,78 @@
         <v>173</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D47" s="24"/>
+        <v>326</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>327</v>
+      </c>
       <c r="E47" s="25"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="26"/>
     </row>
-    <row r="48" spans="1:9" s="27" customFormat="1">
+    <row r="48" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A48" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>27</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D48" s="24"/>
+        <v>328</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>331</v>
+      </c>
       <c r="E48" s="25"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="26"/>
     </row>
-    <row r="49" spans="1:9" s="27" customFormat="1">
+    <row r="49" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A49" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D49" s="24"/>
+        <v>329</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>331</v>
+      </c>
       <c r="E49" s="25"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="26"/>
     </row>
-    <row r="50" spans="1:9" s="27" customFormat="1">
+    <row r="50" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A50" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>29</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D50" s="24"/>
+        <v>330</v>
+      </c>
+      <c r="D50" s="24" t="s">
+        <v>331</v>
+      </c>
       <c r="E50" s="25"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="26"/>
     </row>
-    <row r="51" spans="1:9" s="27" customFormat="1">
+    <row r="51" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A51" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>30</v>
@@ -20941,16 +21214,18 @@
         <v>174</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D51" s="24"/>
+        <v>334</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="E51" s="25"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="26"/>
     </row>
-    <row r="52" spans="1:9" s="27" customFormat="1">
+    <row r="52" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A52" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>31</v>
@@ -20959,16 +21234,18 @@
         <v>175</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D52" s="24"/>
+        <v>332</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>331</v>
+      </c>
       <c r="E52" s="25"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="26"/>
     </row>
-    <row r="53" spans="1:9" s="27" customFormat="1">
+    <row r="53" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A53" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>32</v>
@@ -20977,16 +21254,18 @@
         <v>176</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D53" s="24"/>
+        <v>333</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>331</v>
+      </c>
       <c r="E53" s="25"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="26"/>
     </row>
-    <row r="54" spans="1:9" s="27" customFormat="1">
+    <row r="54" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A54" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>33</v>
@@ -20995,34 +21274,38 @@
         <v>177</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D54" s="24"/>
+        <v>335</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="E54" s="25"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="26"/>
     </row>
-    <row r="55" spans="1:9" s="27" customFormat="1">
+    <row r="55" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A55" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>34</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D55" s="24"/>
+        <v>336</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>337</v>
+      </c>
       <c r="E55" s="25"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="26"/>
     </row>
-    <row r="56" spans="1:9" s="27" customFormat="1">
+    <row r="56" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A56" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>35</v>
@@ -21031,16 +21314,18 @@
         <v>169</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D56" s="24"/>
+        <v>338</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>339</v>
+      </c>
       <c r="E56" s="25"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="26"/>
     </row>
-    <row r="57" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="57" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A57" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>36</v>
@@ -21049,16 +21334,18 @@
         <v>171</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D57" s="24"/>
+        <v>344</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>340</v>
+      </c>
       <c r="E57" s="25"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="67"/>
     </row>
-    <row r="58" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="58" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A58" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>37</v>
@@ -21067,16 +21354,18 @@
         <v>172</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D58" s="24"/>
+        <v>341</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="E58" s="25"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="67"/>
     </row>
-    <row r="59" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="59" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A59" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>38</v>
@@ -21085,52 +21374,58 @@
         <v>178</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D59" s="24"/>
+        <v>342</v>
+      </c>
+      <c r="D59" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="E59" s="25"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="67"/>
     </row>
-    <row r="60" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="60" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A60" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>39</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D60" s="24"/>
+        <v>343</v>
+      </c>
+      <c r="D60" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="E60" s="25"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="67"/>
     </row>
-    <row r="61" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="61" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A61" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>40</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D61" s="24"/>
+        <v>349</v>
+      </c>
+      <c r="D61" s="24" t="s">
+        <v>340</v>
+      </c>
       <c r="E61" s="25"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="67"/>
     </row>
-    <row r="62" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="62" spans="1:9" s="29" customFormat="1" ht="63.75">
       <c r="A62" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>41</v>
@@ -21139,16 +21434,18 @@
         <v>179</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D62" s="24"/>
+        <v>350</v>
+      </c>
+      <c r="D62" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="E62" s="25"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="67"/>
     </row>
-    <row r="63" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="63" spans="1:9" s="29" customFormat="1" ht="63.75">
       <c r="A63" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>42</v>
@@ -21157,137 +21454,151 @@
         <v>180</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D63" s="24"/>
+        <v>351</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="E63" s="25"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="67"/>
     </row>
-    <row r="64" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="64" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A64" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>43</v>
       </c>
-      <c r="B64" s="54" t="s">
-        <v>181</v>
+      <c r="B64" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D64" s="24"/>
+        <v>354</v>
+      </c>
+      <c r="D64" s="24" t="s">
+        <v>352</v>
+      </c>
       <c r="E64" s="25"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="67"/>
     </row>
-    <row r="65" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="65" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A65" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>44</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D65" s="24"/>
+        <v>355</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>352</v>
+      </c>
       <c r="E65" s="25"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="67"/>
     </row>
-    <row r="66" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="66" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A66" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>45</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D66" s="24"/>
+        <v>356</v>
+      </c>
+      <c r="D66" s="24" t="s">
+        <v>353</v>
+      </c>
       <c r="E66" s="25"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="67"/>
     </row>
-    <row r="67" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="67" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A67" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>46</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D67" s="70" t="s">
         <v>282</v>
       </c>
-      <c r="D67" s="24"/>
       <c r="E67" s="25"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="67"/>
     </row>
-    <row r="68" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A68" s="65">
+    <row r="68" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A68" s="43"/>
+      <c r="B68" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" s="61"/>
+      <c r="D68" s="62"/>
+      <c r="E68" s="63"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="64"/>
+      <c r="H68" s="64"/>
+      <c r="I68" s="63"/>
+    </row>
+    <row r="69" spans="1:9" s="29" customFormat="1" ht="38.25">
+      <c r="A69" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>47</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D68" s="70"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="67"/>
-    </row>
-    <row r="69" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A69" s="43"/>
-      <c r="B69" s="53" t="s">
-        <v>147</v>
-      </c>
-      <c r="C69" s="61"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="63"/>
-      <c r="F69" s="64"/>
-      <c r="G69" s="64"/>
-      <c r="H69" s="64"/>
-      <c r="I69" s="63"/>
-    </row>
-    <row r="70" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="B69" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D69" s="24" t="s">
+        <v>358</v>
+      </c>
+      <c r="E69" s="25"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="67"/>
+    </row>
+    <row r="70" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A70" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>48</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>148</v>
+        <v>181</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D70" s="24"/>
+        <v>359</v>
+      </c>
+      <c r="D70" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="E70" s="25"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="67"/>
     </row>
-    <row r="71" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="71" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A71" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>49</v>
@@ -21296,16 +21607,18 @@
         <v>182</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D71" s="24"/>
+        <v>360</v>
+      </c>
+      <c r="D71" s="24" t="s">
+        <v>369</v>
+      </c>
       <c r="E71" s="25"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="67"/>
     </row>
-    <row r="72" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="72" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A72" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>50</v>
@@ -21314,16 +21627,18 @@
         <v>183</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D72" s="24"/>
+        <v>361</v>
+      </c>
+      <c r="D72" s="24" t="s">
+        <v>369</v>
+      </c>
       <c r="E72" s="25"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="67"/>
     </row>
-    <row r="73" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="73" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A73" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>51</v>
@@ -21332,16 +21647,18 @@
         <v>184</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D73" s="24"/>
+        <v>362</v>
+      </c>
+      <c r="D73" s="24" t="s">
+        <v>369</v>
+      </c>
       <c r="E73" s="25"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="67"/>
     </row>
-    <row r="74" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="74" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A74" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>52</v>
@@ -21350,16 +21667,18 @@
         <v>185</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D74" s="24"/>
+        <v>363</v>
+      </c>
+      <c r="D74" s="24" t="s">
+        <v>369</v>
+      </c>
       <c r="E74" s="25"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="67"/>
     </row>
-    <row r="75" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="75" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A75" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>53</v>
@@ -21368,16 +21687,18 @@
         <v>186</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D75" s="24"/>
+        <v>364</v>
+      </c>
+      <c r="D75" s="24" t="s">
+        <v>369</v>
+      </c>
       <c r="E75" s="25"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
       <c r="I75" s="67"/>
     </row>
-    <row r="76" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="76" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A76" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>54</v>
@@ -21386,52 +21707,58 @@
         <v>187</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D76" s="24"/>
+        <v>365</v>
+      </c>
+      <c r="D76" s="24" t="s">
+        <v>369</v>
+      </c>
       <c r="E76" s="25"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="67"/>
     </row>
-    <row r="77" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="77" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A77" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>55</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D77" s="24"/>
+        <v>366</v>
+      </c>
+      <c r="D77" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="E77" s="25"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="67"/>
     </row>
-    <row r="78" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="78" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A78" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>56</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D78" s="24"/>
+        <v>367</v>
+      </c>
+      <c r="D78" s="24" t="s">
+        <v>368</v>
+      </c>
       <c r="E78" s="25"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="67"/>
     </row>
-    <row r="79" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="79" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A79" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>57</v>
@@ -21440,34 +21767,38 @@
         <v>197</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D79" s="1"/>
+        <v>371</v>
+      </c>
+      <c r="D79" s="24" t="s">
+        <v>370</v>
+      </c>
       <c r="E79" s="25"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="67"/>
     </row>
-    <row r="80" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="80" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A80" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>58</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>198</v>
+      <c r="B80" s="54" t="s">
+        <v>191</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D80" s="1"/>
+        <v>383</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="E80" s="25"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="67"/>
     </row>
-    <row r="81" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="81" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A81" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>59</v>
@@ -21476,16 +21807,18 @@
         <v>192</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D81" s="1"/>
+        <v>384</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>373</v>
+      </c>
       <c r="E81" s="25"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="67"/>
     </row>
-    <row r="82" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="82" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A82" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>60</v>
@@ -21494,34 +21827,38 @@
         <v>193</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D82" s="1"/>
+        <v>385</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>374</v>
+      </c>
       <c r="E82" s="25"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="67"/>
     </row>
-    <row r="83" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="83" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A83" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>61</v>
       </c>
       <c r="B83" s="54" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D83" s="1"/>
+        <v>383</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>375</v>
+      </c>
       <c r="E83" s="25"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="67"/>
     </row>
-    <row r="84" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="84" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A84" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>62</v>
@@ -21530,16 +21867,18 @@
         <v>189</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D84" s="1"/>
+        <v>384</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>379</v>
+      </c>
       <c r="E84" s="25"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="67"/>
     </row>
-    <row r="85" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="85" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A85" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>63</v>
@@ -21548,83 +21887,93 @@
         <v>190</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D85" s="1"/>
+        <v>385</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>380</v>
+      </c>
       <c r="E85" s="25"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="67"/>
     </row>
-    <row r="86" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="86" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A86" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>64</v>
       </c>
       <c r="B86" s="54" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D86" s="1"/>
+        <v>387</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>376</v>
+      </c>
       <c r="E86" s="25"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="67"/>
     </row>
-    <row r="87" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A87" s="65">
+    <row r="87" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A87" s="43"/>
+      <c r="B87" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="C87" s="61"/>
+      <c r="D87" s="62"/>
+      <c r="E87" s="63"/>
+      <c r="F87" s="64"/>
+      <c r="G87" s="64"/>
+      <c r="H87" s="64"/>
+      <c r="I87" s="63"/>
+    </row>
+    <row r="88" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A88" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>65</v>
       </c>
-      <c r="B87" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D87" s="1"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="67"/>
-    </row>
-    <row r="88" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A88" s="43"/>
-      <c r="B88" s="53" t="s">
-        <v>149</v>
-      </c>
-      <c r="C88" s="61"/>
-      <c r="D88" s="62"/>
-      <c r="E88" s="63"/>
-      <c r="F88" s="64"/>
-      <c r="G88" s="64"/>
-      <c r="H88" s="64"/>
-      <c r="I88" s="63"/>
-    </row>
-    <row r="89" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="B88" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D88" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="E88" s="25"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="67"/>
+    </row>
+    <row r="89" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A89" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D89" s="24"/>
-      <c r="E89" s="25"/>
+        <v>386</v>
+      </c>
+      <c r="D89" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="E89" s="25" t="s">
+        <v>382</v>
+      </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
       <c r="I89" s="67"/>
     </row>
-    <row r="90" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="90" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A90" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>67</v>
@@ -21633,92 +21982,96 @@
         <v>199</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D90" s="24"/>
+        <v>388</v>
+      </c>
+      <c r="D90" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="E90" s="25"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="67"/>
     </row>
-    <row r="91" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="91" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A91" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>68</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>200</v>
+      <c r="B91" s="54" t="s">
+        <v>195</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D91" s="24"/>
+        <v>387</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>376</v>
+      </c>
       <c r="E91" s="25"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
       <c r="I91" s="67"/>
     </row>
-    <row r="92" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A92" s="65">
-        <f t="shared" ca="1" si="0"/>
+    <row r="92" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A92" s="43"/>
+      <c r="B92" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="C92" s="61"/>
+      <c r="D92" s="62"/>
+      <c r="E92" s="63"/>
+      <c r="F92" s="64"/>
+      <c r="G92" s="64"/>
+      <c r="H92" s="64"/>
+      <c r="I92" s="63"/>
+    </row>
+    <row r="93" spans="1:9" s="27" customFormat="1">
+      <c r="A93" s="65">
+        <f t="shared" ref="A93:A108" ca="1" si="1">IF(OFFSET(A93,-1,0) ="",OFFSET(A93,-2,0)+1,OFFSET(A93,-1,0)+1 )</f>
         <v>69</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D92" s="24"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="67"/>
-    </row>
-    <row r="93" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A93" s="65">
-        <f t="shared" ca="1" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="B93" s="54" t="s">
-        <v>196</v>
+      <c r="B93" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D93" s="1"/>
+        <v>280</v>
+      </c>
+      <c r="D93" s="24"/>
       <c r="E93" s="25"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
-      <c r="I93" s="67"/>
-    </row>
-    <row r="94" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A94" s="43"/>
-      <c r="B94" s="53" t="s">
-        <v>150</v>
-      </c>
-      <c r="C94" s="61"/>
-      <c r="D94" s="62"/>
-      <c r="E94" s="63"/>
-      <c r="F94" s="64"/>
-      <c r="G94" s="64"/>
-      <c r="H94" s="64"/>
-      <c r="I94" s="63"/>
+      <c r="I93" s="26"/>
+    </row>
+    <row r="94" spans="1:9" s="27" customFormat="1">
+      <c r="A94" s="65">
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D94" s="24"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="26"/>
     </row>
     <row r="95" spans="1:9" s="27" customFormat="1">
       <c r="A95" s="65">
-        <f t="shared" ref="A95:A110" ca="1" si="1">IF(OFFSET(A95,-1,0) ="",OFFSET(A95,-2,0)+1,OFFSET(A95,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>71</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D95" s="24"/>
       <c r="E95" s="25"/>
@@ -21736,7 +22089,7 @@
         <v>203</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D96" s="24"/>
       <c r="E96" s="25"/>
@@ -21751,10 +22104,10 @@
         <v>73</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D97" s="24"/>
       <c r="E97" s="25"/>
@@ -21769,10 +22122,10 @@
         <v>74</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D98" s="24"/>
       <c r="E98" s="25"/>
@@ -21787,10 +22140,10 @@
         <v>75</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D99" s="24"/>
       <c r="E99" s="25"/>
@@ -21805,10 +22158,10 @@
         <v>76</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D100" s="24"/>
       <c r="E100" s="25"/>
@@ -21823,10 +22176,10 @@
         <v>77</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D101" s="24"/>
       <c r="E101" s="25"/>
@@ -21841,10 +22194,10 @@
         <v>78</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D102" s="24"/>
       <c r="E102" s="25"/>
@@ -21853,41 +22206,41 @@
       <c r="H102" s="1"/>
       <c r="I102" s="26"/>
     </row>
-    <row r="103" spans="1:9" s="27" customFormat="1">
+    <row r="103" spans="1:9" s="29" customFormat="1" ht="14.25">
       <c r="A103" s="65">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>79</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D103" s="24"/>
       <c r="E103" s="25"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
-      <c r="I103" s="26"/>
-    </row>
-    <row r="104" spans="1:9" s="27" customFormat="1">
+      <c r="I103" s="67"/>
+    </row>
+    <row r="104" spans="1:9" s="29" customFormat="1" ht="14.25">
       <c r="A104" s="65">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>80</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D104" s="24"/>
       <c r="E104" s="25"/>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
-      <c r="I104" s="26"/>
+      <c r="I104" s="67"/>
     </row>
     <row r="105" spans="1:9" s="29" customFormat="1" ht="14.25">
       <c r="A105" s="65">
@@ -21895,10 +22248,10 @@
         <v>81</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D105" s="24"/>
       <c r="E105" s="25"/>
@@ -21913,10 +22266,10 @@
         <v>82</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D106" s="24"/>
       <c r="E106" s="25"/>
@@ -21931,10 +22284,10 @@
         <v>83</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D107" s="24"/>
       <c r="E107" s="25"/>
@@ -21949,10 +22302,10 @@
         <v>84</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D108" s="24"/>
       <c r="E108" s="25"/>
@@ -21963,17 +22316,17 @@
     </row>
     <row r="109" spans="1:9" s="29" customFormat="1" ht="14.25">
       <c r="A109" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>85</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>207</v>
+      <c r="B109" s="54" t="s">
+        <v>218</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D109" s="24"/>
-      <c r="E109" s="25"/>
+        <v>280</v>
+      </c>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
@@ -21981,81 +22334,81 @@
     </row>
     <row r="110" spans="1:9" s="29" customFormat="1" ht="14.25">
       <c r="A110" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>86</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D110" s="24"/>
+        <v>280</v>
+      </c>
+      <c r="D110" s="1"/>
       <c r="E110" s="25"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
       <c r="I110" s="67"/>
     </row>
-    <row r="111" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A111" s="65">
-        <f t="shared" ca="1" si="0"/>
-        <v>87</v>
-      </c>
-      <c r="B111" s="54" t="s">
-        <v>220</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
-      <c r="G111" s="1"/>
-      <c r="H111" s="1"/>
-      <c r="I111" s="67"/>
+    <row r="111" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A111" s="43"/>
+      <c r="B111" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="C111" s="61"/>
+      <c r="D111" s="62"/>
+      <c r="E111" s="63"/>
+      <c r="F111" s="64"/>
+      <c r="G111" s="64"/>
+      <c r="H111" s="64"/>
+      <c r="I111" s="63"/>
     </row>
     <row r="112" spans="1:9" s="29" customFormat="1" ht="14.25">
       <c r="A112" s="65">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D112" s="1"/>
+        <v>280</v>
+      </c>
+      <c r="D112" s="24"/>
       <c r="E112" s="25"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
       <c r="I112" s="67"/>
     </row>
-    <row r="113" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A113" s="43"/>
-      <c r="B113" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="C113" s="61"/>
-      <c r="D113" s="62"/>
-      <c r="E113" s="63"/>
-      <c r="F113" s="64"/>
-      <c r="G113" s="64"/>
-      <c r="H113" s="64"/>
-      <c r="I113" s="63"/>
+    <row r="113" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A113" s="65">
+        <f t="shared" ref="A113:A114" ca="1" si="2">IF(OFFSET(A113,-1,0) ="",OFFSET(A113,-2,0)+1,OFFSET(A113,-1,0)+1 )</f>
+        <v>88</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D113" s="24"/>
+      <c r="E113" s="25"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="67"/>
     </row>
     <row r="114" spans="1:9" s="29" customFormat="1" ht="14.25">
       <c r="A114" s="65">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>89</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D114" s="24"/>
       <c r="E114" s="25"/>
@@ -22064,34 +22417,29 @@
       <c r="H114" s="1"/>
       <c r="I114" s="67"/>
     </row>
-    <row r="115" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A115" s="65">
-        <f t="shared" ref="A115:A116" ca="1" si="2">IF(OFFSET(A115,-1,0) ="",OFFSET(A115,-2,0)+1,OFFSET(A115,-1,0)+1 )</f>
-        <v>90</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D115" s="24"/>
-      <c r="E115" s="25"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="67"/>
+    <row r="115" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A115" s="43"/>
+      <c r="B115" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C115" s="61"/>
+      <c r="D115" s="62"/>
+      <c r="E115" s="63"/>
+      <c r="F115" s="64"/>
+      <c r="G115" s="64"/>
+      <c r="H115" s="64"/>
+      <c r="I115" s="63"/>
     </row>
     <row r="116" spans="1:9" s="29" customFormat="1" ht="14.25">
       <c r="A116" s="65">
-        <f t="shared" ca="1" si="2"/>
-        <v>91</v>
+        <f t="shared" ref="A116" ca="1" si="3">IF(OFFSET(A116,-1,0) ="",OFFSET(A116,-2,0)+1,OFFSET(A116,-1,0)+1 )</f>
+        <v>90</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D116" s="24"/>
       <c r="E116" s="25"/>
@@ -22100,85 +22448,90 @@
       <c r="H116" s="1"/>
       <c r="I116" s="67"/>
     </row>
-    <row r="117" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A117" s="43"/>
-      <c r="B117" s="53" t="s">
-        <v>167</v>
-      </c>
-      <c r="C117" s="61"/>
-      <c r="D117" s="62"/>
-      <c r="E117" s="63"/>
-      <c r="F117" s="64"/>
-      <c r="G117" s="64"/>
-      <c r="H117" s="64"/>
-      <c r="I117" s="63"/>
+    <row r="117" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A117" s="71">
+        <f ca="1">IF(OFFSET(A117,-1,0) ="",OFFSET(A117,-2,0)+1,OFFSET(A117,-1,0)+1 )</f>
+        <v>91</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D117" s="24"/>
+      <c r="E117" s="25"/>
+      <c r="F117" s="25"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="71"/>
     </row>
     <row r="118" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A118" s="65">
-        <f t="shared" ref="A118" ca="1" si="3">IF(OFFSET(A118,-1,0) ="",OFFSET(A118,-2,0)+1,OFFSET(A118,-1,0)+1 )</f>
+      <c r="A118" s="71">
+        <f t="shared" ref="A118:A128" ca="1" si="4">IF(OFFSET(A118,-1,0) ="",OFFSET(A118,-2,0)+1,OFFSET(A118,-1,0)+1 )</f>
         <v>92</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D118" s="24"/>
       <c r="E118" s="25"/>
-      <c r="F118" s="1"/>
+      <c r="F118" s="25"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
-      <c r="I118" s="67"/>
-    </row>
-    <row r="119" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A119" s="71">
-        <f ca="1">IF(OFFSET(A119,-1,0) ="",OFFSET(A119,-2,0)+1,OFFSET(A119,-1,0)+1 )</f>
+      <c r="I118" s="71"/>
+    </row>
+    <row r="119" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A119" s="68"/>
+      <c r="B119" s="90" t="s">
+        <v>213</v>
+      </c>
+      <c r="C119" s="91"/>
+      <c r="D119" s="92"/>
+      <c r="E119" s="69"/>
+      <c r="F119" s="32"/>
+      <c r="G119" s="32"/>
+      <c r="H119" s="32"/>
+      <c r="I119" s="69"/>
+    </row>
+    <row r="120" spans="1:9" s="27" customFormat="1">
+      <c r="A120" s="71">
+        <f t="shared" ca="1" si="4"/>
         <v>93</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D119" s="24"/>
-      <c r="E119" s="25"/>
-      <c r="F119" s="25"/>
-      <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
-      <c r="I119" s="71"/>
-    </row>
-    <row r="120" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A120" s="71">
-        <f t="shared" ref="A120:A130" ca="1" si="4">IF(OFFSET(A120,-1,0) ="",OFFSET(A120,-2,0)+1,OFFSET(A120,-1,0)+1 )</f>
-        <v>94</v>
-      </c>
       <c r="B120" s="1" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D120" s="24"/>
       <c r="E120" s="25"/>
-      <c r="F120" s="25"/>
+      <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
-      <c r="I120" s="71"/>
-    </row>
-    <row r="121" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A121" s="68"/>
-      <c r="B121" s="90" t="s">
-        <v>215</v>
-      </c>
-      <c r="C121" s="91"/>
-      <c r="D121" s="92"/>
-      <c r="E121" s="69"/>
-      <c r="F121" s="32"/>
-      <c r="G121" s="32"/>
-      <c r="H121" s="32"/>
-      <c r="I121" s="69"/>
+      <c r="I120" s="26"/>
+    </row>
+    <row r="121" spans="1:9" s="27" customFormat="1">
+      <c r="A121" s="71">
+        <f t="shared" ca="1" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D121" s="24"/>
+      <c r="E121" s="25"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="26"/>
     </row>
     <row r="122" spans="1:9" s="27" customFormat="1">
       <c r="A122" s="71">
@@ -22186,10 +22539,10 @@
         <v>95</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D122" s="24"/>
       <c r="E122" s="25"/>
@@ -22203,11 +22556,11 @@
         <f t="shared" ca="1" si="4"/>
         <v>96</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>214</v>
+      <c r="B123" s="54" t="s">
+        <v>161</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D123" s="24"/>
       <c r="E123" s="25"/>
@@ -22221,11 +22574,11 @@
         <f t="shared" ca="1" si="4"/>
         <v>97</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>213</v>
+      <c r="B124" s="54" t="s">
+        <v>162</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D124" s="24"/>
       <c r="E124" s="25"/>
@@ -22240,10 +22593,10 @@
         <v>98</v>
       </c>
       <c r="B125" s="54" t="s">
-        <v>161</v>
+        <v>214</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D125" s="24"/>
       <c r="E125" s="25"/>
@@ -22257,11 +22610,11 @@
         <f t="shared" ca="1" si="4"/>
         <v>99</v>
       </c>
-      <c r="B126" s="54" t="s">
-        <v>162</v>
+      <c r="B126" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D126" s="24"/>
       <c r="E126" s="25"/>
@@ -22275,11 +22628,11 @@
         <f t="shared" ca="1" si="4"/>
         <v>100</v>
       </c>
-      <c r="B127" s="54" t="s">
+      <c r="B127" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D127" s="24"/>
       <c r="E127" s="25"/>
@@ -22297,7 +22650,7 @@
         <v>217</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D128" s="24"/>
       <c r="E128" s="25"/>
@@ -22306,61 +22659,25 @@
       <c r="H128" s="1"/>
       <c r="I128" s="26"/>
     </row>
-    <row r="129" spans="1:9" s="27" customFormat="1">
-      <c r="A129" s="71">
-        <f t="shared" ca="1" si="4"/>
-        <v>102</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D129" s="24"/>
-      <c r="E129" s="25"/>
-      <c r="F129" s="1"/>
-      <c r="G129" s="1"/>
-      <c r="H129" s="1"/>
-      <c r="I129" s="26"/>
-    </row>
-    <row r="130" spans="1:9" s="27" customFormat="1">
-      <c r="A130" s="71">
-        <f t="shared" ca="1" si="4"/>
-        <v>103</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D130" s="24"/>
-      <c r="E130" s="25"/>
-      <c r="F130" s="1"/>
-      <c r="G130" s="1"/>
-      <c r="H130" s="1"/>
-      <c r="I130" s="26"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B119:D119"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B121:D121"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F69:H69 F18:H19 F88:H88 F113:H113 F32:H32 F45:H45 F94:H94 F117:H117"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F68:H68 F18:H19 F87:H87 F111:H111 F32:H32 F45:H45 F92:H92 F115:H115"/>
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
-    <dataValidation type="list" allowBlank="1" sqref="F114:H116 F70:H87 F118:H130 F46:H68 F89:H93 F95:H112 F33:H44 F20:H31">
+    <dataValidation type="list" allowBlank="1" sqref="F112:H114 F69:H86 F116:H128 F93:H110 F33:H44 F20:H31 F46:H67 F88:H91">
       <formula1>$A$11:$A$15</formula1>
     </dataValidation>
   </dataValidations>
@@ -22374,7 +22691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
@@ -22678,7 +22995,7 @@
     <row r="18" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="22"/>
       <c r="B18" s="79" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C18" s="80"/>
       <c r="D18" s="81"/>
@@ -22773,7 +23090,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="24"/>
@@ -22802,7 +23119,7 @@
     <row r="26" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A26" s="22"/>
       <c r="B26" s="79" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C26" s="80"/>
       <c r="D26" s="81"/>
@@ -22815,7 +23132,7 @@
     <row r="27" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A27" s="46"/>
       <c r="B27" s="55" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C27" s="44"/>
       <c r="D27" s="45"/>
@@ -22830,7 +23147,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="24"/>
@@ -22846,7 +23163,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="24"/>
@@ -22862,7 +23179,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="24"/>
@@ -22878,7 +23195,7 @@
         <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="24"/>
@@ -22894,7 +23211,7 @@
         <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="24"/>
@@ -22910,7 +23227,7 @@
         <v>13</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="24"/>
@@ -22926,7 +23243,7 @@
         <v>14</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="24"/>
@@ -22942,7 +23259,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="24"/>
@@ -22958,7 +23275,7 @@
         <v>16</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="24"/>
@@ -22971,7 +23288,7 @@
     <row r="37" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="46"/>
       <c r="B37" s="55" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C37" s="44"/>
       <c r="D37" s="45"/>
@@ -22987,7 +23304,7 @@
         <v>17</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="24"/>
@@ -23003,7 +23320,7 @@
         <v>18</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="24"/>
@@ -23019,7 +23336,7 @@
         <v>19</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="24"/>
@@ -23035,7 +23352,7 @@
         <v>20</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="24"/>
@@ -23051,7 +23368,7 @@
         <v>21</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="24"/>
@@ -23064,7 +23381,7 @@
     <row r="43" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A43" s="46"/>
       <c r="B43" s="55" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C43" s="44"/>
       <c r="D43" s="45"/>
@@ -23080,7 +23397,7 @@
         <v>22</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="24"/>
@@ -23096,7 +23413,7 @@
         <v>23</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="24"/>
@@ -23112,7 +23429,7 @@
         <v>24</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="24"/>
@@ -23128,7 +23445,7 @@
         <v>25</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="24"/>
@@ -23144,7 +23461,7 @@
         <v>26</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="24"/>
@@ -23157,7 +23474,7 @@
     <row r="49" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A49" s="46"/>
       <c r="B49" s="55" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C49" s="44"/>
       <c r="D49" s="45"/>
@@ -23173,11 +23490,11 @@
         <v>27</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E50" s="25"/>
       <c r="F50" s="25"/>
@@ -23191,11 +23508,11 @@
         <v>28</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E51" s="25"/>
       <c r="F51" s="1"/>
@@ -23209,11 +23526,11 @@
         <v>29</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E52" s="25"/>
       <c r="F52" s="25"/>
@@ -23227,11 +23544,11 @@
         <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E53" s="25"/>
       <c r="F53" s="1"/>
@@ -23242,7 +23559,7 @@
     <row r="54" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A54" s="46"/>
       <c r="B54" s="55" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C54" s="44"/>
       <c r="D54" s="45"/>
@@ -23255,7 +23572,7 @@
     <row r="55" spans="1:9" s="76" customFormat="1" ht="15.75" customHeight="1">
       <c r="A55" s="72"/>
       <c r="B55" s="77" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C55" s="73"/>
       <c r="D55" s="74"/>
@@ -23271,11 +23588,11 @@
         <v>31</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E56" s="25"/>
       <c r="F56" s="25"/>
@@ -23289,11 +23606,11 @@
         <v>32</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E57" s="25"/>
       <c r="F57" s="25"/>
@@ -23307,11 +23624,11 @@
         <v>33</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E58" s="25"/>
       <c r="F58" s="25"/>
@@ -23322,7 +23639,7 @@
     <row r="59" spans="1:9" s="76" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="72"/>
       <c r="B59" s="77" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C59" s="73"/>
       <c r="D59" s="74"/>
@@ -23338,11 +23655,11 @@
         <v>34</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E60" s="25"/>
       <c r="F60" s="25"/>
@@ -23356,11 +23673,11 @@
         <v>35</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E61" s="25"/>
       <c r="F61" s="1"/>
@@ -23374,11 +23691,11 @@
         <v>36</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E62" s="25"/>
       <c r="F62" s="25"/>
@@ -23392,11 +23709,11 @@
         <v>37</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E63" s="25"/>
       <c r="F63" s="1"/>
@@ -23410,11 +23727,11 @@
         <v>38</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E64" s="25"/>
       <c r="F64" s="25"/>
@@ -23428,11 +23745,11 @@
         <v>39</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E65" s="25"/>
       <c r="F65" s="25"/>
@@ -23443,7 +23760,7 @@
     <row r="66" spans="1:9" s="76" customFormat="1" ht="15.75" customHeight="1">
       <c r="A66" s="72"/>
       <c r="B66" s="77" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C66" s="73"/>
       <c r="D66" s="74"/>
@@ -23459,11 +23776,11 @@
         <v>40</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E67" s="25"/>
       <c r="F67" s="25"/>
@@ -23477,11 +23794,11 @@
         <v>41</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E68" s="25"/>
       <c r="F68" s="1"/>
@@ -23495,11 +23812,11 @@
         <v>42</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E69" s="25"/>
       <c r="F69" s="25"/>
@@ -23513,11 +23830,11 @@
         <v>43</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E70" s="25"/>
       <c r="F70" s="1"/>
@@ -23531,11 +23848,11 @@
         <v>44</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E71" s="25"/>
       <c r="F71" s="25"/>
@@ -23549,11 +23866,11 @@
         <v>45</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E72" s="25"/>
       <c r="F72" s="25"/>
@@ -23564,7 +23881,7 @@
     <row r="73" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A73" s="46"/>
       <c r="B73" s="55" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C73" s="44"/>
       <c r="D73" s="45"/>
@@ -23596,7 +23913,7 @@
         <v>47</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -23612,7 +23929,7 @@
         <v>48</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -23628,7 +23945,7 @@
         <v>49</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="24"/>
@@ -23644,7 +23961,7 @@
         <v>50</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="24"/>
@@ -23656,6 +23973,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="A1:D1"/>
@@ -23663,11 +23985,6 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:H27 F18:H18 F37:H37 F43:H43 F49:H49 F73:H73 F54:H55 F59:H59 F66:H66"/>

</xml_diff>

<commit_message>
updated file on 23/10 (3) - Assignment 2,3
</commit_message>
<xml_diff>
--- a/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
+++ b/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
@@ -264,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F118" authorId="0" shapeId="0">
+    <comment ref="F117" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -453,7 +453,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="427">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -1155,21 +1155,12 @@
     <t>Check Copy/Paste Full Name</t>
   </si>
   <si>
-    <t>Sign up successfully when all fields are entered valid data</t>
-  </si>
-  <si>
     <t>Sign up fail when all fields are entered invalid data</t>
   </si>
   <si>
-    <t>Sign up successfully when all mandatory fields are entered valid data</t>
-  </si>
-  <si>
     <t>2. Check function</t>
   </si>
   <si>
-    <t>When the user clicks Terms and conditions</t>
-  </si>
-  <si>
     <t>Check slide function when the user doesn't enter phone number</t>
   </si>
   <si>
@@ -1177,9 +1168,6 @@
   </si>
   <si>
     <t>Check slide function when the user enters invalid phone number</t>
-  </si>
-  <si>
-    <t>When the user enters valid Full Name</t>
   </si>
   <si>
     <t xml:space="preserve">When the user enters Product Name </t>
@@ -1364,9 +1352,6 @@
   <si>
     <t xml:space="preserve">1. Open Lazada registration page
 2. Observe the display of the Phone Numer </t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page</t>
   </si>
   <si>
     <t>Phone number is blank 
@@ -1381,14 +1366,6 @@
   </si>
   <si>
     <t>Allow copy/paste phone number</t>
-  </si>
-  <si>
-    <t>Spaces are removed, SMS code is sent to the entered phone number</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter space at the beginning and the end of the phone number
-3. Slide to get SMS code</t>
   </si>
   <si>
     <t xml:space="preserve">When the user enters 10 numeric characters  </t>
@@ -1465,11 +1442,6 @@
 2. Enter alphabetic characters</t>
   </si>
   <si>
-    <t>1. Open Lazada registration page
-2. Enter invalid phone number
-3. Slide to get SMS code</t>
-  </si>
-  <si>
     <t>System will show error message “Please enter SMS Verification Code”</t>
   </si>
   <si>
@@ -1512,9 +1484,309 @@
   </si>
   <si>
     <t>1. Open Lazada registration page
+2. Enter valid phone number
+3. Slide to get SMS code
+4. Enter characters
+3. Click on close (x) button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter valid phone number
+3. Slide to get SMS code
+4. Enter space into SMS Verification Code</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Observe the display of the Password</t>
+  </si>
+  <si>
+    <t>Password is blank 
+The placeholder is "Minimum 6 characters with a number and a letter"
+There is a symbol * marks Password as a mandatory field</t>
+  </si>
+  <si>
+    <t>System will show error message “Please enter Password”</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter only alphabetic characters</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter only special characters</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter only numberic characters</t>
+  </si>
+  <si>
+    <t>System will show error message "Password should contain alphabetic and numeric characters"</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter numeric and special characters</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter alphabetic and special characters</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Copy/Paste password</t>
+  </si>
+  <si>
+    <t>Do not allow copy/paste password</t>
+  </si>
+  <si>
+    <t>Spaces are removed
+Sign up successfully, return to login screen</t>
+  </si>
+  <si>
+    <t>System will show error message "The length of Password should be 6-50 characters"</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 5 characters</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter valid phone number
+3. Slide to get SMS code
+4. Enter 5 numeric characters in SMS Verification Code box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Lazada registration page
+2. Enter 51 characters
+</t>
+  </si>
+  <si>
+    <t>Password is shown</t>
+  </si>
+  <si>
+    <t>Password is hided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Lazada registration page
+2. Observe the display of the Eye icon
+3. Enter any character </t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+4. Enter characters
+3. Click on close (x) button</t>
+  </si>
+  <si>
+    <t>Month is blank, the placeholder is "Month"
+Day is blank, the placeholder is "Day"
+Year is blank, the placeholder is "Year"</t>
+  </si>
+  <si>
+    <t>System will show error message “Please select the correct birthday"</t>
+  </si>
+  <si>
+    <t>System will show error message  “Please select the correct birthday"</t>
+  </si>
+  <si>
+    <t>System will show error message “Wrong birthday format"</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select future date</t>
+  </si>
+  <si>
+    <t>There is a scrollbar when the list of Months exceeds the display frame</t>
+  </si>
+  <si>
+    <t>There is a scrollbar when the list of Days exceeds the display frame</t>
+  </si>
+  <si>
+    <t>There is a scrollbar when the list of Years exceeds the display frame</t>
+  </si>
+  <si>
+    <t>The months are fully displayed in the dropdown list and sorted in ascending order</t>
+  </si>
+  <si>
+    <t>Do not allow enter from keyboard</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Observe the display of the Birthday</t>
+  </si>
+  <si>
+    <t>Gender is blank
+The placeholder is "Select"</t>
+  </si>
+  <si>
+    <t>The days are fully displayed in the dropdown list and sorted in ascending order</t>
+  </si>
+  <si>
+    <t>List of years starting from 1990 to 2022 and sorted in descending order</t>
+  </si>
+  <si>
+    <t>There are 2 values: Female and male</t>
+  </si>
+  <si>
+    <t>srollbar maybe not need</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on Month</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on Day</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on Year</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on Gender</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter characters from keyboard</t>
+  </si>
+  <si>
+    <t>System will show error message “Please enter Full Name”</t>
+  </si>
+  <si>
+    <t>System will show error message "The length of Full Name should be 6-50 characters"</t>
+  </si>
+  <si>
+    <t>Full Name is blank 
+The placeholder is "First Last"
+There is a symbol * marks Full Name as a mandatory field</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Observe the display of the Full Name</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Copy/Paste Full Name</t>
+  </si>
+  <si>
+    <t>System will show error message "Full Name should not contain special characters"</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter numeric, alphabetic and special characters</t>
+  </si>
+  <si>
+    <t>Allow copy/paste Full Name</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Observe the display of the Check box</t>
+  </si>
+  <si>
+    <t>There is a check mark in the Check box</t>
+  </si>
+  <si>
+    <t>The Check box is blank</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on ‘Sign up with Email’ button</t>
+  </si>
+  <si>
+    <t>System will show the page to create new account with Email address</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on ‘Facebook’ button</t>
+  </si>
+  <si>
+    <t>New pop-up will be displayed to confirm if user is ready to continue login with Facebook</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on ‘Google’ button</t>
+  </si>
+  <si>
+    <t>New pop-up will be displayed with Google account so that user can select desired account he want to use</t>
+  </si>
+  <si>
+    <t>Sign up successfully when all fields are entered valid datas</t>
+  </si>
+  <si>
+    <t>Sign up successfully when all mandatory fields are entered valid datas</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter invalid phone number 
+3. Slide to get SMS code</t>
+  </si>
+  <si>
+    <t>0000000001</t>
+  </si>
+  <si>
+    <t>0981980721</t>
+  </si>
+  <si>
+    <t>31/2/1999</t>
+  </si>
+  <si>
+    <t>System will show error message "Please enter the sms code"</t>
+  </si>
+  <si>
+    <t>System will show error message "This phone number is linked to another account, please enter another number"</t>
+  </si>
+  <si>
+    <t>System will show error message "Invalid verification code"</t>
+  </si>
+  <si>
+    <t>Go to the page of Terms and conditions</t>
+  </si>
+  <si>
+    <t>When the user clicks on Terms and conditions</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter valid phone number 
+3. Slide to get SMS code</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 11 numeric characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Lazada registration page
+2. Enter 9 numeric characters
+</t>
+  </si>
+  <si>
+    <t>SMS code is sent to the entered phone number</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2.  Don't select Check box</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select Check box</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter space at the beginning and the end of the valid phone number
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
 2. Enter 10 numeric characters (valid phone number)
 3. Other fields are valid
-4. Click Sign up button</t>
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter valid phone number
+3. Slide to get SMS code
+2. Don't enter character
+4. Other fields are valid
+5. Click on Sign Up button</t>
   </si>
   <si>
     <t>1. Open Lazada registration page
@@ -1522,7 +1794,7 @@
 3. Slide to get SMS code
 4. Enter 6 numeric characters (valid SMS Verification Code)
 5. Other fields are valid
-6. Click Sign Up button</t>
+6. Click on Sign Up button</t>
   </si>
   <si>
     <t>1. Open Lazada registration page
@@ -1530,319 +1802,205 @@
 3. Slide to get SMS code
 4. Enter invalid SMS Verification Code
 5. Other fields are valid
-6. Click Sign Up button</t>
+6. Click on Sign Up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Don't enter character
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter alphabetic and numeric characters
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter numeric, alphabetic and special characters
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter space at the beginning and the end of the password
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 6 characters (valid password)
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 10 characters (valid password) 
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 50 characters (valid password) 
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter a valid password where all letters are uppercase
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter a valid password where all letters are lowercase
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on on the Eye icon to show the password</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on on the Eye icon to hide the password</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Don't select birthday
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Month
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Day
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Year
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Month and Day
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Month and Year
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select only Year and Day
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select valid date
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Select invalid date
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on on Day</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Don't select Gender
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter only alphabetic characters
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter only numberic characters
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter space at the beginning and the end of the Full Name
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 6 characters (valid Full Name)
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 10 characters (valid Full Name) 
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter 50 characters (valid Full Name) 
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. All fields are entered valid datas
+3. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. All mandatory fields are entered valid datas
+3. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. All fields are entered invalid datas
+3. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter a registered Phone Number
+3. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Enter expired SMS code
+3. Other fields are valid
+4. Click on Sign up button</t>
+  </si>
+  <si>
+    <t>1. Open Lazada registration page
+2. Click on on Terms and conditions</t>
   </si>
   <si>
     <t>1. Open Lazada registration page
 2. Enter valid phone number
 3. Slide to get SMS code
-4. Enter characters
-3. Click on close (x) button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter valid phone number
-3. Slide to get SMS code
-2. Don't enter character
-4. Other fields are valid
-5. Click Sign Up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter valid phone number
-3. Slide to get SMS code
-4. Enter space into SMS Verification Code</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Observe the display of the Password</t>
-  </si>
-  <si>
-    <t>Password is blank 
-The placeholder is "Minimum 6 characters with a number and a letter"
-There is a symbol * marks Password as a mandatory field</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Don't enter character
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>System will show error message “Please enter Password”</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter only alphabetic characters</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter only special characters</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter only numberic characters</t>
-  </si>
-  <si>
-    <t>System will show error message "Password should contain alphabetic and numeric characters"</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter numeric and special characters</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter alphabetic and special characters</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter alphabetic and numeric characters
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter numeric, alphabetic and special characters
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Copy/Paste password</t>
-  </si>
-  <si>
-    <t>Do not allow copy/paste password</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter space at the beginning and the end of the password
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>Spaces are removed
-Sign up successfully, return to login screen</t>
-  </si>
-  <si>
-    <t>System will show error message "The length of Password should be 6-50 characters"</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter 6 characters (valid password)
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter 10 characters (valid password) 
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter 50 characters (valid password) 
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter 5 characters</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter valid phone number
-3. Slide to get SMS code
-4. Enter 5 numeric characters in SMS Verification Code box</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter valid phone number
-3. Slide to get SMS code
-4. Enter 17 numeric characters in SMS Verification Code box</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter 11 numeric characters
-3. Slide to get SMS code</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter 9 numeric characters
-3. Slide to get SMS code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open Lazada registration page
-2. Enter 51 characters
-</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter a valid password where all letters are uppercase
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter a valid password where all letters are lowercase
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>Password is shown</t>
-  </si>
-  <si>
-    <t>Password is hided</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open Lazada registration page
-2. Observe the display of the Eye icon
-3. Enter any character </t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Click on the Eye icon to show the password</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Click on the Eye icon to hide the password</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-4. Enter characters
-3. Click on close (x) button</t>
-  </si>
-  <si>
-    <t>Month is blank, the placeholder is "Month"
-Day is blank, the placeholder is "Day"
-Year is blank, the placeholder is "Year"</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Don't select birthday
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Select only Month
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Select only Day
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Select only Year
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Select only Month and Day
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Select only Month and Year
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Select only Year and Day
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Select valid date
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Select invalid date
-3. Other fields are valid
-4. Click Sign up button</t>
-  </si>
-  <si>
-    <t>System will show error message “Please select the correct birthday"</t>
-  </si>
-  <si>
-    <t>System will show error message  “Please select the correct birthday"</t>
-  </si>
-  <si>
-    <t>System will show error message “Wrong birthday format"</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Select future date</t>
-  </si>
-  <si>
-    <t>There is a scrollbar when the list of Months exceeds the display frame</t>
-  </si>
-  <si>
-    <t>There is a scrollbar when the list of Days exceeds the display frame</t>
-  </si>
-  <si>
-    <t>There is a scrollbar when the list of Years exceeds the display frame</t>
-  </si>
-  <si>
-    <t>The months are fully displayed in the dropdown list and sorted in ascending order</t>
-  </si>
-  <si>
-    <t>Do not allow enter from keyboard</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Observe the display of the Birthday</t>
-  </si>
-  <si>
-    <t>Gender is blank
-The placeholder is "Select"</t>
-  </si>
-  <si>
-    <t>The days are fully displayed in the dropdown list and sorted in ascending order</t>
-  </si>
-  <si>
-    <t>List of years starting from 1990 to 2022 and sorted in descending order</t>
-  </si>
-  <si>
-    <t>There are 2 values: Female and male</t>
-  </si>
-  <si>
-    <t>srollbar maybe not need</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Click on Month</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Click on Day</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Click on Year</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Click on Gender</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Enter characters from keyboard</t>
-  </si>
-  <si>
-    <t>1. Open Lazada registration page
-2. Don't select Gender
-3. Other fields are valid
-4. Click Sign up button</t>
+4. Enter 7 numeric characters in SMS Verification Code box</t>
   </si>
 </sst>
 </file>
@@ -2160,7 +2318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2411,6 +2569,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -20256,10 +20420,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -20426,15 +20590,15 @@
         <v>13</v>
       </c>
       <c r="B11" s="15">
-        <f>COUNTIF($F$18:$F$126,"*Passed")</f>
+        <f>COUNTIF($F$18:$F$125,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="C11" s="15">
-        <f>COUNTIF($G$18:$G$126,"*Passed")</f>
+        <f>COUNTIF($G$18:$G$125,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="D11" s="15">
-        <f>COUNTIF($H$18:$H$126,"*Passed")</f>
+        <f>COUNTIF($H$18:$H$125,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="E11" s="56"/>
@@ -20448,15 +20612,15 @@
         <v>14</v>
       </c>
       <c r="B12" s="15">
-        <f>COUNTIF($F$18:$F$126,"*Failed*")</f>
+        <f>COUNTIF($F$18:$F$125,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="C12" s="15">
-        <f>COUNTIF($G$18:$G$126,"*Failed*")</f>
+        <f>COUNTIF($G$18:$G$125,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="D12" s="15">
-        <f>COUNTIF($H$18:$H$126,"*Failed*")</f>
+        <f>COUNTIF($H$18:$H$125,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="E12" s="56"/>
@@ -20470,15 +20634,15 @@
         <v>15</v>
       </c>
       <c r="B13" s="15">
-        <f>COUNTIF($F$18:$F$126,"*Not Run*")</f>
+        <f>COUNTIF($F$18:$F$125,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="C13" s="15">
-        <f>COUNTIF($G$18:$G$126,"*Not Run*")</f>
+        <f>COUNTIF($G$18:$G$125,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="D13" s="15">
-        <f>COUNTIF($H$18:$H$126,"*Not Run*")</f>
+        <f>COUNTIF($H$18:$H$125,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="E13" s="8"/>
@@ -20492,15 +20656,15 @@
         <v>16</v>
       </c>
       <c r="B14" s="15">
-        <f>COUNTIF($F$18:$F$126,"*NA*")</f>
+        <f>COUNTIF($F$18:$F$125,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="C14" s="15">
-        <f>COUNTIF($G$18:$G$126,"*NA*")</f>
+        <f>COUNTIF($G$18:$G$125,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="D14" s="15">
-        <f>COUNTIF($H$18:$H$126,"*NA*")</f>
+        <f>COUNTIF($H$18:$H$125,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="E14" s="8"/>
@@ -20514,15 +20678,15 @@
         <v>17</v>
       </c>
       <c r="B15" s="15">
-        <f>COUNTIF($F$18:$F$126,"*Passed in previous build*")</f>
+        <f>COUNTIF($F$18:$F$125,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="C15" s="15">
-        <f>COUNTIF($G$18:$G$126,"*Passed in previous build*")</f>
+        <f>COUNTIF($G$18:$G$125,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="D15" s="15">
-        <f>COUNTIF($H$18:$H$126,"*Passed in previous build*")</f>
+        <f>COUNTIF($H$18:$H$125,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="E15" s="8"/>
@@ -20601,17 +20765,17 @@
     </row>
     <row r="20" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A20" s="65">
-        <f t="shared" ref="A20:A112" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
+        <f t="shared" ref="A20:A111" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="1"/>
@@ -20628,10 +20792,10 @@
         <v>166</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="1"/>
@@ -20648,10 +20812,10 @@
         <v>163</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="1"/>
@@ -20668,10 +20832,10 @@
         <v>164</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="1"/>
@@ -20688,10 +20852,10 @@
         <v>165</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E24" s="25"/>
       <c r="F24" s="1"/>
@@ -20708,10 +20872,10 @@
         <v>170</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E25" s="25"/>
       <c r="F25" s="1"/>
@@ -20719,7 +20883,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="26"/>
     </row>
-    <row r="26" spans="1:9" s="27" customFormat="1" ht="51">
+    <row r="26" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A26" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>7</v>
@@ -20728,10 +20892,10 @@
         <v>169</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>286</v>
+        <v>387</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>285</v>
+        <v>323</v>
       </c>
       <c r="E26" s="25"/>
       <c r="F26" s="1"/>
@@ -20745,13 +20909,13 @@
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>348</v>
+        <v>383</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E27" s="25"/>
       <c r="F27" s="1"/>
@@ -20765,15 +20929,17 @@
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>318</v>
+        <v>388</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>301</v>
-      </c>
-      <c r="E28" s="25"/>
+        <v>294</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>374</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -20785,13 +20951,13 @@
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>347</v>
+        <v>382</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -20808,12 +20974,14 @@
         <v>200</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>309</v>
+        <v>372</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>296</v>
-      </c>
-      <c r="E30" s="1"/>
+        <v>289</v>
+      </c>
+      <c r="E30" s="93" t="s">
+        <v>373</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -20828,10 +20996,10 @@
         <v>160</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D31" s="70" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="1"/>
@@ -20861,10 +21029,10 @@
         <v>168</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E33" s="25"/>
       <c r="F33" s="1"/>
@@ -20881,10 +21049,10 @@
         <v>173</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>322</v>
+        <v>389</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E34" s="25"/>
       <c r="F34" s="1"/>
@@ -20901,10 +21069,10 @@
         <v>163</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="E35" s="25"/>
       <c r="F35" s="1"/>
@@ -20921,10 +21089,10 @@
         <v>164</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E36" s="25"/>
       <c r="F36" s="1"/>
@@ -20941,10 +21109,10 @@
         <v>165</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E37" s="25"/>
       <c r="F37" s="1"/>
@@ -20961,10 +21129,10 @@
         <v>208</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E38" s="25"/>
       <c r="F38" s="1"/>
@@ -20981,10 +21149,10 @@
         <v>169</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E39" s="25"/>
       <c r="F39" s="1"/>
@@ -20998,13 +21166,13 @@
         <v>20</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="E40" s="25"/>
       <c r="F40" s="1"/>
@@ -21018,13 +21186,13 @@
         <v>21</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>319</v>
+        <v>390</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E41" s="25"/>
       <c r="F41" s="1"/>
@@ -21038,13 +21206,13 @@
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>346</v>
+        <v>426</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="E42" s="25"/>
       <c r="F42" s="1"/>
@@ -21058,13 +21226,13 @@
         <v>23</v>
       </c>
       <c r="B43" s="54" t="s">
+        <v>291</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D43" s="24" t="s">
         <v>298</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>305</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -21081,10 +21249,10 @@
         <v>160</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="D44" s="70" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E44" s="25"/>
       <c r="F44" s="1"/>
@@ -21114,10 +21282,10 @@
         <v>168</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="E46" s="25"/>
       <c r="F46" s="1"/>
@@ -21134,10 +21302,10 @@
         <v>173</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>326</v>
+        <v>392</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="E47" s="25"/>
       <c r="F47" s="1"/>
@@ -21154,10 +21322,10 @@
         <v>201</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="E48" s="25"/>
       <c r="F48" s="1"/>
@@ -21174,10 +21342,10 @@
         <v>202</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="E49" s="25"/>
       <c r="F49" s="1"/>
@@ -21194,10 +21362,10 @@
         <v>203</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="E50" s="25"/>
       <c r="F50" s="1"/>
@@ -21214,10 +21382,10 @@
         <v>174</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>334</v>
+        <v>393</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E51" s="25"/>
       <c r="F51" s="1"/>
@@ -21234,10 +21402,10 @@
         <v>175</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="E52" s="25"/>
       <c r="F52" s="1"/>
@@ -21254,10 +21422,10 @@
         <v>176</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="E53" s="25"/>
       <c r="F53" s="1"/>
@@ -21274,10 +21442,10 @@
         <v>177</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>335</v>
+        <v>394</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E54" s="25"/>
       <c r="F54" s="1"/>
@@ -21294,10 +21462,10 @@
         <v>207</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="E55" s="25"/>
       <c r="F55" s="1"/>
@@ -21314,10 +21482,10 @@
         <v>169</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>338</v>
+        <v>395</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="E56" s="25"/>
       <c r="F56" s="1"/>
@@ -21334,10 +21502,10 @@
         <v>171</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="E57" s="25"/>
       <c r="F57" s="1"/>
@@ -21354,10 +21522,10 @@
         <v>172</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>341</v>
+        <v>396</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E58" s="25"/>
       <c r="F58" s="1"/>
@@ -21374,10 +21542,10 @@
         <v>178</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>342</v>
+        <v>397</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E59" s="25"/>
       <c r="F59" s="1"/>
@@ -21394,10 +21562,10 @@
         <v>205</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>343</v>
+        <v>398</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E60" s="25"/>
       <c r="F60" s="1"/>
@@ -21414,10 +21582,10 @@
         <v>204</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="E61" s="25"/>
       <c r="F61" s="1"/>
@@ -21434,10 +21602,10 @@
         <v>179</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>350</v>
+        <v>399</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E62" s="25"/>
       <c r="F62" s="1"/>
@@ -21454,10 +21622,10 @@
         <v>180</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>351</v>
+        <v>400</v>
       </c>
       <c r="D63" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E63" s="25"/>
       <c r="F63" s="1"/>
@@ -21474,10 +21642,10 @@
         <v>144</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="E64" s="25"/>
       <c r="F64" s="1"/>
@@ -21494,10 +21662,10 @@
         <v>145</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>355</v>
+        <v>401</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="E65" s="25"/>
       <c r="F65" s="1"/>
@@ -21514,10 +21682,10 @@
         <v>146</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>356</v>
+        <v>402</v>
       </c>
       <c r="D66" s="24" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="E66" s="25"/>
       <c r="F66" s="1"/>
@@ -21534,10 +21702,10 @@
         <v>160</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
       <c r="D67" s="70" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E67" s="25"/>
       <c r="F67" s="1"/>
@@ -21567,10 +21735,10 @@
         <v>148</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>377</v>
+        <v>342</v>
       </c>
       <c r="D69" s="24" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
       <c r="E69" s="25"/>
       <c r="F69" s="1"/>
@@ -21587,10 +21755,10 @@
         <v>181</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>359</v>
+        <v>403</v>
       </c>
       <c r="D70" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E70" s="25"/>
       <c r="F70" s="1"/>
@@ -21607,10 +21775,10 @@
         <v>182</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>360</v>
+        <v>404</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="E71" s="25"/>
       <c r="F71" s="1"/>
@@ -21627,10 +21795,10 @@
         <v>183</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>361</v>
+        <v>405</v>
       </c>
       <c r="D72" s="24" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="E72" s="25"/>
       <c r="F72" s="1"/>
@@ -21647,10 +21815,10 @@
         <v>184</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>362</v>
+        <v>406</v>
       </c>
       <c r="D73" s="24" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="E73" s="25"/>
       <c r="F73" s="1"/>
@@ -21667,10 +21835,10 @@
         <v>185</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>363</v>
+        <v>407</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="E74" s="25"/>
       <c r="F74" s="1"/>
@@ -21687,10 +21855,10 @@
         <v>186</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>364</v>
+        <v>408</v>
       </c>
       <c r="D75" s="24" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="E75" s="25"/>
       <c r="F75" s="1"/>
@@ -21707,10 +21875,10 @@
         <v>187</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>365</v>
+        <v>409</v>
       </c>
       <c r="D76" s="24" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="E76" s="25"/>
       <c r="F76" s="1"/>
@@ -21727,10 +21895,10 @@
         <v>194</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>366</v>
+        <v>410</v>
       </c>
       <c r="D77" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E77" s="25"/>
       <c r="F77" s="1"/>
@@ -21747,12 +21915,14 @@
         <v>196</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>367</v>
+        <v>411</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="E78" s="25"/>
+        <v>333</v>
+      </c>
+      <c r="E78" s="25" t="s">
+        <v>375</v>
+      </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
@@ -21767,12 +21937,14 @@
         <v>197</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>371</v>
+        <v>336</v>
       </c>
       <c r="D79" s="24" t="s">
-        <v>370</v>
-      </c>
-      <c r="E79" s="25"/>
+        <v>335</v>
+      </c>
+      <c r="E79" s="94">
+        <v>44604</v>
+      </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
@@ -21787,10 +21959,10 @@
         <v>191</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>383</v>
+        <v>348</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>372</v>
+        <v>337</v>
       </c>
       <c r="E80" s="25"/>
       <c r="F80" s="1"/>
@@ -21807,10 +21979,10 @@
         <v>192</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>384</v>
+        <v>349</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>373</v>
+        <v>338</v>
       </c>
       <c r="E81" s="25"/>
       <c r="F81" s="1"/>
@@ -21827,10 +21999,10 @@
         <v>193</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>385</v>
+        <v>350</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>374</v>
+        <v>339</v>
       </c>
       <c r="E82" s="25"/>
       <c r="F82" s="1"/>
@@ -21847,10 +22019,10 @@
         <v>188</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>383</v>
+        <v>348</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>375</v>
+        <v>340</v>
       </c>
       <c r="E83" s="25"/>
       <c r="F83" s="1"/>
@@ -21867,10 +22039,10 @@
         <v>189</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>384</v>
+        <v>412</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>379</v>
+        <v>344</v>
       </c>
       <c r="E84" s="25"/>
       <c r="F84" s="1"/>
@@ -21887,10 +22059,10 @@
         <v>190</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>385</v>
+        <v>350</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>380</v>
+        <v>345</v>
       </c>
       <c r="E85" s="25"/>
       <c r="F85" s="1"/>
@@ -21907,10 +22079,10 @@
         <v>195</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>387</v>
+        <v>352</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>376</v>
+        <v>341</v>
       </c>
       <c r="E86" s="25"/>
       <c r="F86" s="1"/>
@@ -21940,10 +22112,10 @@
         <v>168</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="D88" s="24" t="s">
-        <v>378</v>
+        <v>343</v>
       </c>
       <c r="E88" s="25"/>
       <c r="F88" s="1"/>
@@ -21960,13 +22132,13 @@
         <v>198</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>386</v>
+        <v>351</v>
       </c>
       <c r="D89" s="24" t="s">
-        <v>381</v>
+        <v>346</v>
       </c>
       <c r="E89" s="25" t="s">
-        <v>382</v>
+        <v>347</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
@@ -21982,10 +22154,10 @@
         <v>199</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="D90" s="24" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E90" s="25"/>
       <c r="F90" s="1"/>
@@ -22002,10 +22174,10 @@
         <v>195</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>387</v>
+        <v>352</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>376</v>
+        <v>341</v>
       </c>
       <c r="E91" s="25"/>
       <c r="F91" s="1"/>
@@ -22026,7 +22198,7 @@
       <c r="H92" s="64"/>
       <c r="I92" s="63"/>
     </row>
-    <row r="93" spans="1:9" s="27" customFormat="1">
+    <row r="93" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A93" s="65">
         <f t="shared" ref="A93:A108" ca="1" si="1">IF(OFFSET(A93,-1,0) ="",OFFSET(A93,-2,0)+1,OFFSET(A93,-1,0)+1 )</f>
         <v>69</v>
@@ -22035,196 +22207,218 @@
         <v>168</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D93" s="24"/>
+        <v>356</v>
+      </c>
+      <c r="D93" s="24" t="s">
+        <v>355</v>
+      </c>
       <c r="E93" s="25"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
       <c r="I93" s="26"/>
     </row>
-    <row r="94" spans="1:9" s="27" customFormat="1">
+    <row r="94" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A94" s="65">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A94,-1,0) ="",OFFSET(A94,-2,0)+1,OFFSET(A94,-1,0)+1 )</f>
         <v>70</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D94" s="24"/>
+        <v>392</v>
+      </c>
+      <c r="D94" s="24" t="s">
+        <v>353</v>
+      </c>
       <c r="E94" s="25"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
-      <c r="I94" s="26"/>
-    </row>
-    <row r="95" spans="1:9" s="27" customFormat="1">
+      <c r="I94" s="67"/>
+    </row>
+    <row r="95" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A95" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>71</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D95" s="24"/>
+        <v>414</v>
+      </c>
+      <c r="D95" s="24" t="s">
+        <v>294</v>
+      </c>
       <c r="E95" s="25"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
       <c r="I95" s="26"/>
     </row>
-    <row r="96" spans="1:9" s="27" customFormat="1">
+    <row r="96" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A96" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>72</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D96" s="24"/>
+        <v>316</v>
+      </c>
+      <c r="D96" s="24" t="s">
+        <v>358</v>
+      </c>
       <c r="E96" s="25"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
       <c r="I96" s="26"/>
     </row>
-    <row r="97" spans="1:9" s="27" customFormat="1">
+    <row r="97" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A97" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>73</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D97" s="24"/>
+        <v>415</v>
+      </c>
+      <c r="D97" s="24" t="s">
+        <v>294</v>
+      </c>
       <c r="E97" s="25"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
       <c r="I97" s="26"/>
     </row>
-    <row r="98" spans="1:9" s="27" customFormat="1">
+    <row r="98" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A98" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>74</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D98" s="24"/>
+        <v>393</v>
+      </c>
+      <c r="D98" s="24" t="s">
+        <v>294</v>
+      </c>
       <c r="E98" s="25"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
       <c r="I98" s="26"/>
     </row>
-    <row r="99" spans="1:9" s="27" customFormat="1">
+    <row r="99" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A99" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>75</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D99" s="24"/>
+        <v>319</v>
+      </c>
+      <c r="D99" s="24" t="s">
+        <v>358</v>
+      </c>
       <c r="E99" s="25"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
       <c r="I99" s="26"/>
     </row>
-    <row r="100" spans="1:9" s="27" customFormat="1">
+    <row r="100" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A100" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>76</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D100" s="24"/>
+        <v>320</v>
+      </c>
+      <c r="D100" s="24" t="s">
+        <v>358</v>
+      </c>
       <c r="E100" s="25"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
       <c r="I100" s="26"/>
     </row>
-    <row r="101" spans="1:9" s="27" customFormat="1">
+    <row r="101" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A101" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>77</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D101" s="24"/>
+        <v>359</v>
+      </c>
+      <c r="D101" s="24" t="s">
+        <v>358</v>
+      </c>
       <c r="E101" s="25"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
       <c r="I101" s="26"/>
     </row>
-    <row r="102" spans="1:9" s="27" customFormat="1">
+    <row r="102" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A102" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>78</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D102" s="24"/>
+        <v>357</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>360</v>
+      </c>
       <c r="E102" s="25"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
       <c r="I102" s="26"/>
     </row>
-    <row r="103" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="103" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A103" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>79</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D103" s="24"/>
+        <v>416</v>
+      </c>
+      <c r="D103" s="24" t="s">
+        <v>323</v>
+      </c>
       <c r="E103" s="25"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
-      <c r="I103" s="67"/>
-    </row>
-    <row r="104" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="I103" s="26"/>
+    </row>
+    <row r="104" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A104" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>80</v>
@@ -22233,16 +22427,18 @@
         <v>171</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D104" s="24"/>
+        <v>325</v>
+      </c>
+      <c r="D104" s="24" t="s">
+        <v>354</v>
+      </c>
       <c r="E104" s="25"/>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
       <c r="I104" s="67"/>
     </row>
-    <row r="105" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="105" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A105" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>81</v>
@@ -22251,16 +22447,18 @@
         <v>172</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D105" s="24"/>
+        <v>417</v>
+      </c>
+      <c r="D105" s="24" t="s">
+        <v>294</v>
+      </c>
       <c r="E105" s="25"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
       <c r="I105" s="67"/>
     </row>
-    <row r="106" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="106" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A106" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>82</v>
@@ -22269,16 +22467,18 @@
         <v>178</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D106" s="24"/>
+        <v>418</v>
+      </c>
+      <c r="D106" s="24" t="s">
+        <v>294</v>
+      </c>
       <c r="E106" s="25"/>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
       <c r="I106" s="67"/>
     </row>
-    <row r="107" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="107" spans="1:9" s="29" customFormat="1" ht="51">
       <c r="A107" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>83</v>
@@ -22287,16 +22487,18 @@
         <v>205</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D107" s="24"/>
+        <v>419</v>
+      </c>
+      <c r="D107" s="24" t="s">
+        <v>294</v>
+      </c>
       <c r="E107" s="25"/>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
       <c r="I107" s="67"/>
     </row>
-    <row r="108" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="108" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A108" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>84</v>
@@ -22305,379 +22507,395 @@
         <v>204</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D108" s="24"/>
+        <v>327</v>
+      </c>
+      <c r="D108" s="24" t="s">
+        <v>354</v>
+      </c>
       <c r="E108" s="25"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
       <c r="I108" s="67"/>
     </row>
-    <row r="109" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="109" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A109" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>85</v>
       </c>
-      <c r="B109" s="54" t="s">
-        <v>218</v>
+      <c r="B109" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
+        <v>331</v>
+      </c>
+      <c r="D109" s="70" t="s">
+        <v>277</v>
+      </c>
+      <c r="E109" s="25"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
       <c r="I109" s="67"/>
     </row>
-    <row r="110" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A110" s="65">
+    <row r="110" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A110" s="43"/>
+      <c r="B110" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="C110" s="61"/>
+      <c r="D110" s="62"/>
+      <c r="E110" s="63"/>
+      <c r="F110" s="64"/>
+      <c r="G110" s="64"/>
+      <c r="H110" s="64"/>
+      <c r="I110" s="63"/>
+    </row>
+    <row r="111" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A111" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>86</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D110" s="1"/>
-      <c r="E110" s="25"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-      <c r="I110" s="67"/>
-    </row>
-    <row r="111" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A111" s="43"/>
-      <c r="B111" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="C111" s="61"/>
-      <c r="D111" s="62"/>
-      <c r="E111" s="63"/>
-      <c r="F111" s="64"/>
-      <c r="G111" s="64"/>
-      <c r="H111" s="64"/>
-      <c r="I111" s="63"/>
-    </row>
-    <row r="112" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="B111" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D111" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="E111" s="25"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="67"/>
+    </row>
+    <row r="112" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A112" s="65">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="A112:A113" ca="1" si="2">IF(OFFSET(A112,-1,0) ="",OFFSET(A112,-2,0)+1,OFFSET(A112,-1,0)+1 )</f>
         <v>87</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D112" s="24"/>
+        <v>385</v>
+      </c>
+      <c r="D112" s="24" t="s">
+        <v>363</v>
+      </c>
       <c r="E112" s="25"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
       <c r="I112" s="67"/>
     </row>
-    <row r="113" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="113" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A113" s="65">
-        <f t="shared" ref="A113:A114" ca="1" si="2">IF(OFFSET(A113,-1,0) ="",OFFSET(A113,-2,0)+1,OFFSET(A113,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>88</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D113" s="24"/>
+        <v>386</v>
+      </c>
+      <c r="D113" s="24" t="s">
+        <v>362</v>
+      </c>
       <c r="E113" s="25"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
       <c r="I113" s="67"/>
     </row>
-    <row r="114" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A114" s="65">
-        <f t="shared" ca="1" si="2"/>
+    <row r="114" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A114" s="43"/>
+      <c r="B114" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C114" s="61"/>
+      <c r="D114" s="62"/>
+      <c r="E114" s="63"/>
+      <c r="F114" s="64"/>
+      <c r="G114" s="64"/>
+      <c r="H114" s="64"/>
+      <c r="I114" s="63"/>
+    </row>
+    <row r="115" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A115" s="65">
+        <f t="shared" ref="A115" ca="1" si="3">IF(OFFSET(A115,-1,0) ="",OFFSET(A115,-2,0)+1,OFFSET(A115,-1,0)+1 )</f>
         <v>89</v>
       </c>
-      <c r="B114" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D114" s="24"/>
-      <c r="E114" s="25"/>
-      <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
-      <c r="H114" s="1"/>
-      <c r="I114" s="67"/>
-    </row>
-    <row r="115" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A115" s="43"/>
-      <c r="B115" s="53" t="s">
-        <v>167</v>
-      </c>
-      <c r="C115" s="61"/>
-      <c r="D115" s="62"/>
-      <c r="E115" s="63"/>
-      <c r="F115" s="64"/>
-      <c r="G115" s="64"/>
-      <c r="H115" s="64"/>
-      <c r="I115" s="63"/>
-    </row>
-    <row r="116" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A116" s="65">
-        <f t="shared" ref="A116" ca="1" si="3">IF(OFFSET(A116,-1,0) ="",OFFSET(A116,-2,0)+1,OFFSET(A116,-1,0)+1 )</f>
+      <c r="B115" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D115" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="E115" s="25"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="67"/>
+    </row>
+    <row r="116" spans="1:9" s="29" customFormat="1" ht="38.25">
+      <c r="A116" s="71">
+        <f ca="1">IF(OFFSET(A116,-1,0) ="",OFFSET(A116,-2,0)+1,OFFSET(A116,-1,0)+1 )</f>
         <v>90</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D116" s="24"/>
+        <v>366</v>
+      </c>
+      <c r="D116" s="24" t="s">
+        <v>367</v>
+      </c>
       <c r="E116" s="25"/>
-      <c r="F116" s="1"/>
+      <c r="F116" s="25"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
-      <c r="I116" s="67"/>
-    </row>
-    <row r="117" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="I116" s="71"/>
+    </row>
+    <row r="117" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A117" s="71">
-        <f ca="1">IF(OFFSET(A117,-1,0) ="",OFFSET(A117,-2,0)+1,OFFSET(A117,-1,0)+1 )</f>
+        <f t="shared" ref="A117:A127" ca="1" si="4">IF(OFFSET(A117,-1,0) ="",OFFSET(A117,-2,0)+1,OFFSET(A117,-1,0)+1 )</f>
         <v>91</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D117" s="24"/>
+        <v>368</v>
+      </c>
+      <c r="D117" s="24" t="s">
+        <v>369</v>
+      </c>
       <c r="E117" s="25"/>
       <c r="F117" s="25"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
       <c r="I117" s="71"/>
     </row>
-    <row r="118" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A118" s="71">
-        <f t="shared" ref="A118:A128" ca="1" si="4">IF(OFFSET(A118,-1,0) ="",OFFSET(A118,-2,0)+1,OFFSET(A118,-1,0)+1 )</f>
+    <row r="118" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A118" s="68"/>
+      <c r="B118" s="90" t="s">
+        <v>211</v>
+      </c>
+      <c r="C118" s="91"/>
+      <c r="D118" s="92"/>
+      <c r="E118" s="69"/>
+      <c r="F118" s="32"/>
+      <c r="G118" s="32"/>
+      <c r="H118" s="32"/>
+      <c r="I118" s="69"/>
+    </row>
+    <row r="119" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A119" s="71">
+        <f t="shared" ca="1" si="4"/>
         <v>92</v>
       </c>
-      <c r="B118" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D118" s="24"/>
-      <c r="E118" s="25"/>
-      <c r="F118" s="25"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-      <c r="I118" s="71"/>
-    </row>
-    <row r="119" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A119" s="68"/>
-      <c r="B119" s="90" t="s">
-        <v>213</v>
-      </c>
-      <c r="C119" s="91"/>
-      <c r="D119" s="92"/>
-      <c r="E119" s="69"/>
-      <c r="F119" s="32"/>
-      <c r="G119" s="32"/>
-      <c r="H119" s="32"/>
-      <c r="I119" s="69"/>
-    </row>
-    <row r="120" spans="1:9" s="27" customFormat="1">
+      <c r="B119" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D119" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="E119" s="25"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="26"/>
+    </row>
+    <row r="120" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A120" s="71">
         <f t="shared" ca="1" si="4"/>
         <v>93</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>210</v>
+        <v>371</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D120" s="24"/>
+        <v>421</v>
+      </c>
+      <c r="D120" s="24" t="s">
+        <v>294</v>
+      </c>
       <c r="E120" s="25"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
       <c r="I120" s="26"/>
     </row>
-    <row r="121" spans="1:9" s="27" customFormat="1">
+    <row r="121" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A121" s="71">
         <f t="shared" ca="1" si="4"/>
         <v>94</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D121" s="24"/>
+        <v>422</v>
+      </c>
+      <c r="D121" s="24" t="s">
+        <v>376</v>
+      </c>
       <c r="E121" s="25"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
       <c r="I121" s="26"/>
     </row>
-    <row r="122" spans="1:9" s="27" customFormat="1">
+    <row r="122" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A122" s="71">
         <f t="shared" ca="1" si="4"/>
         <v>95</v>
       </c>
-      <c r="B122" s="1" t="s">
-        <v>211</v>
+      <c r="B122" s="54" t="s">
+        <v>161</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D122" s="24"/>
+        <v>423</v>
+      </c>
+      <c r="D122" s="24" t="s">
+        <v>377</v>
+      </c>
       <c r="E122" s="25"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
       <c r="I122" s="26"/>
     </row>
-    <row r="123" spans="1:9" s="27" customFormat="1">
+    <row r="123" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A123" s="71">
         <f t="shared" ca="1" si="4"/>
         <v>96</v>
       </c>
       <c r="B123" s="54" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D123" s="24"/>
+        <v>424</v>
+      </c>
+      <c r="D123" s="24" t="s">
+        <v>378</v>
+      </c>
       <c r="E123" s="25"/>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
       <c r="I123" s="26"/>
     </row>
-    <row r="124" spans="1:9" s="27" customFormat="1">
+    <row r="124" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A124" s="71">
         <f t="shared" ca="1" si="4"/>
         <v>97</v>
       </c>
       <c r="B124" s="54" t="s">
-        <v>162</v>
+        <v>380</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D124" s="24"/>
+        <v>425</v>
+      </c>
+      <c r="D124" s="24" t="s">
+        <v>379</v>
+      </c>
       <c r="E124" s="25"/>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
       <c r="I124" s="26"/>
     </row>
-    <row r="125" spans="1:9" s="27" customFormat="1">
+    <row r="125" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A125" s="71">
         <f t="shared" ca="1" si="4"/>
         <v>98</v>
       </c>
-      <c r="B125" s="54" t="s">
-        <v>214</v>
+      <c r="B125" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D125" s="24"/>
+        <v>305</v>
+      </c>
+      <c r="D125" s="24" t="s">
+        <v>288</v>
+      </c>
       <c r="E125" s="25"/>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
       <c r="I125" s="26"/>
     </row>
-    <row r="126" spans="1:9" s="27" customFormat="1">
+    <row r="126" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A126" s="71">
         <f t="shared" ca="1" si="4"/>
         <v>99</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D126" s="24"/>
+        <v>381</v>
+      </c>
+      <c r="D126" s="24" t="s">
+        <v>384</v>
+      </c>
       <c r="E126" s="25"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
       <c r="I126" s="26"/>
     </row>
-    <row r="127" spans="1:9" s="27" customFormat="1">
+    <row r="127" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A127" s="71">
         <f t="shared" ca="1" si="4"/>
         <v>100</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D127" s="24"/>
+        <v>372</v>
+      </c>
+      <c r="D127" s="24" t="s">
+        <v>289</v>
+      </c>
       <c r="E127" s="25"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
       <c r="I127" s="26"/>
     </row>
-    <row r="128" spans="1:9" s="27" customFormat="1">
-      <c r="A128" s="71">
-        <f t="shared" ca="1" si="4"/>
-        <v>101</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D128" s="24"/>
-      <c r="E128" s="25"/>
-      <c r="F128" s="1"/>
-      <c r="G128" s="1"/>
-      <c r="H128" s="1"/>
-      <c r="I128" s="26"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="B18:D18"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F68:H68 F18:H19 F87:H87 F111:H111 F32:H32 F45:H45 F92:H92 F115:H115"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F68:H68 F18:H19 F87:H87 F110:H110 F32:H32 F45:H45 F92:H92 F114:H114"/>
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
-    <dataValidation type="list" allowBlank="1" sqref="F112:H114 F69:H86 F116:H128 F93:H110 F33:H44 F20:H31 F46:H67 F88:H91">
+    <dataValidation type="list" allowBlank="1" sqref="F111:H113 F69:H86 F115:H127 F88:H91 F33:H44 F20:H31 F46:H67 F93:H109">
       <formula1>$A$11:$A$15</formula1>
     </dataValidation>
   </dataValidations>
@@ -22995,7 +23213,7 @@
     <row r="18" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="22"/>
       <c r="B18" s="79" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C18" s="80"/>
       <c r="D18" s="81"/>
@@ -23119,7 +23337,7 @@
     <row r="26" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A26" s="22"/>
       <c r="B26" s="79" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C26" s="80"/>
       <c r="D26" s="81"/>
@@ -23132,7 +23350,7 @@
     <row r="27" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A27" s="46"/>
       <c r="B27" s="55" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C27" s="44"/>
       <c r="D27" s="45"/>
@@ -23147,7 +23365,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="24"/>
@@ -23163,7 +23381,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="24"/>
@@ -23179,7 +23397,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="24"/>
@@ -23195,7 +23413,7 @@
         <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="24"/>
@@ -23211,7 +23429,7 @@
         <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="24"/>
@@ -23227,7 +23445,7 @@
         <v>13</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="24"/>
@@ -23243,7 +23461,7 @@
         <v>14</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="24"/>
@@ -23259,7 +23477,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="24"/>
@@ -23275,7 +23493,7 @@
         <v>16</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="24"/>
@@ -23288,7 +23506,7 @@
     <row r="37" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="46"/>
       <c r="B37" s="55" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C37" s="44"/>
       <c r="D37" s="45"/>
@@ -23304,7 +23522,7 @@
         <v>17</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="24"/>
@@ -23320,7 +23538,7 @@
         <v>18</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="24"/>
@@ -23336,7 +23554,7 @@
         <v>19</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="24"/>
@@ -23352,7 +23570,7 @@
         <v>20</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="24"/>
@@ -23368,7 +23586,7 @@
         <v>21</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="24"/>
@@ -23381,7 +23599,7 @@
     <row r="43" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A43" s="46"/>
       <c r="B43" s="55" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C43" s="44"/>
       <c r="D43" s="45"/>
@@ -23397,7 +23615,7 @@
         <v>22</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="24"/>
@@ -23413,7 +23631,7 @@
         <v>23</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="24"/>
@@ -23429,7 +23647,7 @@
         <v>24</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="24"/>
@@ -23445,7 +23663,7 @@
         <v>25</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="24"/>
@@ -23461,7 +23679,7 @@
         <v>26</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="24"/>
@@ -23474,7 +23692,7 @@
     <row r="49" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A49" s="46"/>
       <c r="B49" s="55" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C49" s="44"/>
       <c r="D49" s="45"/>
@@ -23490,11 +23708,11 @@
         <v>27</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="24" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E50" s="25"/>
       <c r="F50" s="25"/>
@@ -23508,11 +23726,11 @@
         <v>28</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="24" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E51" s="25"/>
       <c r="F51" s="1"/>
@@ -23526,11 +23744,11 @@
         <v>29</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="24" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E52" s="25"/>
       <c r="F52" s="25"/>
@@ -23544,11 +23762,11 @@
         <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="24" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E53" s="25"/>
       <c r="F53" s="1"/>
@@ -23559,7 +23777,7 @@
     <row r="54" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A54" s="46"/>
       <c r="B54" s="55" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C54" s="44"/>
       <c r="D54" s="45"/>
@@ -23572,7 +23790,7 @@
     <row r="55" spans="1:9" s="76" customFormat="1" ht="15.75" customHeight="1">
       <c r="A55" s="72"/>
       <c r="B55" s="77" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C55" s="73"/>
       <c r="D55" s="74"/>
@@ -23588,11 +23806,11 @@
         <v>31</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="24" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E56" s="25"/>
       <c r="F56" s="25"/>
@@ -23606,11 +23824,11 @@
         <v>32</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="24" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E57" s="25"/>
       <c r="F57" s="25"/>
@@ -23624,11 +23842,11 @@
         <v>33</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E58" s="25"/>
       <c r="F58" s="25"/>
@@ -23639,7 +23857,7 @@
     <row r="59" spans="1:9" s="76" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="72"/>
       <c r="B59" s="77" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C59" s="73"/>
       <c r="D59" s="74"/>
@@ -23655,11 +23873,11 @@
         <v>34</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="24" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E60" s="25"/>
       <c r="F60" s="25"/>
@@ -23673,11 +23891,11 @@
         <v>35</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="24" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E61" s="25"/>
       <c r="F61" s="1"/>
@@ -23691,11 +23909,11 @@
         <v>36</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="24" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E62" s="25"/>
       <c r="F62" s="25"/>
@@ -23709,11 +23927,11 @@
         <v>37</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="24" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E63" s="25"/>
       <c r="F63" s="1"/>
@@ -23727,11 +23945,11 @@
         <v>38</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="24" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E64" s="25"/>
       <c r="F64" s="25"/>
@@ -23745,11 +23963,11 @@
         <v>39</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E65" s="25"/>
       <c r="F65" s="25"/>
@@ -23760,7 +23978,7 @@
     <row r="66" spans="1:9" s="76" customFormat="1" ht="15.75" customHeight="1">
       <c r="A66" s="72"/>
       <c r="B66" s="77" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C66" s="73"/>
       <c r="D66" s="74"/>
@@ -23776,11 +23994,11 @@
         <v>40</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E67" s="25"/>
       <c r="F67" s="25"/>
@@ -23794,11 +24012,11 @@
         <v>41</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E68" s="25"/>
       <c r="F68" s="1"/>
@@ -23812,11 +24030,11 @@
         <v>42</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E69" s="25"/>
       <c r="F69" s="25"/>
@@ -23830,11 +24048,11 @@
         <v>43</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E70" s="25"/>
       <c r="F70" s="1"/>
@@ -23848,11 +24066,11 @@
         <v>44</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E71" s="25"/>
       <c r="F71" s="25"/>
@@ -23866,11 +24084,11 @@
         <v>45</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E72" s="25"/>
       <c r="F72" s="25"/>
@@ -23881,7 +24099,7 @@
     <row r="73" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A73" s="46"/>
       <c r="B73" s="55" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C73" s="44"/>
       <c r="D73" s="45"/>
@@ -23913,7 +24131,7 @@
         <v>47</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -23929,7 +24147,7 @@
         <v>48</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -23945,7 +24163,7 @@
         <v>49</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="24"/>
@@ -23961,7 +24179,7 @@
         <v>50</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="24"/>
@@ -23973,11 +24191,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="A1:D1"/>
@@ -23985,6 +24198,11 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:H27 F18:H18 F37:H37 F43:H43 F49:H49 F73:H73 F54:H55 F59:H59 F66:H66"/>

</xml_diff>

<commit_message>
Updated file on 30/10 - Assignment 4,5
</commit_message>
<xml_diff>
--- a/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
+++ b/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
@@ -4,101 +4,119 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 1" sheetId="3" r:id="rId1"/>
     <sheet name="Assignment 2" sheetId="4" r:id="rId2"/>
     <sheet name="Assignment 3" sheetId="6" r:id="rId3"/>
     <sheet name="Assignment 4" sheetId="7" r:id="rId4"/>
+    <sheet name="Assignment 5" sheetId="9" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignment 1'!$A$17:$X$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Assignment 2'!$A$19:$Z$128</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Assignment 3'!$A$17:$X$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Assignment 4'!$A$37:$Z$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Assignment 4'!$A$20:$I$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Assignment 5'!$A$17:$X$17</definedName>
     <definedName name="abc" localSheetId="0">#REF!</definedName>
     <definedName name="abc" localSheetId="1">#REF!</definedName>
     <definedName name="abc" localSheetId="2">#REF!</definedName>
     <definedName name="abc" localSheetId="3">#REF!</definedName>
+    <definedName name="abc" localSheetId="4">#REF!</definedName>
     <definedName name="abc">#REF!</definedName>
     <definedName name="Check_inputed_mail_address" localSheetId="0">#REF!</definedName>
     <definedName name="Check_inputed_mail_address" localSheetId="1">#REF!</definedName>
     <definedName name="Check_inputed_mail_address" localSheetId="2">#REF!</definedName>
     <definedName name="Check_inputed_mail_address" localSheetId="3">#REF!</definedName>
+    <definedName name="Check_inputed_mail_address" localSheetId="4">#REF!</definedName>
     <definedName name="Check_inputed_mail_address">#REF!</definedName>
     <definedName name="CS_IT_1.1_001" localSheetId="0">#REF!</definedName>
     <definedName name="CS_IT_1.1_001" localSheetId="1">#REF!</definedName>
     <definedName name="CS_IT_1.1_001" localSheetId="2">#REF!</definedName>
     <definedName name="CS_IT_1.1_001" localSheetId="3">#REF!</definedName>
+    <definedName name="CS_IT_1.1_001" localSheetId="4">#REF!</definedName>
     <definedName name="CS_IT_1.1_001">#REF!</definedName>
     <definedName name="CS_IT_1.1_002" localSheetId="0">#REF!</definedName>
     <definedName name="CS_IT_1.1_002" localSheetId="1">#REF!</definedName>
     <definedName name="CS_IT_1.1_002" localSheetId="2">#REF!</definedName>
     <definedName name="CS_IT_1.1_002" localSheetId="3">#REF!</definedName>
+    <definedName name="CS_IT_1.1_002" localSheetId="4">#REF!</definedName>
     <definedName name="CS_IT_1.1_002">#REF!</definedName>
     <definedName name="CS_IT_1.1_003" localSheetId="0">#REF!</definedName>
     <definedName name="CS_IT_1.1_003" localSheetId="1">#REF!</definedName>
     <definedName name="CS_IT_1.1_003" localSheetId="2">#REF!</definedName>
     <definedName name="CS_IT_1.1_003" localSheetId="3">#REF!</definedName>
+    <definedName name="CS_IT_1.1_003" localSheetId="4">#REF!</definedName>
     <definedName name="CS_IT_1.1_003">#REF!</definedName>
     <definedName name="CS_IT_1.1_004" localSheetId="0">#REF!</definedName>
     <definedName name="CS_IT_1.1_004" localSheetId="1">#REF!</definedName>
     <definedName name="CS_IT_1.1_004" localSheetId="2">#REF!</definedName>
     <definedName name="CS_IT_1.1_004" localSheetId="3">#REF!</definedName>
+    <definedName name="CS_IT_1.1_004" localSheetId="4">#REF!</definedName>
     <definedName name="CS_IT_1.1_004">#REF!</definedName>
     <definedName name="Evaluation" localSheetId="0">#REF!</definedName>
     <definedName name="Evaluation" localSheetId="1">#REF!</definedName>
     <definedName name="Evaluation" localSheetId="2">#REF!</definedName>
     <definedName name="Evaluation" localSheetId="3">#REF!</definedName>
+    <definedName name="Evaluation" localSheetId="4">#REF!</definedName>
     <definedName name="Evaluation">#REF!</definedName>
     <definedName name="JaEnNickname" localSheetId="0">#REF!</definedName>
     <definedName name="JaEnNickname" localSheetId="1">#REF!</definedName>
     <definedName name="JaEnNickname" localSheetId="2">#REF!</definedName>
     <definedName name="JaEnNickname" localSheetId="3">#REF!</definedName>
+    <definedName name="JaEnNickname" localSheetId="4">#REF!</definedName>
     <definedName name="JaEnNickname">#REF!</definedName>
     <definedName name="Mail_Magazine" localSheetId="0">#REF!</definedName>
     <definedName name="Mail_Magazine" localSheetId="1">#REF!</definedName>
     <definedName name="Mail_Magazine" localSheetId="2">#REF!</definedName>
     <definedName name="Mail_Magazine" localSheetId="3">#REF!</definedName>
+    <definedName name="Mail_Magazine" localSheetId="4">#REF!</definedName>
     <definedName name="Mail_Magazine">#REF!</definedName>
     <definedName name="project_code" localSheetId="0">#REF!</definedName>
     <definedName name="project_code" localSheetId="1">#REF!</definedName>
     <definedName name="project_code" localSheetId="2">#REF!</definedName>
     <definedName name="project_code" localSheetId="3">#REF!</definedName>
+    <definedName name="project_code" localSheetId="4">#REF!</definedName>
     <definedName name="project_code">#REF!</definedName>
     <definedName name="ProjectName" localSheetId="0">'[1]Version 1'!#REF!</definedName>
     <definedName name="ProjectName" localSheetId="1">'[1]Version 1'!#REF!</definedName>
     <definedName name="ProjectName" localSheetId="2">'[1]Version 1'!#REF!</definedName>
     <definedName name="ProjectName" localSheetId="3">'[1]Version 1'!#REF!</definedName>
+    <definedName name="ProjectName" localSheetId="4">'[1]Version 1'!#REF!</definedName>
     <definedName name="ProjectName">'[1]Version 1'!#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_001" localSheetId="0">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_001" localSheetId="1">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_001" localSheetId="2">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_001" localSheetId="3">#REF!</definedName>
+    <definedName name="Result_CS_IT_1.1_001" localSheetId="4">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_001">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_002" localSheetId="0">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_002" localSheetId="1">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_002" localSheetId="2">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_002" localSheetId="3">#REF!</definedName>
+    <definedName name="Result_CS_IT_1.1_002" localSheetId="4">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_002">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_003" localSheetId="0">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_003" localSheetId="1">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_003" localSheetId="2">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_003" localSheetId="3">#REF!</definedName>
+    <definedName name="Result_CS_IT_1.1_003" localSheetId="4">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_003">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_004" localSheetId="0">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_004" localSheetId="1">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_004" localSheetId="2">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_004" localSheetId="3">#REF!</definedName>
+    <definedName name="Result_CS_IT_1.1_004" localSheetId="4">#REF!</definedName>
     <definedName name="Result_CS_IT_1.1_004">#REF!</definedName>
     <definedName name="safa" localSheetId="0">#REF!</definedName>
     <definedName name="safa" localSheetId="1">#REF!</definedName>
     <definedName name="safa" localSheetId="2">#REF!</definedName>
     <definedName name="safa" localSheetId="3">#REF!</definedName>
+    <definedName name="safa" localSheetId="4">#REF!</definedName>
     <definedName name="safa">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
@@ -463,8 +481,72 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="F17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pass
+Fail
+Untested
+N/A
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pass
+Fail
+Untested
+N/A
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pass
+Fail
+Untested
+N/A
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="652">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -2292,9 +2374,6 @@
     <t>When the user selects a Ward</t>
   </si>
   <si>
-    <t xml:space="preserve">Check default status </t>
-  </si>
-  <si>
     <t>When Home is in default status</t>
   </si>
   <si>
@@ -2319,9 +2398,6 @@
     <t>Check Office button</t>
   </si>
   <si>
-    <t>New address can be added successfully when all fields are entered valid values</t>
-  </si>
-  <si>
     <t>Add address fail when all fields are entered invalid value</t>
   </si>
   <si>
@@ -2334,7 +2410,537 @@
     <t>Add address fail when the user clicks on the Cancel button</t>
   </si>
   <si>
+    <t>Check default value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special characters:
+- html
+- javascript
+- SQL injection </t>
+  </si>
+  <si>
+    <t>Check mandatory</t>
+  </si>
+  <si>
+    <t>New address as home can be added successfully when all fields are entered valid values</t>
+  </si>
+  <si>
+    <t>New address as office can be added successfully when all fields are entered valid values</t>
+  </si>
+  <si>
     <t>New address can be added successfully when all mandatory fields are entered valid values</t>
+  </si>
+  <si>
+    <t>Open Add New Address screen</t>
+  </si>
+  <si>
+    <t>1. Observe the display of the Full Name</t>
+  </si>
+  <si>
+    <t>1. Don't enter value 
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>Full Name is blank 
+The placeholder is "First Last"</t>
+  </si>
+  <si>
+    <t>1. Enter "Nguyen Thi Van Anh"
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>System will show error message "Please enter your Full name"</t>
+  </si>
+  <si>
+    <t>1. Enter "^&amp;*"
+2. Click on Close (x) button
+3. Enter HTML code: &lt;!DOCTYPE html&gt;&lt;html&gt;&lt;body&gt;&lt;h1&gt;Học lập trình HTML&lt;/h1&gt;&lt;/body&gt;&lt;/html&gt;
+4. Click on Close (x) button
+5. Enter javascript: &lt;script src="myScript.js"&gt;&lt;/script&gt;
+6. Click on Close (x) button
+7. Enter SQL injection: SELECT * FROM Users WHERE Username = 'Vanh' AND Password = '12345678'</t>
+  </si>
+  <si>
+    <t>System will show error message "Name should not contain special characters"</t>
+  </si>
+  <si>
+    <t>1. Enter "12345678"
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter "Vanh1234"
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter "123$%^"</t>
+  </si>
+  <si>
+    <t>1. Enter "Vanh$%^"</t>
+  </si>
+  <si>
+    <t>1. Enter "Vanh1234%^&amp;"</t>
+  </si>
+  <si>
+    <t>Allow Copy/Paste Full Name</t>
+  </si>
+  <si>
+    <t>1. Enter " Nguyen Thi Van Anh "
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>'System will show error message "The name length should be 2-50 characters"</t>
+  </si>
+  <si>
+    <t>1. Enter 2 characters (valid Full Name)
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 3 characters (valid Full Name)
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 50 characters (valid Full Name)
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Observe the display of the Phone Number</t>
+  </si>
+  <si>
+    <t>System will show error message "The name length should be 2-50 characters"</t>
+  </si>
+  <si>
+    <t>System will show error message "Please enter your Phone number"</t>
+  </si>
+  <si>
+    <t>Phone Number is blank 
+The placeholder is "Please enter your Phone number"</t>
+  </si>
+  <si>
+    <t>1. Enter any character
+2. Click on close (x) button</t>
+  </si>
+  <si>
+    <t>1. Enter "^&amp;*"
+2. Enter HTML code: &lt;!DOCTYPE html&gt;&lt;html&gt;&lt;body&gt;&lt;h1&gt;Học lập trình HTML&lt;/h1&gt;&lt;/body&gt;&lt;/html&gt;
+3. Enter javascript: &lt;script src="myScript.js"&gt;&lt;/script&gt;
+4. Enter SQL injection: SELECT * FROM Users WHERE Username = 'Vanh' AND Password = '12345678'</t>
+  </si>
+  <si>
+    <t>1. Enter "0981980721"
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter " 0981 980 721 "</t>
+  </si>
+  <si>
+    <t>System will show error message "The length of phone number should be 10 characters"</t>
+  </si>
+  <si>
+    <t>1. Enter "123"</t>
+  </si>
+  <si>
+    <t>1. Enter "09819807211"</t>
+  </si>
+  <si>
+    <t>1. Enter "Nguyen Thi Van Anh"</t>
+  </si>
+  <si>
+    <t>1. Enter "0981980721"</t>
+  </si>
+  <si>
+    <t>1. Observe the display of the Address</t>
+  </si>
+  <si>
+    <t>System will show error message "Please enter your Address"</t>
+  </si>
+  <si>
+    <t>Allow Copy/Paste Address</t>
+  </si>
+  <si>
+    <t>Address is blank 
+The placeholder is "Please enter your Address"</t>
+  </si>
+  <si>
+    <t>1. Enter "Đường Láng"
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>System will show error message "The Address should not contain special characters"</t>
+  </si>
+  <si>
+    <t>1. Enter " Đường Láng "
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>'System will show error message "The Address length should be 5-350 characters"</t>
+  </si>
+  <si>
+    <t>System will show error message "The Address length should be 5-350 characters"</t>
+  </si>
+  <si>
+    <t>1. Enter 5 characters (valid Address)
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 6 characters (valid Address)
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 350 characters (valid Address)
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 4 characters</t>
+  </si>
+  <si>
+    <t>1. Enter 351 characters</t>
+  </si>
+  <si>
+    <t>1. Enter 1 character</t>
+  </si>
+  <si>
+    <t>1. Enter 51 characters</t>
+  </si>
+  <si>
+    <t>System will show error message "Please select your Province"</t>
+  </si>
+  <si>
+    <t>Province is blank
+The placeholder is "Please choose your Province"</t>
+  </si>
+  <si>
+    <t>Sorting trong lazada trình bày khó</t>
+  </si>
+  <si>
+    <t>There is a scrollbar when the list of Province exceeds the display frame</t>
+  </si>
+  <si>
+    <t>There are 63 provinces of VN</t>
+  </si>
+  <si>
+    <t>Do not allow paste, allow copy Province</t>
+  </si>
+  <si>
+    <t>1. Click on Province</t>
+  </si>
+  <si>
+    <t>1. Click on Province
+2. Observe the display of dropdown list</t>
+  </si>
+  <si>
+    <t>1. Click on District</t>
+  </si>
+  <si>
+    <t>1. Don't select value
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Click on Province
+2. Select a Province
+3. Enter other fields are valid
+4. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>Check Copy/Paste Province</t>
+  </si>
+  <si>
+    <t>Check Copy/Paste Ward</t>
+  </si>
+  <si>
+    <t>Check Copy/Paste District</t>
+  </si>
+  <si>
+    <t>1. Paste value
+2. Click on Province
+2. Select a Province
+3. Copy value
+4. Paste into other text fields</t>
+  </si>
+  <si>
+    <t>1. Enter character</t>
+  </si>
+  <si>
+    <t>1. Observe the display of the Province</t>
+  </si>
+  <si>
+    <t>1. Observe the display of the District</t>
+  </si>
+  <si>
+    <t>1. Select a Province
+2. Observe the display of the District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">District is blank and disable
+The placeholder is "Please choose your District"
+</t>
+  </si>
+  <si>
+    <t>District is enable</t>
+  </si>
+  <si>
+    <t>There is a scrollbar when the list of District exceeds the display frame</t>
+  </si>
+  <si>
+    <t>System will show error message "Please select your District"</t>
+  </si>
+  <si>
+    <t>1. Click on District
+2. Select a District
+3. Enter other fields are valid
+4. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>Do not allow paste, allow copy District</t>
+  </si>
+  <si>
+    <t>1. Paste value
+2. Click on District
+2. Select a District
+3. Copy value
+4. Paste into other text fields</t>
+  </si>
+  <si>
+    <t>1. Click on District
+2. Observe the display of dropdown list</t>
+  </si>
+  <si>
+    <t>1.Copy/Paste "abc123$%^"</t>
+  </si>
+  <si>
+    <t>Allow Copy/Paste only numeric characters</t>
+  </si>
+  <si>
+    <t>1. Observe the display of the Ward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ward is blank and disable
+The placeholder is "Please choose your Ward"
+</t>
+  </si>
+  <si>
+    <t>Ward is enable</t>
+  </si>
+  <si>
+    <t>1. Click on Ward
+2. Observe the display of dropdown list</t>
+  </si>
+  <si>
+    <t>1. Click on Ward</t>
+  </si>
+  <si>
+    <t>There is a scrollbar when the list of Ward exceeds the display frame</t>
+  </si>
+  <si>
+    <t>System will show error message "Please select your Ward"</t>
+  </si>
+  <si>
+    <t>1. Click on Ward
+2. Select a Ward
+3. Enter other fields are valid
+4. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Paste value
+2. Click on Ward
+2. Select a Ward
+3. Copy value
+4. Paste into other text fields</t>
+  </si>
+  <si>
+    <t>Do not allow paste, allow copy Ward</t>
+  </si>
+  <si>
+    <t>1. Select a District
+2. Observe the display of the Ward</t>
+  </si>
+  <si>
+    <t>Value of Dropdown will be depended on Province value and sorted alphabetically</t>
+  </si>
+  <si>
+    <t>Value of Dropdown will be depended on District value and sorted alphabetically</t>
+  </si>
+  <si>
+    <t>1. Observe the display of the Home button</t>
+  </si>
+  <si>
+    <t>Home button is enable and unchecked</t>
+  </si>
+  <si>
+    <t>Icon on Home button is gray</t>
+  </si>
+  <si>
+    <t>1. Don’t click on Home button
+2. Observe the display of the Home button</t>
+  </si>
+  <si>
+    <t>1. Click on Home button
+2. Observe the display of Home button</t>
+  </si>
+  <si>
+    <t>Icon on Home button is hightlighted</t>
+  </si>
+  <si>
+    <t>1. Observe the display of the Office button</t>
+  </si>
+  <si>
+    <t>Office button is enable and unchecked</t>
+  </si>
+  <si>
+    <t>1. Don’t click on Office button
+2. Observe the display of the Office button</t>
+  </si>
+  <si>
+    <t>Icon on Office button is gray</t>
+  </si>
+  <si>
+    <t>1. Click on Office button
+2. Observe the display of Office button</t>
+  </si>
+  <si>
+    <t>Icon on Office button is hightlighted</t>
+  </si>
+  <si>
+    <t>1. Enter all fields are valid
+2. Select Home button
+3. Click on Save button</t>
+  </si>
+  <si>
+    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book</t>
+  </si>
+  <si>
+    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book, automatic delete all leading, trailing spaces from Full Name</t>
+  </si>
+  <si>
+    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book, automatic delete all leading, trailing spaces from Address</t>
+  </si>
+  <si>
+    <t>Add new address as home successfully, return to Address book screen, new address will be displayed on the top of Address Book</t>
+  </si>
+  <si>
+    <t>Add new address as office successfully, return to Address book screen, new address will be displayed on the top of Address Book</t>
+  </si>
+  <si>
+    <t>1. Enter all fields are valid
+2. Select Office button
+3. Click on Save button</t>
+  </si>
+  <si>
+    <t>1. Enter all mandatory fields are valid
+2. Don't Select Office button/Home button
+3. Click on Save button</t>
+  </si>
+  <si>
+    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book
+Two button: Home and Office are displayed at the created address</t>
+  </si>
+  <si>
+    <t>1. Enter all fields are invalid
+2. Click on Save button</t>
+  </si>
+  <si>
+    <t>Add address fail, the system will display the corresponding error message below each field</t>
+  </si>
+  <si>
+    <t>1. Enter value into fields
+2. Click on Cancel button</t>
+  </si>
+  <si>
+    <t>Precondition: The user added 1 address
+1. Enter the value of all fields same previous address
+2. Click on Save button</t>
+  </si>
+  <si>
+    <t>Add address fail, return to Address book screen</t>
+  </si>
+  <si>
+    <t>When the user adds duplicate addresses</t>
+  </si>
+  <si>
+    <t>Precondition: The user added 1 address
+1. Enter Full Name and Phone number are same Previous address
+2. Enter other fields are different
+2. Click on Save button</t>
+  </si>
+  <si>
+    <t>When the user adds a new address completely different from the previous one</t>
+  </si>
+  <si>
+    <t>When the user adds a new address with the same consignee as the previous address</t>
+  </si>
+  <si>
+    <t>Precondition: The user added 1 address
+1. Enter the value of all fields are different previous address
+2. Click on Save button</t>
+  </si>
+  <si>
+    <t>1. Check Delete Address function</t>
+  </si>
+  <si>
+    <t>Verify that a confirmation pop-up is displayed when the user click on Delete icon</t>
+  </si>
+  <si>
+    <t>Delete address successfully when the user click on Delete button on pop-up</t>
+  </si>
+  <si>
+    <t>Delete address fail when the user click on Cancel button on pop-up</t>
+  </si>
+  <si>
+    <t>Verify that the user cannot delete default address</t>
+  </si>
+  <si>
+    <t>Show error message "You cannot delete your default address"</t>
+  </si>
+  <si>
+    <t>Delete address successfully, this address is not displayed in Address Book anymore</t>
+  </si>
+  <si>
+    <t>1. Select an address
+1. Click on Delete icon</t>
+  </si>
+  <si>
+    <t>1. Select an address that is not default address
+2. Click on Delete icon
+3. Click on Delete button on pop-up</t>
+  </si>
+  <si>
+    <t>1. Select an address
+2. Click on Delete icon
+3. Click on Delete button on pop-up</t>
+  </si>
+  <si>
+    <t>1. Select default address
+2. Click on Delete icon
+3. Click on Delete button on pop-up</t>
+  </si>
+  <si>
+    <t>1. Select an address
+2. Click on Delete icon
+3. Click on Cancel button on pop-up</t>
+  </si>
+  <si>
+    <t>Delete address fail, return to the Edit address screen</t>
+  </si>
+  <si>
+    <t>Delete address fail when the user click on Close (x) icon on pop-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A confirmation pop-up is displayed
+This pop up shows selected address information correctly </t>
   </si>
 </sst>
 </file>
@@ -2841,7 +3447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3291,6 +3897,33 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3601,7 +4234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD61"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
@@ -21137,8 +21770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121:XFD121"/>
+    <sheetView showGridLines="0" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -23141,8 +23774,8 @@
       <c r="C103" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="D103" s="24" t="s">
-        <v>364</v>
+      <c r="D103" s="107" t="s">
+        <v>529</v>
       </c>
       <c r="E103" s="84"/>
       <c r="F103" s="1"/>
@@ -26299,8 +26932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X983"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -30224,18 +30857,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I976"/>
+  <dimension ref="A1:I982"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView showGridLines="0" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111:C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="36" customWidth="1"/>
     <col min="2" max="2" width="61.42578125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" style="37" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" style="37" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" style="175" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" style="37" customWidth="1"/>
     <col min="5" max="5" width="32.140625" style="147" customWidth="1"/>
     <col min="6" max="6" width="13" style="37" customWidth="1"/>
     <col min="7" max="8" width="9.7109375" style="37" customWidth="1"/>
@@ -30309,7 +30942,9 @@
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="157"/>
+      <c r="B6" s="157" t="s">
+        <v>516</v>
+      </c>
       <c r="C6" s="158"/>
       <c r="D6" s="158"/>
       <c r="E6" s="77"/>
@@ -30354,7 +30989,7 @@
         <f>F17</f>
         <v>Internal Build 03112011</v>
       </c>
-      <c r="C9" s="13" t="str">
+      <c r="C9" s="167" t="str">
         <f>G17</f>
         <v>Internal build 14112011</v>
       </c>
@@ -30376,7 +31011,7 @@
         <f>SUM(B11:B14)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="170">
         <f>SUM(C11:C14)</f>
         <v>0</v>
       </c>
@@ -30395,15 +31030,15 @@
         <v>13</v>
       </c>
       <c r="B11" s="15">
-        <f>COUNTIF($F$18:$F$103,"*Passed")</f>
+        <f>COUNTIF($F$18:$F$107,"*Passed")</f>
         <v>0</v>
       </c>
-      <c r="C11" s="15">
-        <f>COUNTIF($G$18:$G$103,"*Passed")</f>
+      <c r="C11" s="171">
+        <f>COUNTIF($G$18:$G$107,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="D11" s="15">
-        <f>COUNTIF($H$18:$H$103,"*Passed")</f>
+        <f>COUNTIF($H$18:$H$107,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="E11" s="78"/>
@@ -30417,15 +31052,15 @@
         <v>14</v>
       </c>
       <c r="B12" s="15">
-        <f>COUNTIF($F$18:$F$103,"*Failed*")</f>
+        <f>COUNTIF($F$18:$F$107,"*Failed*")</f>
         <v>0</v>
       </c>
-      <c r="C12" s="15">
-        <f>COUNTIF($G$18:$G$103,"*Failed*")</f>
+      <c r="C12" s="171">
+        <f>COUNTIF($G$18:$G$107,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="D12" s="15">
-        <f>COUNTIF($H$18:$H$103,"*Failed*")</f>
+        <f>COUNTIF($H$18:$H$107,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="E12" s="78"/>
@@ -30439,15 +31074,15 @@
         <v>15</v>
       </c>
       <c r="B13" s="15">
-        <f>COUNTIF($F$18:$F$103,"*Not Run*")</f>
+        <f>COUNTIF($F$18:$F$107,"*Not Run*")</f>
         <v>0</v>
       </c>
-      <c r="C13" s="15">
-        <f>COUNTIF($G$18:$G$103,"*Not Run*")</f>
+      <c r="C13" s="171">
+        <f>COUNTIF($G$18:$G$107,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="D13" s="15">
-        <f>COUNTIF($H$18:$H$103,"*Not Run*")</f>
+        <f>COUNTIF($H$18:$H$107,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="E13" s="79"/>
@@ -30461,15 +31096,15 @@
         <v>16</v>
       </c>
       <c r="B14" s="15">
-        <f>COUNTIF($F$18:$F$103,"*NA*")</f>
+        <f>COUNTIF($F$18:$F$107,"*NA*")</f>
         <v>0</v>
       </c>
-      <c r="C14" s="15">
-        <f>COUNTIF($G$18:$G$103,"*NA*")</f>
+      <c r="C14" s="171">
+        <f>COUNTIF($G$18:$G$107,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="D14" s="15">
-        <f>COUNTIF($H$18:$H$103,"*NA*")</f>
+        <f>COUNTIF($H$18:$H$107,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="E14" s="79"/>
@@ -30483,15 +31118,15 @@
         <v>17</v>
       </c>
       <c r="B15" s="15">
-        <f>COUNTIF($F$18:$F$103,"*Passed in previous build*")</f>
+        <f>COUNTIF($F$18:$F$107,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
-      <c r="C15" s="15">
-        <f>COUNTIF($G$18:$G$103,"*Passed in previous build*")</f>
+      <c r="C15" s="171">
+        <f>COUNTIF($G$18:$G$107,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="D15" s="15">
-        <f>COUNTIF($H$18:$H$103,"*Passed in previous build*")</f>
+        <f>COUNTIF($H$18:$H$107,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="E15" s="79"/>
@@ -30503,7 +31138,7 @@
     <row r="16" spans="1:9" s="21" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="57"/>
       <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
+      <c r="C16" s="172"/>
       <c r="D16" s="18"/>
       <c r="E16" s="80"/>
       <c r="F16" s="148" t="s">
@@ -30520,7 +31155,7 @@
       <c r="B17" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="168" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="42" t="s">
@@ -30560,7 +31195,7 @@
       <c r="B19" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="C19" s="61"/>
+      <c r="C19" s="169"/>
       <c r="D19" s="62"/>
       <c r="E19" s="83"/>
       <c r="F19" s="64"/>
@@ -30568,160 +31203,202 @@
       <c r="H19" s="64"/>
       <c r="I19" s="63"/>
     </row>
-    <row r="20" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="20" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A20" s="65">
-        <f t="shared" ref="A20:A35" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
+        <f t="shared" ref="A20:A36" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="24"/>
+        <v>510</v>
+      </c>
+      <c r="C20" s="173" t="s">
+        <v>517</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>519</v>
+      </c>
       <c r="E20" s="84"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="26"/>
     </row>
-    <row r="21" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="21" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A21" s="65">
-        <f ca="1">IF(OFFSET(A21,-1,0) ="",OFFSET(A21,-2,0)+1,OFFSET(A21,-1,0)+1 )</f>
+        <f t="shared" ref="A21:A31" ca="1" si="1">IF(OFFSET(A21,-1,0) ="",OFFSET(A21,-2,0)+1,OFFSET(A21,-1,0)+1 )</f>
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="24"/>
+        <v>512</v>
+      </c>
+      <c r="C21" s="173" t="s">
+        <v>518</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>521</v>
+      </c>
       <c r="E21" s="84"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="67"/>
     </row>
-    <row r="22" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="22" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A22" s="65">
         <f ca="1">IF(OFFSET(A22,-1,0) ="",OFFSET(A22,-2,0)+1,OFFSET(A22,-1,0)+1 )</f>
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="24"/>
+        <v>160</v>
+      </c>
+      <c r="C22" s="173" t="s">
+        <v>539</v>
+      </c>
+      <c r="D22" s="70" t="s">
+        <v>253</v>
+      </c>
       <c r="E22" s="84"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="26"/>
-    </row>
-    <row r="23" spans="1:9" s="27" customFormat="1" ht="12.75">
+      <c r="I22" s="67"/>
+    </row>
+    <row r="23" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A23" s="65">
-        <f ca="1">IF(OFFSET(A23,-1,0) ="",OFFSET(A23,-2,0)+1,OFFSET(A23,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="24"/>
+        <v>201</v>
+      </c>
+      <c r="C23" s="173" t="s">
+        <v>520</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E23" s="84"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="26"/>
     </row>
-    <row r="24" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="24" spans="1:9" s="27" customFormat="1" ht="127.5">
       <c r="A24" s="65">
-        <f ca="1">IF(OFFSET(A24,-1,0) ="",OFFSET(A24,-2,0)+1,OFFSET(A24,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="84"/>
+        <v>202</v>
+      </c>
+      <c r="C24" s="173" t="s">
+        <v>522</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>523</v>
+      </c>
+      <c r="E24" s="84" t="s">
+        <v>511</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="26"/>
     </row>
-    <row r="25" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="25" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A25" s="65">
-        <f ca="1">IF(OFFSET(A25,-1,0) ="",OFFSET(A25,-2,0)+1,OFFSET(A25,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="24"/>
+        <v>203</v>
+      </c>
+      <c r="C25" s="173" t="s">
+        <v>524</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E25" s="84"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="26"/>
     </row>
-    <row r="26" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="26" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A26" s="65">
-        <f ca="1">IF(OFFSET(A26,-1,0) ="",OFFSET(A26,-2,0)+1,OFFSET(A26,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="24"/>
+        <v>174</v>
+      </c>
+      <c r="C26" s="173" t="s">
+        <v>525</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E26" s="84"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="26"/>
     </row>
-    <row r="27" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="27" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A27" s="65">
-        <f ca="1">IF(OFFSET(A27,-1,0) ="",OFFSET(A27,-2,0)+1,OFFSET(A27,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="24"/>
+        <v>175</v>
+      </c>
+      <c r="C27" s="173" t="s">
+        <v>526</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>523</v>
+      </c>
       <c r="E27" s="84"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="26"/>
     </row>
-    <row r="28" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="28" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A28" s="65">
-        <f ca="1">IF(OFFSET(A28,-1,0) ="",OFFSET(A28,-2,0)+1,OFFSET(A28,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="24"/>
+        <v>176</v>
+      </c>
+      <c r="C28" s="173" t="s">
+        <v>527</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>523</v>
+      </c>
       <c r="E28" s="84"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="26"/>
     </row>
-    <row r="29" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="29" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A29" s="65">
-        <f ca="1">IF(OFFSET(A29,-1,0) ="",OFFSET(A29,-2,0)+1,OFFSET(A29,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="24"/>
+        <v>177</v>
+      </c>
+      <c r="C29" s="173" t="s">
+        <v>528</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>523</v>
+      </c>
       <c r="E29" s="84"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -30730,110 +31407,138 @@
     </row>
     <row r="30" spans="1:9" s="27" customFormat="1" ht="12.75">
       <c r="A30" s="65">
-        <f ca="1">IF(OFFSET(A30,-1,0) ="",OFFSET(A30,-2,0)+1,OFFSET(A30,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="24"/>
+        <v>208</v>
+      </c>
+      <c r="C30" s="173" t="s">
+        <v>591</v>
+      </c>
+      <c r="D30" s="107" t="s">
+        <v>529</v>
+      </c>
       <c r="E30" s="84"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="26"/>
     </row>
-    <row r="31" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="31" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A31" s="65">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="24"/>
+        <v>169</v>
+      </c>
+      <c r="C31" s="173" t="s">
+        <v>530</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>620</v>
+      </c>
       <c r="E31" s="84"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="67"/>
-    </row>
-    <row r="32" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="I31" s="26"/>
+    </row>
+    <row r="32" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A32" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="24"/>
+        <v>482</v>
+      </c>
+      <c r="C32" s="173" t="s">
+        <v>562</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>531</v>
+      </c>
       <c r="E32" s="84"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="67"/>
     </row>
-    <row r="33" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="33" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A33" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="24"/>
+        <v>483</v>
+      </c>
+      <c r="C33" s="173" t="s">
+        <v>532</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E33" s="84"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="67"/>
     </row>
-    <row r="34" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="34" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A34" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="24"/>
+        <v>484</v>
+      </c>
+      <c r="C34" s="173" t="s">
+        <v>533</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E34" s="84"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="67"/>
     </row>
-    <row r="35" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="35" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A35" s="65">
         <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="24"/>
+        <v>205</v>
+      </c>
+      <c r="C35" s="173" t="s">
+        <v>534</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E35" s="84"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="67"/>
     </row>
-    <row r="36" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="36" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A36" s="65">
-        <f ca="1">IF(OFFSET(A36,-1,0) ="",OFFSET(A36,-2,0)+1,OFFSET(A36,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="70"/>
+        <v>204</v>
+      </c>
+      <c r="C36" s="173" t="s">
+        <v>563</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>536</v>
+      </c>
       <c r="E36" s="84"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -30845,7 +31550,7 @@
       <c r="B37" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="C37" s="61"/>
+      <c r="C37" s="169"/>
       <c r="D37" s="62"/>
       <c r="E37" s="83"/>
       <c r="F37" s="64"/>
@@ -30853,349 +31558,437 @@
       <c r="H37" s="64"/>
       <c r="I37" s="63"/>
     </row>
-    <row r="38" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="38" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A38" s="65">
-        <f t="shared" ref="A38:A90" ca="1" si="1">IF(OFFSET(A38,-1,0) ="",OFFSET(A38,-2,0)+1,OFFSET(A38,-1,0)+1 )</f>
+        <f t="shared" ref="A38:A92" ca="1" si="2">IF(OFFSET(A38,-1,0) ="",OFFSET(A38,-2,0)+1,OFFSET(A38,-1,0)+1 )</f>
         <v>18</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="24"/>
+        <v>510</v>
+      </c>
+      <c r="C38" s="173" t="s">
+        <v>535</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>538</v>
+      </c>
       <c r="E38" s="84"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="26"/>
     </row>
-    <row r="39" spans="1:9" s="105" customFormat="1" ht="14.25">
+    <row r="39" spans="1:9" s="105" customFormat="1" ht="38.25">
       <c r="A39" s="100">
         <f ca="1">IF(OFFSET(A39,-1,0) ="",OFFSET(A39,-2,0)+1,OFFSET(A39,-1,0)+1 )</f>
         <v>19</v>
       </c>
-      <c r="B39" s="101" t="s">
-        <v>166</v>
-      </c>
-      <c r="C39" s="101"/>
-      <c r="D39" s="102"/>
+      <c r="B39" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C39" s="173" t="s">
+        <v>518</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>537</v>
+      </c>
       <c r="E39" s="107"/>
       <c r="F39" s="107"/>
       <c r="G39" s="101"/>
       <c r="H39" s="101"/>
       <c r="I39" s="104"/>
     </row>
-    <row r="40" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="40" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A40" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">IF(OFFSET(A40,-1,0) ="",OFFSET(A40,-2,0)+1,OFFSET(A40,-1,0)+1 )</f>
         <v>20</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="84"/>
+      <c r="B40" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" s="173" t="s">
+        <v>539</v>
+      </c>
+      <c r="D40" s="70" t="s">
+        <v>253</v>
+      </c>
+      <c r="E40" s="85"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="26"/>
+      <c r="I40" s="67"/>
     </row>
     <row r="41" spans="1:9" s="27" customFormat="1" ht="12.75">
       <c r="A41" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>21</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="24"/>
+        <v>163</v>
+      </c>
+      <c r="C41" s="173" t="s">
+        <v>546</v>
+      </c>
+      <c r="D41" s="103" t="s">
+        <v>259</v>
+      </c>
       <c r="E41" s="84"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="26"/>
     </row>
-    <row r="42" spans="1:9" s="110" customFormat="1" ht="12.75">
-      <c r="A42" s="100">
-        <f t="shared" ca="1" si="1"/>
+    <row r="42" spans="1:9" s="27" customFormat="1" ht="89.25">
+      <c r="A42" s="65">
+        <f t="shared" ca="1" si="2"/>
         <v>22</v>
       </c>
-      <c r="B42" s="101" t="s">
+      <c r="B42" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" s="173" t="s">
+        <v>540</v>
+      </c>
+      <c r="D42" s="96" t="s">
+        <v>260</v>
+      </c>
+      <c r="E42" s="84" t="s">
+        <v>511</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="26"/>
+    </row>
+    <row r="43" spans="1:9" s="110" customFormat="1" ht="12.75">
+      <c r="A43" s="100">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="B43" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="C42" s="101"/>
-      <c r="D42" s="107"/>
-      <c r="E42" s="107"/>
-      <c r="F42" s="107"/>
-      <c r="G42" s="101"/>
-      <c r="H42" s="101"/>
-      <c r="I42" s="109"/>
-    </row>
-    <row r="43" spans="1:9" s="27" customFormat="1" ht="12.75">
-      <c r="A43" s="65">
-        <f t="shared" ca="1" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="173" t="s">
+        <v>547</v>
+      </c>
+      <c r="D43" s="107" t="s">
+        <v>364</v>
+      </c>
+      <c r="E43" s="107"/>
+      <c r="F43" s="107"/>
+      <c r="G43" s="101"/>
+      <c r="H43" s="101"/>
+      <c r="I43" s="109"/>
+    </row>
+    <row r="44" spans="1:9" s="27" customFormat="1" ht="12.75">
+      <c r="A44" s="65">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="107"/>
-      <c r="E43" s="85"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="26"/>
-    </row>
-    <row r="44" spans="1:9" s="118" customFormat="1" ht="12.75">
-      <c r="A44" s="114">
-        <f t="shared" ca="1" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B44" s="115" t="s">
+      <c r="C44" s="173" t="s">
+        <v>591</v>
+      </c>
+      <c r="D44" s="107" t="s">
+        <v>592</v>
+      </c>
+      <c r="E44" s="85"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="26"/>
+    </row>
+    <row r="45" spans="1:9" s="118" customFormat="1" ht="12.75">
+      <c r="A45" s="114">
+        <f t="shared" ca="1" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="B45" s="115" t="s">
         <v>169</v>
       </c>
-      <c r="C44" s="115"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="116"/>
-      <c r="F44" s="116"/>
-      <c r="G44" s="115"/>
-      <c r="H44" s="115"/>
-      <c r="I44" s="117"/>
-    </row>
-    <row r="45" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A45" s="65">
-        <f t="shared" ca="1" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="174" t="s">
+        <v>542</v>
+      </c>
+      <c r="D45" s="103" t="s">
+        <v>265</v>
+      </c>
+      <c r="E45" s="116"/>
+      <c r="F45" s="116"/>
+      <c r="G45" s="115"/>
+      <c r="H45" s="115"/>
+      <c r="I45" s="117"/>
+    </row>
+    <row r="46" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A46" s="65">
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="85"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="67"/>
-    </row>
-    <row r="46" spans="1:9" s="105" customFormat="1" ht="14.25">
-      <c r="A46" s="100">
-        <f t="shared" ca="1" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="B46" s="101" t="s">
+      <c r="C46" s="173" t="s">
+        <v>544</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>543</v>
+      </c>
+      <c r="E46" s="85"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="67"/>
+    </row>
+    <row r="47" spans="1:9" s="105" customFormat="1" ht="38.25">
+      <c r="A47" s="100">
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="B47" s="101" t="s">
         <v>485</v>
       </c>
-      <c r="C46" s="101"/>
-      <c r="D46" s="102"/>
-      <c r="E46" s="103"/>
-      <c r="F46" s="101"/>
-      <c r="G46" s="101"/>
-      <c r="H46" s="101"/>
-      <c r="I46" s="104"/>
-    </row>
-    <row r="47" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A47" s="65">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="173" t="s">
+        <v>541</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="E47" s="103"/>
+      <c r="F47" s="101"/>
+      <c r="G47" s="101"/>
+      <c r="H47" s="101"/>
+      <c r="I47" s="104"/>
+    </row>
+    <row r="48" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A48" s="65">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="85"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="67"/>
-    </row>
-    <row r="48" spans="1:9" s="105" customFormat="1" ht="14.25">
-      <c r="A48" s="100">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="B48" s="101" t="s">
-        <v>200</v>
-      </c>
-      <c r="C48" s="101"/>
-      <c r="D48" s="102"/>
-      <c r="E48" s="103"/>
-      <c r="F48" s="101"/>
-      <c r="G48" s="101"/>
-      <c r="H48" s="101"/>
-      <c r="I48" s="104"/>
-    </row>
-    <row r="49" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A49" s="65">
-        <f t="shared" ca="1" si="1"/>
+      <c r="C48" s="173" t="s">
+        <v>545</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>543</v>
+      </c>
+      <c r="E48" s="85"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="67"/>
+    </row>
+    <row r="49" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A49" s="43"/>
+      <c r="B49" s="53" t="s">
+        <v>477</v>
+      </c>
+      <c r="C49" s="169"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="63"/>
+    </row>
+    <row r="50" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A50" s="65">
+        <f t="shared" ref="A50:A66" ca="1" si="3">IF(OFFSET(A50,-1,0) ="",OFFSET(A50,-2,0)+1,OFFSET(A50,-1,0)+1 )</f>
         <v>29</v>
       </c>
-      <c r="B49" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="70"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="67"/>
-    </row>
-    <row r="50" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A50" s="43"/>
-      <c r="B50" s="53" t="s">
-        <v>477</v>
-      </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="62"/>
-      <c r="E50" s="83"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="63"/>
-    </row>
-    <row r="51" spans="1:9" s="27" customFormat="1" ht="12.75">
+      <c r="B50" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="C50" s="173" t="s">
+        <v>548</v>
+      </c>
+      <c r="D50" s="24" t="s">
+        <v>551</v>
+      </c>
+      <c r="E50" s="84"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="26"/>
+    </row>
+    <row r="51" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A51" s="65">
-        <f t="shared" ref="A51:A66" ca="1" si="2">IF(OFFSET(A51,-1,0) ="",OFFSET(A51,-2,0)+1,OFFSET(A51,-1,0)+1 )</f>
+        <f t="shared" ref="A51:A61" ca="1" si="4">IF(OFFSET(A51,-1,0) ="",OFFSET(A51,-2,0)+1,OFFSET(A51,-1,0)+1 )</f>
         <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="24"/>
+        <v>512</v>
+      </c>
+      <c r="C51" s="173" t="s">
+        <v>518</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>549</v>
+      </c>
       <c r="E51" s="84"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="26"/>
-    </row>
-    <row r="52" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="I51" s="67"/>
+    </row>
+    <row r="52" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A52" s="65">
         <f ca="1">IF(OFFSET(A52,-1,0) ="",OFFSET(A52,-2,0)+1,OFFSET(A52,-1,0)+1 )</f>
         <v>31</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="24"/>
+        <v>160</v>
+      </c>
+      <c r="C52" s="173" t="s">
+        <v>539</v>
+      </c>
+      <c r="D52" s="70" t="s">
+        <v>253</v>
+      </c>
       <c r="E52" s="84"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="67"/>
     </row>
-    <row r="53" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="53" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A53" s="65">
-        <f ca="1">IF(OFFSET(A53,-1,0) ="",OFFSET(A53,-2,0)+1,OFFSET(A53,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="4"/>
         <v>32</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="24"/>
+      <c r="C53" s="173" t="s">
+        <v>552</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E53" s="84"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="26"/>
     </row>
-    <row r="54" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="54" spans="1:9" s="27" customFormat="1" ht="127.5">
       <c r="A54" s="65">
-        <f ca="1">IF(OFFSET(A54,-1,0) ="",OFFSET(A54,-2,0)+1,OFFSET(A54,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="4"/>
         <v>33</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="84"/>
+      <c r="C54" s="173" t="s">
+        <v>522</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>553</v>
+      </c>
+      <c r="E54" s="84" t="s">
+        <v>511</v>
+      </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="26"/>
     </row>
-    <row r="55" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="55" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A55" s="65">
-        <f ca="1">IF(OFFSET(A55,-1,0) ="",OFFSET(A55,-2,0)+1,OFFSET(A55,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="4"/>
         <v>34</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="24"/>
+      <c r="C55" s="173" t="s">
+        <v>524</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E55" s="84"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="26"/>
     </row>
-    <row r="56" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="56" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A56" s="65">
-        <f ca="1">IF(OFFSET(A56,-1,0) ="",OFFSET(A56,-2,0)+1,OFFSET(A56,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="4"/>
         <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="24"/>
+      <c r="C56" s="173" t="s">
+        <v>525</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E56" s="84"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="26"/>
     </row>
-    <row r="57" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="57" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A57" s="65">
-        <f ca="1">IF(OFFSET(A57,-1,0) ="",OFFSET(A57,-2,0)+1,OFFSET(A57,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="4"/>
         <v>36</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="24"/>
+      <c r="C57" s="173" t="s">
+        <v>526</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>553</v>
+      </c>
       <c r="E57" s="84"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="26"/>
     </row>
-    <row r="58" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="58" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A58" s="65">
-        <f ca="1">IF(OFFSET(A58,-1,0) ="",OFFSET(A58,-2,0)+1,OFFSET(A58,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="4"/>
         <v>37</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="24"/>
+      <c r="C58" s="173" t="s">
+        <v>527</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>553</v>
+      </c>
       <c r="E58" s="84"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="26"/>
     </row>
-    <row r="59" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="59" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A59" s="65">
-        <f ca="1">IF(OFFSET(A59,-1,0) ="",OFFSET(A59,-2,0)+1,OFFSET(A59,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="4"/>
         <v>38</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="24"/>
+      <c r="C59" s="173" t="s">
+        <v>528</v>
+      </c>
+      <c r="D59" s="24" t="s">
+        <v>553</v>
+      </c>
       <c r="E59" s="84"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -31204,219 +31997,272 @@
     </row>
     <row r="60" spans="1:9" s="27" customFormat="1" ht="12.75">
       <c r="A60" s="65">
-        <f ca="1">IF(OFFSET(A60,-1,0) ="",OFFSET(A60,-2,0)+1,OFFSET(A60,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="4"/>
         <v>39</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="24"/>
+      <c r="C60" s="173" t="s">
+        <v>591</v>
+      </c>
+      <c r="D60" s="107" t="s">
+        <v>550</v>
+      </c>
       <c r="E60" s="84"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="26"/>
     </row>
-    <row r="61" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="61" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A61" s="65">
-        <f ca="1">IF(OFFSET(A61,-1,0) ="",OFFSET(A61,-2,0)+1,OFFSET(A61,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="4"/>
         <v>40</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="24"/>
+      <c r="C61" s="173" t="s">
+        <v>554</v>
+      </c>
+      <c r="D61" s="24" t="s">
+        <v>621</v>
+      </c>
       <c r="E61" s="84"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="26"/>
     </row>
-    <row r="62" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="62" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A62" s="65">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>41</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="24"/>
+      <c r="C62" s="173" t="s">
+        <v>560</v>
+      </c>
+      <c r="D62" s="24" t="s">
+        <v>555</v>
+      </c>
       <c r="E62" s="84"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="67"/>
     </row>
-    <row r="63" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="63" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A63" s="65">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>42</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="24"/>
+      <c r="C63" s="173" t="s">
+        <v>557</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E63" s="84"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="67"/>
     </row>
-    <row r="64" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="64" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A64" s="65">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>43</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="24"/>
+      <c r="C64" s="173" t="s">
+        <v>558</v>
+      </c>
+      <c r="D64" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E64" s="84"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="67"/>
     </row>
-    <row r="65" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="65" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A65" s="65">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>44</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="24"/>
+      <c r="C65" s="173" t="s">
+        <v>559</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E65" s="84"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="67"/>
     </row>
-    <row r="66" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="66" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A66" s="65">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>45</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="24"/>
+      <c r="C66" s="173" t="s">
+        <v>561</v>
+      </c>
+      <c r="D66" s="24" t="s">
+        <v>556</v>
+      </c>
       <c r="E66" s="84"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="67"/>
     </row>
-    <row r="67" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A67" s="65">
-        <f ca="1">IF(OFFSET(A67,-1,0) ="",OFFSET(A67,-2,0)+1,OFFSET(A67,-1,0)+1 )</f>
+    <row r="67" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A67" s="43"/>
+      <c r="B67" s="53" t="s">
+        <v>478</v>
+      </c>
+      <c r="C67" s="169"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="83"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
+      <c r="H67" s="64"/>
+      <c r="I67" s="63"/>
+    </row>
+    <row r="68" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A68" s="65">
+        <f t="shared" ca="1" si="2"/>
         <v>46</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="70"/>
-      <c r="E67" s="84"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="67"/>
-    </row>
-    <row r="68" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A68" s="43"/>
-      <c r="B68" s="53" t="s">
-        <v>478</v>
-      </c>
-      <c r="C68" s="61"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="83"/>
-      <c r="F68" s="64"/>
-      <c r="G68" s="64"/>
-      <c r="H68" s="64"/>
-      <c r="I68" s="63"/>
-    </row>
-    <row r="69" spans="1:9" s="27" customFormat="1" ht="12.75">
+      <c r="B68" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="C68" s="173" t="s">
+        <v>580</v>
+      </c>
+      <c r="D68" s="24" t="s">
+        <v>565</v>
+      </c>
+      <c r="E68" s="84"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="26"/>
+    </row>
+    <row r="69" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A69" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">IF(OFFSET(A69,-1,0) ="",OFFSET(A69,-2,0)+1,OFFSET(A69,-1,0)+1 )</f>
         <v>47</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="84"/>
+      <c r="B69" s="101" t="s">
+        <v>198</v>
+      </c>
+      <c r="C69" s="173" t="s">
+        <v>571</v>
+      </c>
+      <c r="D69" s="102" t="s">
+        <v>568</v>
+      </c>
+      <c r="E69" s="84" t="s">
+        <v>566</v>
+      </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="26"/>
     </row>
-    <row r="70" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="70" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A70" s="65">
-        <f ca="1">IF(OFFSET(A70,-1,0) ="",OFFSET(A70,-2,0)+1,OFFSET(A70,-1,0)+1 )</f>
+        <f t="shared" ref="A70:A71" ca="1" si="5">IF(OFFSET(A70,-1,0) ="",OFFSET(A70,-2,0)+1,OFFSET(A70,-1,0)+1 )</f>
         <v>48</v>
       </c>
-      <c r="B70" s="101" t="s">
-        <v>198</v>
-      </c>
-      <c r="C70" s="1"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="84"/>
+      <c r="B70" s="54" t="s">
+        <v>493</v>
+      </c>
+      <c r="C70" s="173" t="s">
+        <v>570</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>567</v>
+      </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="26"/>
     </row>
-    <row r="71" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="71" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A71" s="65">
-        <f t="shared" ref="A71:A72" ca="1" si="3">IF(OFFSET(A71,-1,0) ="",OFFSET(A71,-2,0)+1,OFFSET(A71,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="5"/>
         <v>49</v>
       </c>
-      <c r="B71" s="54" t="s">
-        <v>493</v>
-      </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="24"/>
+      <c r="B71" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C71" s="173" t="s">
+        <v>573</v>
+      </c>
+      <c r="D71" s="24" t="s">
+        <v>564</v>
+      </c>
       <c r="E71" s="84"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="26"/>
     </row>
-    <row r="72" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="72" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A72" s="65">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>50</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C72" s="1"/>
-      <c r="D72" s="24"/>
+      <c r="B72" s="101" t="s">
+        <v>492</v>
+      </c>
+      <c r="C72" s="173" t="s">
+        <v>574</v>
+      </c>
+      <c r="D72" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E72" s="84"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="26"/>
     </row>
-    <row r="73" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="73" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A73" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>51</v>
       </c>
-      <c r="B73" s="101" t="s">
-        <v>492</v>
-      </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="24"/>
+      <c r="B73" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C73" s="173" t="s">
+        <v>578</v>
+      </c>
+      <c r="D73" s="101" t="s">
+        <v>569</v>
+      </c>
       <c r="E73" s="84"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -31425,14 +32271,18 @@
     </row>
     <row r="74" spans="1:9" s="27" customFormat="1" ht="12.75">
       <c r="A74" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>52</v>
       </c>
       <c r="B74" s="112" t="s">
         <v>195</v>
       </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="24"/>
+      <c r="C74" s="173" t="s">
+        <v>579</v>
+      </c>
+      <c r="D74" s="101" t="s">
+        <v>312</v>
+      </c>
       <c r="E74" s="84"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -31444,7 +32294,7 @@
       <c r="B75" s="53" t="s">
         <v>479</v>
       </c>
-      <c r="C75" s="61"/>
+      <c r="C75" s="169"/>
       <c r="D75" s="62"/>
       <c r="E75" s="83"/>
       <c r="F75" s="64"/>
@@ -31452,39 +32302,47 @@
       <c r="H75" s="64"/>
       <c r="I75" s="63"/>
     </row>
-    <row r="76" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="76" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A76" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>53</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="C76" s="1"/>
-      <c r="D76" s="24"/>
+        <v>510</v>
+      </c>
+      <c r="C76" s="173" t="s">
+        <v>581</v>
+      </c>
+      <c r="D76" s="24" t="s">
+        <v>583</v>
+      </c>
       <c r="E76" s="84"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="26"/>
     </row>
-    <row r="77" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="77" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A77" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>54</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="C77" s="1"/>
-      <c r="D77" s="24"/>
+        <v>508</v>
+      </c>
+      <c r="C77" s="173" t="s">
+        <v>582</v>
+      </c>
+      <c r="D77" s="102" t="s">
+        <v>584</v>
+      </c>
       <c r="E77" s="84"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="26"/>
     </row>
-    <row r="78" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="78" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A78" s="65">
         <f ca="1">IF(OFFSET(A78,-1,0) ="",OFFSET(A78,-2,0)+1,OFFSET(A78,-1,0)+1 )</f>
         <v>55</v>
@@ -31492,419 +32350,608 @@
       <c r="B78" s="101" t="s">
         <v>198</v>
       </c>
-      <c r="C78" s="1"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="84"/>
+      <c r="C78" s="173" t="s">
+        <v>590</v>
+      </c>
+      <c r="D78" s="84" t="s">
+        <v>604</v>
+      </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="26"/>
     </row>
-    <row r="79" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="79" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A79" s="65">
-        <f t="shared" ref="A79:A80" ca="1" si="4">IF(OFFSET(A79,-1,0) ="",OFFSET(A79,-2,0)+1,OFFSET(A79,-1,0)+1 )</f>
+        <f t="shared" ref="A79:A80" ca="1" si="6">IF(OFFSET(A79,-1,0) ="",OFFSET(A79,-2,0)+1,OFFSET(A79,-1,0)+1 )</f>
         <v>56</v>
       </c>
       <c r="B79" s="54" t="s">
         <v>495</v>
       </c>
-      <c r="C79" s="1"/>
-      <c r="D79" s="24"/>
+      <c r="C79" s="173" t="s">
+        <v>572</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="E79" s="84"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="26"/>
     </row>
-    <row r="80" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="80" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A80" s="65">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>57</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C80" s="1"/>
-      <c r="D80" s="24"/>
+        <v>512</v>
+      </c>
+      <c r="C80" s="173" t="s">
+        <v>573</v>
+      </c>
+      <c r="D80" s="24" t="s">
+        <v>586</v>
+      </c>
       <c r="E80" s="84"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="26"/>
     </row>
-    <row r="81" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="81" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A81" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>58</v>
       </c>
       <c r="B81" s="101" t="s">
         <v>494</v>
       </c>
-      <c r="C81" s="1"/>
-      <c r="D81" s="24"/>
+      <c r="C81" s="173" t="s">
+        <v>587</v>
+      </c>
+      <c r="D81" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E81" s="84"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="26"/>
     </row>
-    <row r="82" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="82" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A82" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>59</v>
       </c>
-      <c r="B82" s="112" t="s">
-        <v>195</v>
-      </c>
-      <c r="C82" s="1"/>
-      <c r="D82" s="24"/>
+      <c r="B82" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C82" s="173" t="s">
+        <v>589</v>
+      </c>
+      <c r="D82" s="101" t="s">
+        <v>588</v>
+      </c>
       <c r="E82" s="84"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="26"/>
     </row>
-    <row r="83" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A83" s="43"/>
-      <c r="B83" s="53" t="s">
+    <row r="83" spans="1:9" s="27" customFormat="1" ht="12.75">
+      <c r="A83" s="65">
+        <f t="shared" ca="1" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="B83" s="112" t="s">
+        <v>195</v>
+      </c>
+      <c r="C83" s="173" t="s">
+        <v>579</v>
+      </c>
+      <c r="D83" s="101" t="s">
+        <v>312</v>
+      </c>
+      <c r="E83" s="84"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="26"/>
+    </row>
+    <row r="84" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A84" s="43"/>
+      <c r="B84" s="53" t="s">
         <v>480</v>
       </c>
-      <c r="C83" s="61"/>
-      <c r="D83" s="62"/>
-      <c r="E83" s="83"/>
-      <c r="F83" s="64"/>
-      <c r="G83" s="64"/>
-      <c r="H83" s="64"/>
-      <c r="I83" s="63"/>
-    </row>
-    <row r="84" spans="1:9" s="27" customFormat="1" ht="12.75">
-      <c r="A84" s="65">
-        <f t="shared" ca="1" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C84" s="1"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="84"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="26"/>
-    </row>
-    <row r="85" spans="1:9" s="27" customFormat="1" ht="12.75">
+      <c r="C84" s="169"/>
+      <c r="D84" s="62"/>
+      <c r="E84" s="83"/>
+      <c r="F84" s="64"/>
+      <c r="G84" s="64"/>
+      <c r="H84" s="64"/>
+      <c r="I84" s="63"/>
+    </row>
+    <row r="85" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A85" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>61</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="C85" s="1"/>
-      <c r="D85" s="24"/>
+        <v>510</v>
+      </c>
+      <c r="C85" s="173" t="s">
+        <v>593</v>
+      </c>
+      <c r="D85" s="24" t="s">
+        <v>594</v>
+      </c>
       <c r="E85" s="84"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="26"/>
     </row>
-    <row r="86" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="86" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A86" s="65">
-        <f ca="1">IF(OFFSET(A86,-1,0) ="",OFFSET(A86,-2,0)+1,OFFSET(A86,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>62</v>
       </c>
-      <c r="B86" s="101" t="s">
-        <v>198</v>
-      </c>
-      <c r="C86" s="1"/>
-      <c r="D86" s="24"/>
+      <c r="B86" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C86" s="173" t="s">
+        <v>603</v>
+      </c>
+      <c r="D86" s="102" t="s">
+        <v>595</v>
+      </c>
       <c r="E86" s="84"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="26"/>
     </row>
-    <row r="87" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="87" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A87" s="65">
-        <f t="shared" ref="A87:A88" ca="1" si="5">IF(OFFSET(A87,-1,0) ="",OFFSET(A87,-2,0)+1,OFFSET(A87,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A87,-1,0) ="",OFFSET(A87,-2,0)+1,OFFSET(A87,-1,0)+1 )</f>
         <v>63</v>
       </c>
-      <c r="B87" s="54" t="s">
-        <v>496</v>
-      </c>
-      <c r="C87" s="1"/>
-      <c r="D87" s="24"/>
+      <c r="B87" s="101" t="s">
+        <v>198</v>
+      </c>
+      <c r="C87" s="173" t="s">
+        <v>596</v>
+      </c>
+      <c r="D87" s="84" t="s">
+        <v>605</v>
+      </c>
       <c r="E87" s="84"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
       <c r="I87" s="26"/>
     </row>
-    <row r="88" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="88" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A88" s="65">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="A88:A89" ca="1" si="7">IF(OFFSET(A88,-1,0) ="",OFFSET(A88,-2,0)+1,OFFSET(A88,-1,0)+1 )</f>
         <v>64</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C88" s="1"/>
-      <c r="D88" s="24"/>
+      <c r="B88" s="54" t="s">
+        <v>496</v>
+      </c>
+      <c r="C88" s="173" t="s">
+        <v>597</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>598</v>
+      </c>
       <c r="E88" s="84"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
       <c r="I88" s="26"/>
     </row>
-    <row r="89" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="89" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A89" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="7"/>
         <v>65</v>
       </c>
-      <c r="B89" s="101" t="s">
-        <v>497</v>
-      </c>
-      <c r="C89" s="1"/>
-      <c r="D89" s="24"/>
+      <c r="B89" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C89" s="173" t="s">
+        <v>573</v>
+      </c>
+      <c r="D89" s="24" t="s">
+        <v>599</v>
+      </c>
       <c r="E89" s="84"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
       <c r="I89" s="26"/>
     </row>
-    <row r="90" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="90" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A90" s="65">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>66</v>
       </c>
-      <c r="B90" s="112" t="s">
-        <v>195</v>
-      </c>
-      <c r="C90" s="1"/>
-      <c r="D90" s="24"/>
+      <c r="B90" s="101" t="s">
+        <v>497</v>
+      </c>
+      <c r="C90" s="173" t="s">
+        <v>600</v>
+      </c>
+      <c r="D90" s="24" t="s">
+        <v>619</v>
+      </c>
       <c r="E90" s="84"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="26"/>
     </row>
-    <row r="91" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A91" s="43"/>
-      <c r="B91" s="53" t="s">
-        <v>505</v>
-      </c>
-      <c r="C91" s="61"/>
-      <c r="D91" s="62"/>
-      <c r="E91" s="83"/>
-      <c r="F91" s="64"/>
-      <c r="G91" s="64"/>
-      <c r="H91" s="64"/>
-      <c r="I91" s="63"/>
-    </row>
-    <row r="92" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="91" spans="1:9" s="27" customFormat="1" ht="63.75">
+      <c r="A91" s="65">
+        <f t="shared" ca="1" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C91" s="173" t="s">
+        <v>601</v>
+      </c>
+      <c r="D91" s="101" t="s">
+        <v>602</v>
+      </c>
+      <c r="E91" s="84"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="26"/>
+    </row>
+    <row r="92" spans="1:9" s="27" customFormat="1" ht="12.75">
       <c r="A92" s="65">
-        <f t="shared" ref="A92:A98" ca="1" si="6">IF(OFFSET(A92,-1,0) ="",OFFSET(A92,-2,0)+1,OFFSET(A92,-1,0)+1 )</f>
-        <v>67</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="C92" s="1"/>
-      <c r="D92" s="24"/>
+        <f t="shared" ca="1" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="B92" s="112" t="s">
+        <v>195</v>
+      </c>
+      <c r="C92" s="173" t="s">
+        <v>579</v>
+      </c>
+      <c r="D92" s="101" t="s">
+        <v>312</v>
+      </c>
       <c r="E92" s="84"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
-      <c r="I92" s="67"/>
-    </row>
-    <row r="93" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A93" s="65">
-        <f t="shared" ca="1" si="6"/>
-        <v>68</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="C93" s="1"/>
-      <c r="D93" s="24"/>
-      <c r="E93" s="84"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="67"/>
+      <c r="I92" s="26"/>
+    </row>
+    <row r="93" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A93" s="43"/>
+      <c r="B93" s="53" t="s">
+        <v>504</v>
+      </c>
+      <c r="C93" s="169"/>
+      <c r="D93" s="62"/>
+      <c r="E93" s="83"/>
+      <c r="F93" s="64"/>
+      <c r="G93" s="64"/>
+      <c r="H93" s="64"/>
+      <c r="I93" s="63"/>
     </row>
     <row r="94" spans="1:9" s="29" customFormat="1" ht="14.25">
       <c r="A94" s="65">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="A94:A100" ca="1" si="8">IF(OFFSET(A94,-1,0) ="",OFFSET(A94,-2,0)+1,OFFSET(A94,-1,0)+1 )</f>
         <v>69</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="C94" s="1"/>
-      <c r="D94" s="24"/>
+        <v>498</v>
+      </c>
+      <c r="C94" s="173" t="s">
+        <v>606</v>
+      </c>
+      <c r="D94" s="24" t="s">
+        <v>607</v>
+      </c>
       <c r="E94" s="84"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
       <c r="I94" s="67"/>
     </row>
-    <row r="95" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A95" s="43"/>
-      <c r="B95" s="53" t="s">
-        <v>506</v>
-      </c>
-      <c r="C95" s="61"/>
-      <c r="D95" s="62"/>
-      <c r="E95" s="83"/>
-      <c r="F95" s="64"/>
-      <c r="G95" s="64"/>
-      <c r="H95" s="64"/>
-      <c r="I95" s="63"/>
-    </row>
-    <row r="96" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="95" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A95" s="65">
+        <f t="shared" ca="1" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C95" s="173" t="s">
+        <v>609</v>
+      </c>
+      <c r="D95" s="24" t="s">
+        <v>608</v>
+      </c>
+      <c r="E95" s="84"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="67"/>
+    </row>
+    <row r="96" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A96" s="65">
-        <f t="shared" ca="1" si="6"/>
-        <v>70</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>71</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="C96" s="1"/>
-      <c r="D96" s="24"/>
+        <v>500</v>
+      </c>
+      <c r="C96" s="173" t="s">
+        <v>610</v>
+      </c>
+      <c r="D96" s="24" t="s">
+        <v>611</v>
+      </c>
       <c r="E96" s="84"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
       <c r="I96" s="67"/>
     </row>
-    <row r="97" spans="1:9" s="29" customFormat="1" ht="14.25">
-      <c r="A97" s="65">
-        <f t="shared" ca="1" si="6"/>
-        <v>71</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C97" s="1"/>
-      <c r="D97" s="24"/>
-      <c r="E97" s="84"/>
-      <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="67"/>
+    <row r="97" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A97" s="43"/>
+      <c r="B97" s="53" t="s">
+        <v>505</v>
+      </c>
+      <c r="C97" s="169"/>
+      <c r="D97" s="62"/>
+      <c r="E97" s="83"/>
+      <c r="F97" s="64"/>
+      <c r="G97" s="64"/>
+      <c r="H97" s="64"/>
+      <c r="I97" s="63"/>
     </row>
     <row r="98" spans="1:9" s="29" customFormat="1" ht="14.25">
       <c r="A98" s="65">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="8"/>
         <v>72</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="C98" s="1"/>
-      <c r="D98" s="24"/>
+        <v>501</v>
+      </c>
+      <c r="C98" s="173" t="s">
+        <v>612</v>
+      </c>
+      <c r="D98" s="24" t="s">
+        <v>613</v>
+      </c>
       <c r="E98" s="84"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
       <c r="I98" s="67"/>
     </row>
-    <row r="99" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A99" s="68"/>
-      <c r="B99" s="160" t="s">
-        <v>210</v>
-      </c>
-      <c r="C99" s="161"/>
-      <c r="D99" s="162"/>
-      <c r="E99" s="86"/>
-      <c r="F99" s="32"/>
-      <c r="G99" s="32"/>
-      <c r="H99" s="32"/>
-      <c r="I99" s="69"/>
-    </row>
-    <row r="100" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A100" s="71">
-        <f t="shared" ref="A100:A103" ca="1" si="7">IF(OFFSET(A100,-1,0) ="",OFFSET(A100,-2,0)+1,OFFSET(A100,-1,0)+1 )</f>
+    <row r="99" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A99" s="65">
+        <f t="shared" ca="1" si="8"/>
         <v>73</v>
       </c>
+      <c r="B99" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C99" s="173" t="s">
+        <v>614</v>
+      </c>
+      <c r="D99" s="24" t="s">
+        <v>615</v>
+      </c>
+      <c r="E99" s="84"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="67"/>
+    </row>
+    <row r="100" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A100" s="65">
+        <f t="shared" ca="1" si="8"/>
+        <v>74</v>
+      </c>
       <c r="B100" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="C100" s="1"/>
-      <c r="D100" s="24"/>
+        <v>503</v>
+      </c>
+      <c r="C100" s="173" t="s">
+        <v>616</v>
+      </c>
+      <c r="D100" s="24" t="s">
+        <v>617</v>
+      </c>
       <c r="E100" s="84"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
-      <c r="I100" s="26"/>
-    </row>
-    <row r="101" spans="1:9" s="27" customFormat="1" ht="25.5">
-      <c r="A101" s="71">
-        <f t="shared" ca="1" si="7"/>
-        <v>74</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="C101" s="1"/>
-      <c r="D101" s="24"/>
-      <c r="E101" s="84"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="26"/>
-    </row>
-    <row r="102" spans="1:9" s="27" customFormat="1" ht="12.75">
+      <c r="I100" s="67"/>
+    </row>
+    <row r="101" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A101" s="68"/>
+      <c r="B101" s="160" t="s">
+        <v>210</v>
+      </c>
+      <c r="C101" s="161"/>
+      <c r="D101" s="162"/>
+      <c r="E101" s="86"/>
+      <c r="F101" s="32"/>
+      <c r="G101" s="32"/>
+      <c r="H101" s="32"/>
+      <c r="I101" s="69"/>
+    </row>
+    <row r="102" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A102" s="71">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="A102:A109" ca="1" si="9">IF(OFFSET(A102,-1,0) ="",OFFSET(A102,-2,0)+1,OFFSET(A102,-1,0)+1 )</f>
         <v>75</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="C102" s="1"/>
-      <c r="D102" s="24"/>
+        <v>513</v>
+      </c>
+      <c r="C102" s="173" t="s">
+        <v>618</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>622</v>
+      </c>
       <c r="E102" s="84"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
       <c r="I102" s="26"/>
     </row>
-    <row r="103" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="103" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A103" s="71">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v>76</v>
       </c>
-      <c r="B103" s="54" t="s">
-        <v>511</v>
-      </c>
-      <c r="C103" s="1"/>
-      <c r="D103" s="24"/>
+      <c r="B103" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C103" s="173" t="s">
+        <v>624</v>
+      </c>
+      <c r="D103" s="24" t="s">
+        <v>623</v>
+      </c>
       <c r="E103" s="84"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
       <c r="I103" s="26"/>
     </row>
-    <row r="104" spans="1:9" ht="12.75">
-      <c r="E104" s="87"/>
-    </row>
-    <row r="105" spans="1:9" ht="12.75">
-      <c r="E105" s="87"/>
-    </row>
-    <row r="106" spans="1:9" ht="12.75">
-      <c r="E106" s="87"/>
-    </row>
-    <row r="107" spans="1:9" ht="12.75">
-      <c r="E107" s="87"/>
-    </row>
-    <row r="108" spans="1:9" ht="12.75">
-      <c r="E108" s="87"/>
-    </row>
-    <row r="109" spans="1:9" ht="12.75">
-      <c r="E109" s="87"/>
+    <row r="104" spans="1:9" s="27" customFormat="1" ht="63.75">
+      <c r="A104" s="71">
+        <f t="shared" ca="1" si="9"/>
+        <v>77</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C104" s="173" t="s">
+        <v>625</v>
+      </c>
+      <c r="D104" s="24" t="s">
+        <v>626</v>
+      </c>
+      <c r="E104" s="84"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="26"/>
+    </row>
+    <row r="105" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A105" s="71">
+        <f t="shared" ca="1" si="9"/>
+        <v>78</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C105" s="173" t="s">
+        <v>627</v>
+      </c>
+      <c r="D105" s="24" t="s">
+        <v>628</v>
+      </c>
+      <c r="E105" s="84"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="26"/>
+    </row>
+    <row r="106" spans="1:9" s="27" customFormat="1" ht="25.5">
+      <c r="A106" s="71">
+        <f t="shared" ca="1" si="9"/>
+        <v>79</v>
+      </c>
+      <c r="B106" s="54" t="s">
+        <v>509</v>
+      </c>
+      <c r="C106" s="173" t="s">
+        <v>629</v>
+      </c>
+      <c r="D106" s="24" t="s">
+        <v>631</v>
+      </c>
+      <c r="E106" s="84"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="26"/>
+    </row>
+    <row r="107" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A107" s="71">
+        <f t="shared" ca="1" si="9"/>
+        <v>80</v>
+      </c>
+      <c r="B107" s="54" t="s">
+        <v>632</v>
+      </c>
+      <c r="C107" s="173" t="s">
+        <v>630</v>
+      </c>
+      <c r="D107" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="E107" s="84"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="26"/>
+    </row>
+    <row r="108" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A108" s="71">
+        <f t="shared" ca="1" si="9"/>
+        <v>81</v>
+      </c>
+      <c r="B108" s="54" t="s">
+        <v>634</v>
+      </c>
+      <c r="C108" s="173" t="s">
+        <v>636</v>
+      </c>
+      <c r="D108" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="E108" s="84"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="26"/>
+    </row>
+    <row r="109" spans="1:9" s="27" customFormat="1" ht="63.75">
+      <c r="A109" s="71">
+        <f t="shared" ca="1" si="9"/>
+        <v>82</v>
+      </c>
+      <c r="B109" s="54" t="s">
+        <v>635</v>
+      </c>
+      <c r="C109" s="173" t="s">
+        <v>633</v>
+      </c>
+      <c r="D109" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="E109" s="84"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="26"/>
     </row>
     <row r="110" spans="1:9" ht="12.75">
       <c r="E110" s="87"/>
@@ -34507,14 +35554,476 @@
     <row r="976" spans="5:5" ht="12.75">
       <c r="E976" s="87"/>
     </row>
+    <row r="977" spans="5:5" ht="12.75">
+      <c r="E977" s="87"/>
+    </row>
+    <row r="978" spans="5:5" ht="12.75">
+      <c r="E978" s="87"/>
+    </row>
+    <row r="979" spans="5:5" ht="12.75">
+      <c r="E979" s="87"/>
+    </row>
+    <row r="980" spans="5:5" ht="12.75">
+      <c r="E980" s="87"/>
+    </row>
+    <row r="981" spans="5:5" ht="12.75">
+      <c r="E981" s="87"/>
+    </row>
+    <row r="982" spans="5:5" ht="12.75">
+      <c r="E982" s="87"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A20:I109"/>
   <mergeCells count="12">
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" sqref="F38 F41:F42 F20:H36 F44 F94:H96 F77:H83 F68:H74 F85:H92 F98:H109 F50:H66 G38:H39 G41:H48 F40:H40 F46:F48">
+      <formula1>$A$11:$A$15</formula1>
+    </dataValidation>
+    <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F75:H76 F93:H93 F84:H84 F37:H37 F67:H67 F18:H19 F49:H49 F97:H97"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="12" style="36" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="37" customWidth="1"/>
+    <col min="3" max="4" width="35.140625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" style="37" customWidth="1"/>
+    <col min="6" max="8" width="9.7109375" style="37" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="37" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="4" customFormat="1" ht="14.25">
+      <c r="A1" s="152"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:24" s="4" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A2" s="153" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:24" s="4" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="154"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:24" s="9" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A4" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="156" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="156"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="X4" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="9" customFormat="1" ht="144.75" customHeight="1">
+      <c r="A5" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="157"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="X5" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" s="9" customFormat="1" ht="25.5">
+      <c r="A6" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="157"/>
+      <c r="C6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:24" s="9" customFormat="1">
+      <c r="A7" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="158" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="158"/>
+      <c r="D7" s="158"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="8"/>
+      <c r="X7" s="11"/>
+    </row>
+    <row r="8" spans="1:24" s="12" customFormat="1">
+      <c r="A8" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="159"/>
+      <c r="C8" s="159"/>
+      <c r="D8" s="159"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:24" s="12" customFormat="1">
+      <c r="A9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="13" t="str">
+        <f>F17</f>
+        <v>Internal Build 03112011</v>
+      </c>
+      <c r="C9" s="13" t="str">
+        <f>G17</f>
+        <v>Internal build 14112011</v>
+      </c>
+      <c r="D9" s="13" t="str">
+        <f>H17</f>
+        <v>External build 16112011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" s="12" customFormat="1">
+      <c r="A10" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="14">
+        <f>SUM(B11:B14)</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="14">
+        <f>SUM(C11:C14)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="14">
+        <f>SUM(D11:D14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" s="12" customFormat="1">
+      <c r="A11" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="15">
+        <f>COUNTIF($F$18:$F$21,"*Passed")</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
+        <f>COUNTIF($G$18:$G$21,"*Passed")</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="15">
+        <f>COUNTIF($H$18:$H$21,"*Passed")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" s="12" customFormat="1">
+      <c r="A12" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="15">
+        <f>COUNTIF($F$18:$F$21,"*Failed*")</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="15">
+        <f>COUNTIF($G$18:$G$21,"*Failed*")</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="15">
+        <f>COUNTIF($H$18:$H$21,"*Failed*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" s="12" customFormat="1">
+      <c r="A13" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="15">
+        <f>COUNTIF($F$18:$F$21,"*Not Run*")</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="15">
+        <f>COUNTIF($G$18:$G$21,"*Not Run*")</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="15">
+        <f>COUNTIF($H$18:$H$21,"*Not Run*")</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:24" s="12" customFormat="1">
+      <c r="A14" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="15">
+        <f>COUNTIF($F$18:$F$21,"*NA*")</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="15">
+        <f>COUNTIF($G$18:$G$21,"*NA*")</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="15">
+        <f>COUNTIF($H$18:$H$21,"*NA*")</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:24" s="12" customFormat="1" ht="38.25">
+      <c r="A15" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="15">
+        <f>COUNTIF($F$18:$F$21,"*Passed in previous build*")</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="15">
+        <f>COUNTIF($G$18:$G$21,"*Passed in previous build*")</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="15">
+        <f>COUNTIF($H$18:$H$21,"*Passed in previous build*")</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:24" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="148" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="148"/>
+      <c r="H16" s="148"/>
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="1:9" s="21" customFormat="1" ht="38.25">
+      <c r="A17" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A18" s="22"/>
+      <c r="B18" s="149" t="s">
+        <v>637</v>
+      </c>
+      <c r="C18" s="150"/>
+      <c r="D18" s="151"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="22"/>
+    </row>
+    <row r="19" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>651</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="26"/>
+    </row>
+    <row r="20" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A20" s="2">
+        <f t="shared" ref="A20:A23" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>642</v>
+      </c>
+      <c r="E20" s="25"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:9" s="27" customFormat="1" ht="51">
+      <c r="A21" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>643</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A22" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>649</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A23" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>649</v>
+      </c>
+      <c r="E23" s="25"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B99:D99"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:E3"/>
@@ -34523,11 +36032,11 @@
     <mergeCell ref="B5:D5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="F45:F49 F84:H90 F20:H36 F69:H74 G38:H49 F38 F40:F41 F51:H67 F43 F77:H82 F92:H94 F96:H103">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:H18"/>
+    <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
+    <dataValidation type="list" allowBlank="1" sqref="F19:H23">
       <formula1>$A$11:$A$15</formula1>
     </dataValidation>
-    <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F75:H76 F91:H91 F83:H83 F37:H37 F68:H68 F18:H19 F50:H50 F95:H95"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated file on 03/11 - Assignment 4,5
</commit_message>
<xml_diff>
--- a/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
+++ b/Test Design Techniques - Nguyễn Thị Vân Anh.xlsx
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignment 1'!$A$17:$X$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Assignment 2'!$A$19:$Z$128</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Assignment 3'!$A$17:$X$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Assignment 4'!$A$20:$I$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Assignment 4'!$A$20:$I$108</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Assignment 5'!$A$17:$X$17</definedName>
     <definedName name="abc" localSheetId="0">#REF!</definedName>
     <definedName name="abc" localSheetId="1">#REF!</definedName>
@@ -546,7 +546,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="705">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -2326,72 +2326,18 @@
 4. Click on Sign up button</t>
   </si>
   <si>
-    <t xml:space="preserve">When the user enters less than 2 characters  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When the user enters 2 characters  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When the user enters greater than 2 and less than 50 characters  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When the user enters 10 numeric characters </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When the user enters less than 5 characters  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When the user enters 5 characters  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When the user enters greater than 5 and less than 350 characters  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When the user enters 350 characters  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When the user enters greater than 350 characters  </t>
-  </si>
-  <si>
     <t>Check Copy/Paste Address</t>
   </si>
   <si>
     <t>When the user selects a Province</t>
   </si>
   <si>
-    <t>Check scroll bar of Province</t>
-  </si>
-  <si>
     <t>When the user selects a District</t>
   </si>
   <si>
-    <t>Check scroll bar of District</t>
-  </si>
-  <si>
-    <t>Check scroll bar of Ward</t>
-  </si>
-  <si>
     <t>When the user selects a Ward</t>
   </si>
   <si>
-    <t>When Home is in default status</t>
-  </si>
-  <si>
-    <t>When Home is unchecked</t>
-  </si>
-  <si>
-    <t>When Home is checked</t>
-  </si>
-  <si>
-    <t>When Office is in default status</t>
-  </si>
-  <si>
-    <t>When Office is unchecked</t>
-  </si>
-  <si>
-    <t>When Office is checked</t>
-  </si>
-  <si>
     <t>Check Home button</t>
   </si>
   <si>
@@ -2408,9 +2354,6 @@
   </si>
   <si>
     <t>Add address fail when the user clicks on the Cancel button</t>
-  </si>
-  <si>
-    <t>Check default value</t>
   </si>
   <si>
     <t xml:space="preserve">Special characters:
@@ -2419,9 +2362,6 @@
 - SQL injection </t>
   </si>
   <si>
-    <t>Check mandatory</t>
-  </si>
-  <si>
     <t>New address as home can be added successfully when all fields are entered valid values</t>
   </si>
   <si>
@@ -2435,80 +2375,22 @@
   </si>
   <si>
     <t>1. Observe the display of the Full Name</t>
-  </si>
-  <si>
-    <t>1. Don't enter value 
-2. Enter other fields are valid
-3. Click on "Save" button</t>
   </si>
   <si>
     <t>Full Name is blank 
 The placeholder is "First Last"</t>
   </si>
   <si>
-    <t>1. Enter "Nguyen Thi Van Anh"
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
     <t>System will show error message "Please enter your Full name"</t>
   </si>
   <si>
-    <t>1. Enter "^&amp;*"
-2. Click on Close (x) button
-3. Enter HTML code: &lt;!DOCTYPE html&gt;&lt;html&gt;&lt;body&gt;&lt;h1&gt;Học lập trình HTML&lt;/h1&gt;&lt;/body&gt;&lt;/html&gt;
-4. Click on Close (x) button
-5. Enter javascript: &lt;script src="myScript.js"&gt;&lt;/script&gt;
-6. Click on Close (x) button
-7. Enter SQL injection: SELECT * FROM Users WHERE Username = 'Vanh' AND Password = '12345678'</t>
-  </si>
-  <si>
     <t>System will show error message "Name should not contain special characters"</t>
   </si>
   <si>
-    <t>1. Enter "12345678"
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
-    <t>1. Enter "Vanh1234"
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
-    <t>1. Enter "123$%^"</t>
-  </si>
-  <si>
-    <t>1. Enter "Vanh$%^"</t>
-  </si>
-  <si>
-    <t>1. Enter "Vanh1234%^&amp;"</t>
-  </si>
-  <si>
     <t>Allow Copy/Paste Full Name</t>
   </si>
   <si>
-    <t>1. Enter " Nguyen Thi Van Anh "
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
     <t>'System will show error message "The name length should be 2-50 characters"</t>
-  </si>
-  <si>
-    <t>1. Enter 2 characters (valid Full Name)
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
-    <t>1. Enter 3 characters (valid Full Name)
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
-    <t>1. Enter 50 characters (valid Full Name)
-2. Enter other fields are valid
-3. Click on "Save" button</t>
   </si>
   <si>
     <t>1. Observe the display of the Phone Number</t>
@@ -2524,37 +2406,7 @@
 The placeholder is "Please enter your Phone number"</t>
   </si>
   <si>
-    <t>1. Enter any character
-2. Click on close (x) button</t>
-  </si>
-  <si>
-    <t>1. Enter "^&amp;*"
-2. Enter HTML code: &lt;!DOCTYPE html&gt;&lt;html&gt;&lt;body&gt;&lt;h1&gt;Học lập trình HTML&lt;/h1&gt;&lt;/body&gt;&lt;/html&gt;
-3. Enter javascript: &lt;script src="myScript.js"&gt;&lt;/script&gt;
-4. Enter SQL injection: SELECT * FROM Users WHERE Username = 'Vanh' AND Password = '12345678'</t>
-  </si>
-  <si>
-    <t>1. Enter "0981980721"
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
-    <t>1. Enter " 0981 980 721 "</t>
-  </si>
-  <si>
     <t>System will show error message "The length of phone number should be 10 characters"</t>
-  </si>
-  <si>
-    <t>1. Enter "123"</t>
-  </si>
-  <si>
-    <t>1. Enter "09819807211"</t>
-  </si>
-  <si>
-    <t>1. Enter "Nguyen Thi Van Anh"</t>
-  </si>
-  <si>
-    <t>1. Enter "0981980721"</t>
   </si>
   <si>
     <t>1. Observe the display of the Address</t>
@@ -2570,50 +2422,13 @@
 The placeholder is "Please enter your Address"</t>
   </si>
   <si>
-    <t>1. Enter "Đường Láng"
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
     <t>System will show error message "The Address should not contain special characters"</t>
   </si>
   <si>
-    <t>1. Enter " Đường Láng "
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
     <t>'System will show error message "The Address length should be 5-350 characters"</t>
   </si>
   <si>
     <t>System will show error message "The Address length should be 5-350 characters"</t>
-  </si>
-  <si>
-    <t>1. Enter 5 characters (valid Address)
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
-    <t>1. Enter 6 characters (valid Address)
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
-    <t>1. Enter 350 characters (valid Address)
-2. Enter other fields are valid
-3. Click on "Save" button</t>
-  </si>
-  <si>
-    <t>1. Enter 4 characters</t>
-  </si>
-  <si>
-    <t>1. Enter 351 characters</t>
-  </si>
-  <si>
-    <t>1. Enter 1 character</t>
-  </si>
-  <si>
-    <t>1. Enter 51 characters</t>
   </si>
   <si>
     <t>System will show error message "Please select your Province"</t>
@@ -2623,26 +2438,11 @@
 The placeholder is "Please choose your Province"</t>
   </si>
   <si>
-    <t>Sorting trong lazada trình bày khó</t>
-  </si>
-  <si>
-    <t>There is a scrollbar when the list of Province exceeds the display frame</t>
-  </si>
-  <si>
-    <t>There are 63 provinces of VN</t>
-  </si>
-  <si>
     <t>Do not allow paste, allow copy Province</t>
-  </si>
-  <si>
-    <t>1. Click on Province</t>
   </si>
   <si>
     <t>1. Click on Province
 2. Observe the display of dropdown list</t>
-  </si>
-  <si>
-    <t>1. Click on District</t>
   </si>
   <si>
     <t>1. Don't select value
@@ -2665,282 +2465,671 @@
     <t>Check Copy/Paste District</t>
   </si>
   <si>
-    <t>1. Paste value
+    <t>1. Observe the display of the Province</t>
+  </si>
+  <si>
+    <t>1. Select a Province
+2. Observe the display of the District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">District is blank and disable
+The placeholder is "Please choose your District"
+</t>
+  </si>
+  <si>
+    <t>District is enable</t>
+  </si>
+  <si>
+    <t>System will show error message "Please select your District"</t>
+  </si>
+  <si>
+    <t>1. Click on District
+2. Select a District
+3. Enter other fields are valid
+4. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>Do not allow paste, allow copy District</t>
+  </si>
+  <si>
+    <t>1. Click on District
+2. Observe the display of dropdown list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ward is blank and disable
+The placeholder is "Please choose your Ward"
+</t>
+  </si>
+  <si>
+    <t>Ward is enable</t>
+  </si>
+  <si>
+    <t>1. Click on Ward
+2. Observe the display of dropdown list</t>
+  </si>
+  <si>
+    <t>System will show error message "Please select your Ward"</t>
+  </si>
+  <si>
+    <t>1. Click on Ward
+2. Select a Ward
+3. Enter other fields are valid
+4. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>Do not allow paste, allow copy Ward</t>
+  </si>
+  <si>
+    <t>1. Select a District
+2. Observe the display of the Ward</t>
+  </si>
+  <si>
+    <t>1. Observe the display of the Home button</t>
+  </si>
+  <si>
+    <t>Home button is enable and unchecked</t>
+  </si>
+  <si>
+    <t>Icon on Home button is gray</t>
+  </si>
+  <si>
+    <t>1. Don’t click on Home button
+2. Observe the display of the Home button</t>
+  </si>
+  <si>
+    <t>1. Click on Home button
+2. Observe the display of Home button</t>
+  </si>
+  <si>
+    <t>Icon on Home button is hightlighted</t>
+  </si>
+  <si>
+    <t>1. Observe the display of the Office button</t>
+  </si>
+  <si>
+    <t>Office button is enable and unchecked</t>
+  </si>
+  <si>
+    <t>1. Don’t click on Office button
+2. Observe the display of the Office button</t>
+  </si>
+  <si>
+    <t>Icon on Office button is gray</t>
+  </si>
+  <si>
+    <t>1. Click on Office button
+2. Observe the display of Office button</t>
+  </si>
+  <si>
+    <t>Icon on Office button is hightlighted</t>
+  </si>
+  <si>
+    <t>1. Enter all fields are valid
+2. Select Home button
+3. Click on Save button</t>
+  </si>
+  <si>
+    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book</t>
+  </si>
+  <si>
+    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book, automatic delete all leading, trailing spaces from Full Name</t>
+  </si>
+  <si>
+    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book, automatic delete all leading, trailing spaces from Address</t>
+  </si>
+  <si>
+    <t>Add new address as home successfully, return to Address book screen, new address will be displayed on the top of Address Book</t>
+  </si>
+  <si>
+    <t>Add new address as office successfully, return to Address book screen, new address will be displayed on the top of Address Book</t>
+  </si>
+  <si>
+    <t>1. Enter all fields are valid
+2. Select Office button
+3. Click on Save button</t>
+  </si>
+  <si>
+    <t>1. Enter all mandatory fields are valid
+2. Don't Select Office button/Home button
+3. Click on Save button</t>
+  </si>
+  <si>
+    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book
+Two button: Home and Office are displayed at the created address</t>
+  </si>
+  <si>
+    <t>1. Enter all fields are invalid
+2. Click on Save button</t>
+  </si>
+  <si>
+    <t>Add address fail, the system will display the corresponding error message below each field</t>
+  </si>
+  <si>
+    <t>1. Enter value into fields
+2. Click on Cancel button</t>
+  </si>
+  <si>
+    <t>Precondition: The user added 1 address
+1. Enter the value of all fields same previous address
+2. Click on Save button</t>
+  </si>
+  <si>
+    <t>Add address fail, return to Address book screen</t>
+  </si>
+  <si>
+    <t>When the user adds duplicate addresses</t>
+  </si>
+  <si>
+    <t>Precondition: The user added 1 address
+1. Enter Full Name and Phone number are same Previous address
+2. Enter other fields are different
+2. Click on Save button</t>
+  </si>
+  <si>
+    <t>When the user adds a new address completely different from the previous one</t>
+  </si>
+  <si>
+    <t>When the user adds a new address with the same consignee as the previous address</t>
+  </si>
+  <si>
+    <t>Precondition: The user added 1 address
+1. Enter the value of all fields are different previous address
+2. Click on Save button</t>
+  </si>
+  <si>
+    <t>1. Check Delete Address function</t>
+  </si>
+  <si>
+    <t>Verify that a confirmation pop-up is displayed when the user click on Delete icon</t>
+  </si>
+  <si>
+    <t>Delete address successfully when the user click on Delete button on pop-up</t>
+  </si>
+  <si>
+    <t>Delete address fail when the user click on Cancel button on pop-up</t>
+  </si>
+  <si>
+    <t>Verify that the user cannot delete default address</t>
+  </si>
+  <si>
+    <t>Show error message "You cannot delete your default address"</t>
+  </si>
+  <si>
+    <t>Delete address successfully, this address is not displayed in Address Book anymore</t>
+  </si>
+  <si>
+    <t>1. Select an address
+1. Click on Delete icon</t>
+  </si>
+  <si>
+    <t>1. Select an address that is not default address
+2. Click on Delete icon
+3. Click on Delete button on pop-up</t>
+  </si>
+  <si>
+    <t>1. Select an address
+2. Click on Delete icon
+3. Click on Delete button on pop-up</t>
+  </si>
+  <si>
+    <t>1. Select default address
+2. Click on Delete icon
+3. Click on Delete button on pop-up</t>
+  </si>
+  <si>
+    <t>1. Select an address
+2. Click on Delete icon
+3. Click on Cancel button on pop-up</t>
+  </si>
+  <si>
+    <t>Delete address fail, return to the Edit address screen</t>
+  </si>
+  <si>
+    <t>Delete address fail when the user click on Close (x) icon on pop-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A confirmation pop-up is displayed
+This pop up shows selected address information correctly </t>
+  </si>
+  <si>
+    <t>Show "123"
+Allow Copy/Paste only numeric characters</t>
+  </si>
+  <si>
+    <t>All will show error message "The Address should not contain special characters"</t>
+  </si>
+  <si>
+    <t>Precondition: The user don't select District
+1. Observe the display of the Ward</t>
+  </si>
+  <si>
+    <t>Precondition: The user don't select Province
+1. Observe the display of the District</t>
+  </si>
+  <si>
+    <t>Delete address fail when the user pressed ESC key from keyboard</t>
+  </si>
+  <si>
+    <t>1. Select an address
+2. Click on Delete icon
+3.  Pressed ESC key from keyboard</t>
+  </si>
+  <si>
+    <t>Check default value of Full Name</t>
+  </si>
+  <si>
+    <t>Check mandatory of Ful Name</t>
+  </si>
+  <si>
+    <t>1. Don't enter value into the Full Name
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter any character into the Full Name
+2. Click on Clear all button</t>
+  </si>
+  <si>
+    <t>1. Enter "Nguyen Thi Van Anh" into the Full Name
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter "^&amp;*" into the Full Name
+2. Click on Clear all button
+3. Enter HTML code: &lt;!DOCTYPE html&gt;&lt;html&gt;&lt;body&gt;&lt;h1&gt;Học lập trình HTML&lt;/h1&gt;&lt;/body&gt;&lt;/html&gt; into the Full Name
+4. Click on Clear all button
+5. Enter javascript: &lt;script src="myScript.js"&gt;&lt;/script&gt; into the Full Name
+6. Click on Clear all button
+7. Enter SQL injection: SELECT * FROM Users WHERE Username = 'Vanh' AND Password = '12345678' into the Full Name</t>
+  </si>
+  <si>
+    <t>Check Full Name when the user clicks on Clear all button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters only alphabetic characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters only special characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters only numeric characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters alphabetic and numeric characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters numeric and special characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters alphabetic and special characters  </t>
+  </si>
+  <si>
+    <t>Check Full Name when the user enters alphabetic, numeric and special characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters less than 2 characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters 2 characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters greater than 2 and less than 50 characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters 50 characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Full Name when the user enters greater than 50 characters  </t>
+  </si>
+  <si>
+    <t>1. Enter "12345678" into the Full Name
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter "Vanh1234" into the Full Name
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter "123$%^" into the Full Name</t>
+  </si>
+  <si>
+    <t>1. Enter "Vanh$%^" into the Full Name</t>
+  </si>
+  <si>
+    <t>1. Enter "Vanh1234%^&amp;" into the Full Name</t>
+  </si>
+  <si>
+    <t>1.Copy/Paste "abc123$%^" into the Full Name</t>
+  </si>
+  <si>
+    <t>1. Enter " Nguyen Thi Van Anh " into the Full Name
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 1 character into the Full Name</t>
+  </si>
+  <si>
+    <t>1. Enter 2 characters (valid Full Name) into the Full Name
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 3 characters (valid Full Name) into the Full Name
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 50 characters (valid Full Name) into the Full Name
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 51 characters into the Full Name</t>
+  </si>
+  <si>
+    <t>Check Trim space of Full Name</t>
+  </si>
+  <si>
+    <t>Check Phone Number when the user clicks on Clear all button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Phone Number when the user enters alphabetic characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Phone Number when the user enters special characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Phone Number when the user enters numeric characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Phone Number when the user enters less than 10 numeric characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Phone Number when the user enters 10 numeric characters </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Phone Number when the user enters greater than 10 numeric characters  </t>
+  </si>
+  <si>
+    <t>Check default value of Phone Number</t>
+  </si>
+  <si>
+    <t>Check mandatory of Phone Number</t>
+  </si>
+  <si>
+    <t>Check Trim space of Phone Number</t>
+  </si>
+  <si>
+    <t>1. Don't enter value into the Phone Number
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter any character  into the Phone Number
+2. Click on Clear all button</t>
+  </si>
+  <si>
+    <t>1. Enter "Nguyen Thi Van Anh"  into the Phone Number</t>
+  </si>
+  <si>
+    <t>1. Enter "^&amp;*"  into the Phone Number
+2. Enter HTML code: &lt;!DOCTYPE html&gt;&lt;html&gt;&lt;body&gt;&lt;h1&gt;Học lập trình HTML&lt;/h1&gt;&lt;/body&gt;&lt;/html&gt;  into the Phone Number
+3. Enter javascript: &lt;script src="myScript.js"&gt;&lt;/script&gt; into the Phone Number
+4. Enter SQL injection: SELECT * FROM Users WHERE Username = 'Vanh' AND Password = '12345678'  into the Phone Number</t>
+  </si>
+  <si>
+    <t>1. Enter "0981980721"  into the Phone Number</t>
+  </si>
+  <si>
+    <t>1.Copy/Paste "abc123$%^"  into the Phone Number</t>
+  </si>
+  <si>
+    <t>1. Enter " 0981 980 721 "  into the Phone Number</t>
+  </si>
+  <si>
+    <t>1. Enter "123"  into the Phone Number</t>
+  </si>
+  <si>
+    <t>1. Enter "0981980721"  into the Phone Number
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter "09819807211"  into the Phone Number</t>
+  </si>
+  <si>
+    <t>Check default value of Address</t>
+  </si>
+  <si>
+    <t>Check mandatory of Address</t>
+  </si>
+  <si>
+    <t>Check Trim space of Address</t>
+  </si>
+  <si>
+    <t>Check Address when the user clicks on Clear all button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters only alphabetic characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters only special characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters only numeric characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters alphabetic and numeric characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters numeric and special characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters alphabetic and special characters  </t>
+  </si>
+  <si>
+    <t>Check Address when the user enters alphabetic, numeric and special characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters less than 5 characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters 5 characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters greater than 5 and less than 350 characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters 350 characters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Address when the user enters greater than 350 characters  </t>
+  </si>
+  <si>
+    <t>1. Don't enter value into the Address
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter any character into the Address
+2. Click on Clear all button</t>
+  </si>
+  <si>
+    <t>1. Enter "Đường Láng" into the Address
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter "^&amp;*" into the Address
+2. Click on Clear all button
+3. Enter HTML code: &lt;!DOCTYPE html&gt;&lt;html&gt;&lt;body&gt;&lt;h1&gt;Học lập trình HTML&lt;/h1&gt;&lt;/body&gt;&lt;/html&gt; into the Address
+4. Click on Clear all button
+5. Enter javascript: &lt;script src="myScript.js"&gt;&lt;/script&gt; into the Address
+6. Click on Clear all button
+7. Enter SQL injection: SELECT * FROM Users WHERE Username = 'Vanh' AND Password = '12345678' into the Address</t>
+  </si>
+  <si>
+    <t>1. Enter "12345678" into the Address
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter "Vanh1234" into the Address
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter "123$%^" into the Address</t>
+  </si>
+  <si>
+    <t>1. Enter "Vanh$%^" into the Address</t>
+  </si>
+  <si>
+    <t>1. Enter "Vanh1234%^&amp;" into the Address</t>
+  </si>
+  <si>
+    <t>1.Copy/Paste "abc123$%^" into the Address</t>
+  </si>
+  <si>
+    <t>1. Enter " Đường Láng " into the Address
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 4 characters into the Address</t>
+  </si>
+  <si>
+    <t>1. Enter 5 characters (valid Address) into the Address
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 6 characters (valid Address) into the Address
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 350 characters (valid Address) into the Address
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>1. Enter 351 characters into the Address</t>
+  </si>
+  <si>
+    <t>Check default value of Province</t>
+  </si>
+  <si>
+    <t>Check mandatory of Province</t>
+  </si>
+  <si>
+    <t>Check Province when the user enters from keyboard</t>
+  </si>
+  <si>
+    <t>1. Don't select any Province value
+2. Enter other fields are valid
+3. Click on "Save" button</t>
+  </si>
+  <si>
+    <t>There are 63 provinces of VN that sorted alphabetically
+There is a scrollbar when the list of Province exceeds the display frame</t>
+  </si>
+  <si>
+    <t>1. Paste value into Province
 2. Click on Province
 2. Select a Province
 3. Copy value
 4. Paste into other text fields</t>
   </si>
   <si>
-    <t>1. Enter character</t>
-  </si>
-  <si>
-    <t>1. Observe the display of the Province</t>
-  </si>
-  <si>
-    <t>1. Observe the display of the District</t>
-  </si>
-  <si>
-    <t>1. Select a Province
-2. Observe the display of the District</t>
-  </si>
-  <si>
-    <t xml:space="preserve">District is blank and disable
-The placeholder is "Please choose your District"
-</t>
-  </si>
-  <si>
-    <t>District is enable</t>
-  </si>
-  <si>
-    <t>There is a scrollbar when the list of District exceeds the display frame</t>
-  </si>
-  <si>
-    <t>System will show error message "Please select your District"</t>
-  </si>
-  <si>
-    <t>1. Click on District
-2. Select a District
-3. Enter other fields are valid
-4. Click on "Save" button</t>
-  </si>
-  <si>
-    <t>Do not allow paste, allow copy District</t>
-  </si>
-  <si>
-    <t>1. Paste value
+    <t>1. Enter character from keyboard</t>
+  </si>
+  <si>
+    <t>Check default value of District</t>
+  </si>
+  <si>
+    <t>Check mandatory of District</t>
+  </si>
+  <si>
+    <t>Value of Dropdown will be depended on Province value and sorted alphabetically.
+There is a scrollbar when the list of District exceeds the display frame.</t>
+  </si>
+  <si>
+    <t>1. Paste value into District
 2. Click on District
 2. Select a District
 3. Copy value
 4. Paste into other text fields</t>
   </si>
   <si>
-    <t>1. Click on District
-2. Observe the display of dropdown list</t>
-  </si>
-  <si>
-    <t>1.Copy/Paste "abc123$%^"</t>
-  </si>
-  <si>
-    <t>Allow Copy/Paste only numeric characters</t>
-  </si>
-  <si>
-    <t>1. Observe the display of the Ward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ward is blank and disable
-The placeholder is "Please choose your Ward"
-</t>
-  </si>
-  <si>
-    <t>Ward is enable</t>
-  </si>
-  <si>
-    <t>1. Click on Ward
-2. Observe the display of dropdown list</t>
-  </si>
-  <si>
-    <t>1. Click on Ward</t>
-  </si>
-  <si>
-    <t>There is a scrollbar when the list of Ward exceeds the display frame</t>
-  </si>
-  <si>
-    <t>System will show error message "Please select your Ward"</t>
-  </si>
-  <si>
-    <t>1. Click on Ward
-2. Select a Ward
-3. Enter other fields are valid
-4. Click on "Save" button</t>
-  </si>
-  <si>
-    <t>1. Paste value
+    <t>Check default value of Ward</t>
+  </si>
+  <si>
+    <t>Check mandatory  of Ward</t>
+  </si>
+  <si>
+    <t>Value of Dropdown will be depended on District value and sorted alphabetically
+There is a scrollbar when the list of Ward exceeds the display frame</t>
+  </si>
+  <si>
+    <t>Check dropdown list and scrollbar of Province</t>
+  </si>
+  <si>
+    <t>Check dropdown list and scrollbar of District</t>
+  </si>
+  <si>
+    <t>Check dropdown list and scrollbar of Ward</t>
+  </si>
+  <si>
+    <t>1. Paste value into the Ward
 2. Click on Ward
 2. Select a Ward
 3. Copy value
 4. Paste into other text fields</t>
   </si>
   <si>
-    <t>Do not allow paste, allow copy Ward</t>
-  </si>
-  <si>
-    <t>1. Select a District
-2. Observe the display of the Ward</t>
-  </si>
-  <si>
-    <t>Value of Dropdown will be depended on Province value and sorted alphabetically</t>
-  </si>
-  <si>
-    <t>Value of Dropdown will be depended on District value and sorted alphabetically</t>
-  </si>
-  <si>
-    <t>1. Observe the display of the Home button</t>
-  </si>
-  <si>
-    <t>Home button is enable and unchecked</t>
-  </si>
-  <si>
-    <t>Icon on Home button is gray</t>
-  </si>
-  <si>
-    <t>1. Don’t click on Home button
-2. Observe the display of the Home button</t>
+    <t>Check Home button when Home is in default status</t>
+  </si>
+  <si>
+    <t>Check Home button when Home is unchecked</t>
+  </si>
+  <si>
+    <t>Check Home button when Home is checked</t>
+  </si>
+  <si>
+    <t>Check Office button when Office is in default status</t>
+  </si>
+  <si>
+    <t>Check Office button when Office is unchecked</t>
+  </si>
+  <si>
+    <t>Check Office button when Office is checked</t>
+  </si>
+  <si>
+    <t>Check Home button when the user switches selection from Home to Office</t>
+  </si>
+  <si>
+    <t>Check Home button when the user switches selection from Office to Home</t>
   </si>
   <si>
     <t>1. Click on Home button
-2. Observe the display of Home button</t>
-  </si>
-  <si>
-    <t>Icon on Home button is hightlighted</t>
-  </si>
-  <si>
-    <t>1. Observe the display of the Office button</t>
-  </si>
-  <si>
-    <t>Office button is enable and unchecked</t>
-  </si>
-  <si>
-    <t>1. Don’t click on Office button
-2. Observe the display of the Office button</t>
-  </si>
-  <si>
-    <t>Icon on Office button is gray</t>
+2. Click on Office button
+3. Observe the display of Home button</t>
+  </si>
+  <si>
+    <t>Icon on Home button is not highlighted anymore</t>
+  </si>
+  <si>
+    <t>Icon on Office button is not highlighted anymore</t>
   </si>
   <si>
     <t>1. Click on Office button
-2. Observe the display of Office button</t>
-  </si>
-  <si>
-    <t>Icon on Office button is hightlighted</t>
-  </si>
-  <si>
-    <t>1. Enter all fields are valid
-2. Select Home button
-3. Click on Save button</t>
-  </si>
-  <si>
-    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book</t>
-  </si>
-  <si>
-    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book, automatic delete all leading, trailing spaces from Full Name</t>
-  </si>
-  <si>
-    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book, automatic delete all leading, trailing spaces from Address</t>
-  </si>
-  <si>
-    <t>Add new address as home successfully, return to Address book screen, new address will be displayed on the top of Address Book</t>
-  </si>
-  <si>
-    <t>Add new address as office successfully, return to Address book screen, new address will be displayed on the top of Address Book</t>
-  </si>
-  <si>
-    <t>1. Enter all fields are valid
-2. Select Office button
-3. Click on Save button</t>
-  </si>
-  <si>
-    <t>1. Enter all mandatory fields are valid
-2. Don't Select Office button/Home button
-3. Click on Save button</t>
-  </si>
-  <si>
-    <t>Add new address successfully, return to Address book screen, new address will be displayed on the top of Address Book
-Two button: Home and Office are displayed at the created address</t>
-  </si>
-  <si>
-    <t>1. Enter all fields are invalid
-2. Click on Save button</t>
-  </si>
-  <si>
-    <t>Add address fail, the system will display the corresponding error message below each field</t>
-  </si>
-  <si>
-    <t>1. Enter value into fields
-2. Click on Cancel button</t>
-  </si>
-  <si>
-    <t>Precondition: The user added 1 address
-1. Enter the value of all fields same previous address
-2. Click on Save button</t>
-  </si>
-  <si>
-    <t>Add address fail, return to Address book screen</t>
-  </si>
-  <si>
-    <t>When the user adds duplicate addresses</t>
-  </si>
-  <si>
-    <t>Precondition: The user added 1 address
-1. Enter Full Name and Phone number are same Previous address
-2. Enter other fields are different
-2. Click on Save button</t>
-  </si>
-  <si>
-    <t>When the user adds a new address completely different from the previous one</t>
-  </si>
-  <si>
-    <t>When the user adds a new address with the same consignee as the previous address</t>
-  </si>
-  <si>
-    <t>Precondition: The user added 1 address
-1. Enter the value of all fields are different previous address
-2. Click on Save button</t>
-  </si>
-  <si>
-    <t>1. Check Delete Address function</t>
-  </si>
-  <si>
-    <t>Verify that a confirmation pop-up is displayed when the user click on Delete icon</t>
-  </si>
-  <si>
-    <t>Delete address successfully when the user click on Delete button on pop-up</t>
-  </si>
-  <si>
-    <t>Delete address fail when the user click on Cancel button on pop-up</t>
-  </si>
-  <si>
-    <t>Verify that the user cannot delete default address</t>
-  </si>
-  <si>
-    <t>Show error message "You cannot delete your default address"</t>
-  </si>
-  <si>
-    <t>Delete address successfully, this address is not displayed in Address Book anymore</t>
-  </si>
-  <si>
-    <t>1. Select an address
-1. Click on Delete icon</t>
-  </si>
-  <si>
-    <t>1. Select an address that is not default address
-2. Click on Delete icon
-3. Click on Delete button on pop-up</t>
-  </si>
-  <si>
-    <t>1. Select an address
-2. Click on Delete icon
-3. Click on Delete button on pop-up</t>
-  </si>
-  <si>
-    <t>1. Select default address
-2. Click on Delete icon
-3. Click on Delete button on pop-up</t>
-  </si>
-  <si>
-    <t>1. Select an address
-2. Click on Delete icon
-3. Click on Cancel button on pop-up</t>
-  </si>
-  <si>
-    <t>Delete address fail, return to the Edit address screen</t>
-  </si>
-  <si>
-    <t>Delete address fail when the user click on Close (x) icon on pop-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A confirmation pop-up is displayed
-This pop up shows selected address information correctly </t>
+2. Click on Home button
+3. Observe the display of Home button</t>
   </si>
 </sst>
 </file>
@@ -3842,6 +4031,33 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3896,33 +4112,6 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4250,10 +4439,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" ht="14.25">
-      <c r="A1" s="152"/>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
+      <c r="A1" s="161"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -4262,13 +4451,13 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:24" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="154"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="163"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -4277,9 +4466,9 @@
     </row>
     <row r="3" spans="1:24" s="4" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="154"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="163"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -4290,11 +4479,11 @@
       <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="165"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -4308,9 +4497,9 @@
       <c r="A5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="157"/>
-      <c r="C5" s="158"/>
-      <c r="D5" s="158"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -4324,9 +4513,9 @@
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="157"/>
-      <c r="C6" s="158"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="166"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4337,11 +4526,11 @@
       <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="158" t="s">
+      <c r="B7" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="167"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -4353,9 +4542,9 @@
       <c r="A8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="159"/>
-      <c r="C8" s="159"/>
-      <c r="D8" s="159"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="168"/>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:24" s="12" customFormat="1">
@@ -4498,11 +4687,11 @@
       <c r="C16" s="17"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
-      <c r="F16" s="148" t="s">
+      <c r="F16" s="157" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="148"/>
-      <c r="H16" s="148"/>
+      <c r="G16" s="157"/>
+      <c r="H16" s="157"/>
       <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:16384" s="21" customFormat="1" ht="38.25">
@@ -4536,11 +4725,11 @@
     </row>
     <row r="18" spans="1:16384" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="22"/>
-      <c r="B18" s="149" t="s">
+      <c r="B18" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="150"/>
-      <c r="D18" s="151"/>
+      <c r="C18" s="159"/>
+      <c r="D18" s="160"/>
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
@@ -21389,11 +21578,11 @@
     </row>
     <row r="43" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A43" s="30"/>
-      <c r="B43" s="149" t="s">
+      <c r="B43" s="158" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="150"/>
-      <c r="D43" s="151"/>
+      <c r="C43" s="159"/>
+      <c r="D43" s="160"/>
       <c r="E43" s="31"/>
       <c r="F43" s="32"/>
       <c r="G43" s="32"/>
@@ -21788,10 +21977,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="14.25">
-      <c r="A1" s="152"/>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
+      <c r="A1" s="161"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
       <c r="E1" s="76"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -21799,13 +21988,13 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="163"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="172"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -21813,9 +22002,9 @@
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="164"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="173"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -21825,11 +22014,11 @@
       <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="165"/>
       <c r="E4" s="77"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -21840,9 +22029,9 @@
       <c r="A5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="157"/>
-      <c r="C5" s="158"/>
-      <c r="D5" s="158"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
       <c r="E5" s="77"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -21853,9 +22042,9 @@
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="157"/>
-      <c r="C6" s="158"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="166"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
       <c r="E6" s="77"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -21866,11 +22055,11 @@
       <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="158" t="s">
+      <c r="B7" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="167"/>
       <c r="E7" s="77"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -21881,9 +22070,9 @@
       <c r="A8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="159"/>
-      <c r="C8" s="159"/>
-      <c r="D8" s="159"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="168"/>
       <c r="E8" s="77"/>
       <c r="F8" s="56"/>
       <c r="G8" s="56"/>
@@ -22050,11 +22239,11 @@
       <c r="C16" s="58"/>
       <c r="D16" s="18"/>
       <c r="E16" s="80"/>
-      <c r="F16" s="148" t="s">
+      <c r="F16" s="157" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="148"/>
-      <c r="H16" s="148"/>
+      <c r="G16" s="157"/>
+      <c r="H16" s="157"/>
       <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" s="21" customFormat="1" ht="38.25">
@@ -22088,11 +22277,11 @@
     </row>
     <row r="18" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="59"/>
-      <c r="B18" s="160" t="s">
+      <c r="B18" s="169" t="s">
         <v>158</v>
       </c>
-      <c r="C18" s="161"/>
-      <c r="D18" s="162"/>
+      <c r="C18" s="170"/>
+      <c r="D18" s="171"/>
       <c r="E18" s="82"/>
       <c r="F18" s="60"/>
       <c r="G18" s="60"/>
@@ -23775,7 +23964,7 @@
         <v>326</v>
       </c>
       <c r="D103" s="107" t="s">
-        <v>529</v>
+        <v>501</v>
       </c>
       <c r="E103" s="84"/>
       <c r="F103" s="1"/>
@@ -24071,11 +24260,11 @@
     </row>
     <row r="119" spans="1:26" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A119" s="68"/>
-      <c r="B119" s="160" t="s">
+      <c r="B119" s="169" t="s">
         <v>210</v>
       </c>
-      <c r="C119" s="161"/>
-      <c r="D119" s="162"/>
+      <c r="C119" s="170"/>
+      <c r="D119" s="171"/>
       <c r="E119" s="86"/>
       <c r="F119" s="32"/>
       <c r="G119" s="32"/>
@@ -26949,10 +27138,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" ht="14.25">
-      <c r="A1" s="152"/>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
+      <c r="A1" s="161"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
       <c r="E1" s="119"/>
       <c r="F1" s="119"/>
       <c r="G1" s="119"/>
@@ -26961,13 +27150,13 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:24" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="166"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="175"/>
       <c r="F2" s="120"/>
       <c r="G2" s="120"/>
       <c r="H2" s="120"/>
@@ -26976,9 +27165,9 @@
     </row>
     <row r="3" spans="1:24" s="4" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="166"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="175"/>
       <c r="F3" s="120"/>
       <c r="G3" s="120"/>
       <c r="H3" s="120"/>
@@ -26989,11 +27178,11 @@
       <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="165"/>
       <c r="E4" s="121"/>
       <c r="F4" s="121"/>
       <c r="G4" s="121"/>
@@ -27007,9 +27196,9 @@
       <c r="A5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="157"/>
-      <c r="C5" s="158"/>
-      <c r="D5" s="158"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
       <c r="E5" s="121"/>
       <c r="F5" s="121"/>
       <c r="G5" s="121"/>
@@ -27023,9 +27212,9 @@
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="157"/>
-      <c r="C6" s="158"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="166"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
       <c r="E6" s="121"/>
       <c r="F6" s="121"/>
       <c r="G6" s="121"/>
@@ -27036,11 +27225,11 @@
       <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="158" t="s">
+      <c r="B7" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="167"/>
       <c r="E7" s="121"/>
       <c r="F7" s="121"/>
       <c r="G7" s="121"/>
@@ -27052,9 +27241,9 @@
       <c r="A8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="159"/>
-      <c r="C8" s="159"/>
-      <c r="D8" s="159"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="168"/>
       <c r="E8" s="121"/>
       <c r="F8" s="124"/>
       <c r="G8" s="124"/>
@@ -27221,11 +27410,11 @@
       <c r="C16" s="92"/>
       <c r="D16" s="18"/>
       <c r="E16" s="126"/>
-      <c r="F16" s="165" t="s">
+      <c r="F16" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="165"/>
-      <c r="H16" s="165"/>
+      <c r="G16" s="174"/>
+      <c r="H16" s="174"/>
       <c r="I16" s="127"/>
     </row>
     <row r="17" spans="1:9" s="21" customFormat="1" ht="38.25">
@@ -27259,11 +27448,11 @@
     </row>
     <row r="18" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="22"/>
-      <c r="B18" s="149" t="s">
+      <c r="B18" s="158" t="s">
         <v>221</v>
       </c>
-      <c r="C18" s="150"/>
-      <c r="D18" s="151"/>
+      <c r="C18" s="159"/>
+      <c r="D18" s="160"/>
       <c r="E18" s="129"/>
       <c r="F18" s="130"/>
       <c r="G18" s="130"/>
@@ -27291,11 +27480,11 @@
     </row>
     <row r="20" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="22"/>
-      <c r="B20" s="149" t="s">
+      <c r="B20" s="158" t="s">
         <v>222</v>
       </c>
-      <c r="C20" s="150"/>
-      <c r="D20" s="151"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="160"/>
       <c r="E20" s="129"/>
       <c r="F20" s="130"/>
       <c r="G20" s="130"/>
@@ -30857,17 +31046,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I982"/>
+  <dimension ref="A1:I981"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111:C112"/>
+    <sheetView showGridLines="0" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="36" customWidth="1"/>
     <col min="2" max="2" width="61.42578125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" style="175" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" style="156" customWidth="1"/>
     <col min="4" max="4" width="39.7109375" style="37" customWidth="1"/>
     <col min="5" max="5" width="32.140625" style="147" customWidth="1"/>
     <col min="6" max="6" width="13" style="37" customWidth="1"/>
@@ -30877,10 +31066,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="14.25">
-      <c r="A1" s="152"/>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
+      <c r="A1" s="161"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
       <c r="E1" s="76"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -30888,13 +31077,13 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="163"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="172"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -30902,9 +31091,9 @@
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="164"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="173"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -30914,11 +31103,11 @@
       <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="165"/>
       <c r="E4" s="77"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -30929,9 +31118,9 @@
       <c r="A5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="157"/>
-      <c r="C5" s="158"/>
-      <c r="D5" s="158"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
       <c r="E5" s="77"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -30942,11 +31131,11 @@
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="157" t="s">
-        <v>516</v>
-      </c>
-      <c r="C6" s="158"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="166" t="s">
+        <v>496</v>
+      </c>
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
       <c r="E6" s="77"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -30957,11 +31146,11 @@
       <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="158" t="s">
+      <c r="B7" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="167"/>
       <c r="E7" s="77"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -30972,9 +31161,9 @@
       <c r="A8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="159"/>
-      <c r="C8" s="159"/>
-      <c r="D8" s="159"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="168"/>
       <c r="E8" s="77"/>
       <c r="F8" s="56"/>
       <c r="G8" s="56"/>
@@ -30989,7 +31178,7 @@
         <f>F17</f>
         <v>Internal Build 03112011</v>
       </c>
-      <c r="C9" s="167" t="str">
+      <c r="C9" s="148" t="str">
         <f>G17</f>
         <v>Internal build 14112011</v>
       </c>
@@ -31011,7 +31200,7 @@
         <f>SUM(B11:B14)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="170">
+      <c r="C10" s="151">
         <f>SUM(C11:C14)</f>
         <v>0</v>
       </c>
@@ -31030,15 +31219,15 @@
         <v>13</v>
       </c>
       <c r="B11" s="15">
-        <f>COUNTIF($F$18:$F$107,"*Passed")</f>
+        <f>COUNTIF($F$18:$F$106,"*Passed")</f>
         <v>0</v>
       </c>
-      <c r="C11" s="171">
-        <f>COUNTIF($G$18:$G$107,"*Passed")</f>
+      <c r="C11" s="152">
+        <f>COUNTIF($G$18:$G$106,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="D11" s="15">
-        <f>COUNTIF($H$18:$H$107,"*Passed")</f>
+        <f>COUNTIF($H$18:$H$106,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="E11" s="78"/>
@@ -31052,15 +31241,15 @@
         <v>14</v>
       </c>
       <c r="B12" s="15">
-        <f>COUNTIF($F$18:$F$107,"*Failed*")</f>
+        <f>COUNTIF($F$18:$F$106,"*Failed*")</f>
         <v>0</v>
       </c>
-      <c r="C12" s="171">
-        <f>COUNTIF($G$18:$G$107,"*Failed*")</f>
+      <c r="C12" s="152">
+        <f>COUNTIF($G$18:$G$106,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="D12" s="15">
-        <f>COUNTIF($H$18:$H$107,"*Failed*")</f>
+        <f>COUNTIF($H$18:$H$106,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="E12" s="78"/>
@@ -31074,15 +31263,15 @@
         <v>15</v>
       </c>
       <c r="B13" s="15">
-        <f>COUNTIF($F$18:$F$107,"*Not Run*")</f>
+        <f>COUNTIF($F$18:$F$106,"*Not Run*")</f>
         <v>0</v>
       </c>
-      <c r="C13" s="171">
-        <f>COUNTIF($G$18:$G$107,"*Not Run*")</f>
+      <c r="C13" s="152">
+        <f>COUNTIF($G$18:$G$106,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="D13" s="15">
-        <f>COUNTIF($H$18:$H$107,"*Not Run*")</f>
+        <f>COUNTIF($H$18:$H$106,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="E13" s="79"/>
@@ -31096,15 +31285,15 @@
         <v>16</v>
       </c>
       <c r="B14" s="15">
-        <f>COUNTIF($F$18:$F$107,"*NA*")</f>
+        <f>COUNTIF($F$18:$F$106,"*NA*")</f>
         <v>0</v>
       </c>
-      <c r="C14" s="171">
-        <f>COUNTIF($G$18:$G$107,"*NA*")</f>
+      <c r="C14" s="152">
+        <f>COUNTIF($G$18:$G$106,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="D14" s="15">
-        <f>COUNTIF($H$18:$H$107,"*NA*")</f>
+        <f>COUNTIF($H$18:$H$106,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="E14" s="79"/>
@@ -31118,15 +31307,15 @@
         <v>17</v>
       </c>
       <c r="B15" s="15">
-        <f>COUNTIF($F$18:$F$107,"*Passed in previous build*")</f>
+        <f>COUNTIF($F$18:$F$106,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
-      <c r="C15" s="171">
-        <f>COUNTIF($G$18:$G$107,"*Passed in previous build*")</f>
+      <c r="C15" s="152">
+        <f>COUNTIF($G$18:$G$106,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="D15" s="15">
-        <f>COUNTIF($H$18:$H$107,"*Passed in previous build*")</f>
+        <f>COUNTIF($H$18:$H$106,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="E15" s="79"/>
@@ -31138,14 +31327,14 @@
     <row r="16" spans="1:9" s="21" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="57"/>
       <c r="B16" s="58"/>
-      <c r="C16" s="172"/>
+      <c r="C16" s="153"/>
       <c r="D16" s="18"/>
       <c r="E16" s="80"/>
-      <c r="F16" s="148" t="s">
+      <c r="F16" s="157" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="148"/>
-      <c r="H16" s="148"/>
+      <c r="G16" s="157"/>
+      <c r="H16" s="157"/>
       <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" s="21" customFormat="1" ht="38.25">
@@ -31155,7 +31344,7 @@
       <c r="B17" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="168" t="s">
+      <c r="C17" s="149" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="42" t="s">
@@ -31179,11 +31368,11 @@
     </row>
     <row r="18" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="59"/>
-      <c r="B18" s="160" t="s">
+      <c r="B18" s="169" t="s">
         <v>476</v>
       </c>
-      <c r="C18" s="161"/>
-      <c r="D18" s="162"/>
+      <c r="C18" s="170"/>
+      <c r="D18" s="171"/>
       <c r="E18" s="82"/>
       <c r="F18" s="60"/>
       <c r="G18" s="60"/>
@@ -31195,7 +31384,7 @@
       <c r="B19" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="C19" s="169"/>
+      <c r="C19" s="150"/>
       <c r="D19" s="62"/>
       <c r="E19" s="83"/>
       <c r="F19" s="64"/>
@@ -31209,13 +31398,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="C20" s="173" t="s">
-        <v>517</v>
+        <v>591</v>
+      </c>
+      <c r="C20" s="154" t="s">
+        <v>497</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>519</v>
+        <v>498</v>
       </c>
       <c r="E20" s="84"/>
       <c r="F20" s="1"/>
@@ -31229,13 +31418,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="C21" s="173" t="s">
-        <v>518</v>
+        <v>592</v>
+      </c>
+      <c r="C21" s="154" t="s">
+        <v>593</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>521</v>
+        <v>499</v>
       </c>
       <c r="E21" s="84"/>
       <c r="F21" s="1"/>
@@ -31249,10 +31438,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C22" s="173" t="s">
-        <v>539</v>
+        <v>597</v>
+      </c>
+      <c r="C22" s="154" t="s">
+        <v>594</v>
       </c>
       <c r="D22" s="70" t="s">
         <v>253</v>
@@ -31269,13 +31458,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C23" s="173" t="s">
-        <v>520</v>
+        <v>598</v>
+      </c>
+      <c r="C23" s="154" t="s">
+        <v>595</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E23" s="84"/>
       <c r="F23" s="1"/>
@@ -31283,22 +31472,22 @@
       <c r="H23" s="1"/>
       <c r="I23" s="26"/>
     </row>
-    <row r="24" spans="1:9" s="27" customFormat="1" ht="127.5">
+    <row r="24" spans="1:9" s="27" customFormat="1" ht="153">
       <c r="A24" s="65">
         <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C24" s="173" t="s">
-        <v>522</v>
+        <v>599</v>
+      </c>
+      <c r="C24" s="154" t="s">
+        <v>596</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>523</v>
+        <v>586</v>
       </c>
       <c r="E24" s="84" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -31311,13 +31500,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C25" s="173" t="s">
-        <v>524</v>
+        <v>600</v>
+      </c>
+      <c r="C25" s="154" t="s">
+        <v>610</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E25" s="84"/>
       <c r="F25" s="1"/>
@@ -31331,13 +31520,13 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C26" s="173" t="s">
-        <v>525</v>
+        <v>601</v>
+      </c>
+      <c r="C26" s="154" t="s">
+        <v>611</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E26" s="84"/>
       <c r="F26" s="1"/>
@@ -31351,13 +31540,13 @@
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C27" s="173" t="s">
-        <v>526</v>
+        <v>602</v>
+      </c>
+      <c r="C27" s="154" t="s">
+        <v>612</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>523</v>
+        <v>500</v>
       </c>
       <c r="E27" s="84"/>
       <c r="F27" s="1"/>
@@ -31371,13 +31560,13 @@
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C28" s="173" t="s">
-        <v>527</v>
+        <v>603</v>
+      </c>
+      <c r="C28" s="154" t="s">
+        <v>613</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>523</v>
+        <v>500</v>
       </c>
       <c r="E28" s="84"/>
       <c r="F28" s="1"/>
@@ -31391,13 +31580,13 @@
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C29" s="173" t="s">
-        <v>528</v>
+        <v>604</v>
+      </c>
+      <c r="C29" s="154" t="s">
+        <v>614</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>523</v>
+        <v>500</v>
       </c>
       <c r="E29" s="84"/>
       <c r="F29" s="1"/>
@@ -31413,11 +31602,11 @@
       <c r="B30" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C30" s="173" t="s">
-        <v>591</v>
+      <c r="C30" s="154" t="s">
+        <v>615</v>
       </c>
       <c r="D30" s="107" t="s">
-        <v>529</v>
+        <v>501</v>
       </c>
       <c r="E30" s="84"/>
       <c r="F30" s="1"/>
@@ -31431,13 +31620,13 @@
         <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C31" s="173" t="s">
-        <v>530</v>
+        <v>622</v>
+      </c>
+      <c r="C31" s="154" t="s">
+        <v>616</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>620</v>
+        <v>553</v>
       </c>
       <c r="E31" s="84"/>
       <c r="F31" s="1"/>
@@ -31451,13 +31640,13 @@
         <v>13</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="C32" s="173" t="s">
-        <v>562</v>
+        <v>605</v>
+      </c>
+      <c r="C32" s="154" t="s">
+        <v>617</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>531</v>
+        <v>502</v>
       </c>
       <c r="E32" s="84"/>
       <c r="F32" s="1"/>
@@ -31471,13 +31660,13 @@
         <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="C33" s="173" t="s">
-        <v>532</v>
+        <v>606</v>
+      </c>
+      <c r="C33" s="154" t="s">
+        <v>618</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E33" s="84"/>
       <c r="F33" s="1"/>
@@ -31491,13 +31680,13 @@
         <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="C34" s="173" t="s">
-        <v>533</v>
+        <v>607</v>
+      </c>
+      <c r="C34" s="154" t="s">
+        <v>619</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E34" s="84"/>
       <c r="F34" s="1"/>
@@ -31511,13 +31700,13 @@
         <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C35" s="173" t="s">
-        <v>534</v>
+        <v>608</v>
+      </c>
+      <c r="C35" s="154" t="s">
+        <v>620</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E35" s="84"/>
       <c r="F35" s="1"/>
@@ -31531,13 +31720,13 @@
         <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C36" s="173" t="s">
-        <v>563</v>
+        <v>609</v>
+      </c>
+      <c r="C36" s="154" t="s">
+        <v>621</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>536</v>
+        <v>504</v>
       </c>
       <c r="E36" s="84"/>
       <c r="F36" s="1"/>
@@ -31550,7 +31739,7 @@
       <c r="B37" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="C37" s="169"/>
+      <c r="C37" s="150"/>
       <c r="D37" s="62"/>
       <c r="E37" s="83"/>
       <c r="F37" s="64"/>
@@ -31560,17 +31749,17 @@
     </row>
     <row r="38" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A38" s="65">
-        <f t="shared" ref="A38:A92" ca="1" si="2">IF(OFFSET(A38,-1,0) ="",OFFSET(A38,-2,0)+1,OFFSET(A38,-1,0)+1 )</f>
+        <f t="shared" ref="A38:A89" ca="1" si="2">IF(OFFSET(A38,-1,0) ="",OFFSET(A38,-2,0)+1,OFFSET(A38,-1,0)+1 )</f>
         <v>18</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="C38" s="173" t="s">
-        <v>535</v>
+        <v>630</v>
+      </c>
+      <c r="C38" s="154" t="s">
+        <v>503</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>538</v>
+        <v>506</v>
       </c>
       <c r="E38" s="84"/>
       <c r="F38" s="1"/>
@@ -31584,13 +31773,13 @@
         <v>19</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="C39" s="173" t="s">
-        <v>518</v>
+        <v>631</v>
+      </c>
+      <c r="C39" s="154" t="s">
+        <v>633</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>537</v>
+        <v>505</v>
       </c>
       <c r="E39" s="107"/>
       <c r="F39" s="107"/>
@@ -31604,10 +31793,10 @@
         <v>20</v>
       </c>
       <c r="B40" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="C40" s="173" t="s">
-        <v>539</v>
+        <v>623</v>
+      </c>
+      <c r="C40" s="154" t="s">
+        <v>634</v>
       </c>
       <c r="D40" s="70" t="s">
         <v>253</v>
@@ -31624,10 +31813,10 @@
         <v>21</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C41" s="173" t="s">
-        <v>546</v>
+        <v>624</v>
+      </c>
+      <c r="C41" s="154" t="s">
+        <v>635</v>
       </c>
       <c r="D41" s="103" t="s">
         <v>259</v>
@@ -31638,22 +31827,22 @@
       <c r="H41" s="1"/>
       <c r="I41" s="26"/>
     </row>
-    <row r="42" spans="1:9" s="27" customFormat="1" ht="89.25">
+    <row r="42" spans="1:9" s="27" customFormat="1" ht="114.75">
       <c r="A42" s="65">
         <f t="shared" ca="1" si="2"/>
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C42" s="173" t="s">
-        <v>540</v>
+        <v>625</v>
+      </c>
+      <c r="C42" s="154" t="s">
+        <v>636</v>
       </c>
       <c r="D42" s="96" t="s">
         <v>260</v>
       </c>
       <c r="E42" s="84" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -31666,10 +31855,10 @@
         <v>23</v>
       </c>
       <c r="B43" s="101" t="s">
-        <v>165</v>
-      </c>
-      <c r="C43" s="173" t="s">
-        <v>547</v>
+        <v>626</v>
+      </c>
+      <c r="C43" s="154" t="s">
+        <v>637</v>
       </c>
       <c r="D43" s="107" t="s">
         <v>364</v>
@@ -31680,7 +31869,7 @@
       <c r="H43" s="101"/>
       <c r="I43" s="109"/>
     </row>
-    <row r="44" spans="1:9" s="27" customFormat="1" ht="12.75">
+    <row r="44" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A44" s="65">
         <f t="shared" ca="1" si="2"/>
         <v>24</v>
@@ -31688,11 +31877,11 @@
       <c r="B44" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C44" s="173" t="s">
-        <v>591</v>
+      <c r="C44" s="154" t="s">
+        <v>638</v>
       </c>
       <c r="D44" s="107" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="E44" s="85"/>
       <c r="F44" s="1"/>
@@ -31706,10 +31895,10 @@
         <v>25</v>
       </c>
       <c r="B45" s="115" t="s">
-        <v>169</v>
-      </c>
-      <c r="C45" s="174" t="s">
-        <v>542</v>
+        <v>632</v>
+      </c>
+      <c r="C45" s="155" t="s">
+        <v>639</v>
       </c>
       <c r="D45" s="103" t="s">
         <v>265</v>
@@ -31726,13 +31915,13 @@
         <v>26</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C46" s="173" t="s">
-        <v>544</v>
+        <v>627</v>
+      </c>
+      <c r="C46" s="154" t="s">
+        <v>640</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>543</v>
+        <v>507</v>
       </c>
       <c r="E46" s="85"/>
       <c r="F46" s="1"/>
@@ -31746,13 +31935,13 @@
         <v>27</v>
       </c>
       <c r="B47" s="101" t="s">
-        <v>485</v>
-      </c>
-      <c r="C47" s="173" t="s">
-        <v>541</v>
+        <v>628</v>
+      </c>
+      <c r="C47" s="154" t="s">
+        <v>641</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E47" s="103"/>
       <c r="F47" s="101"/>
@@ -31766,13 +31955,13 @@
         <v>28</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C48" s="173" t="s">
-        <v>545</v>
+        <v>629</v>
+      </c>
+      <c r="C48" s="154" t="s">
+        <v>642</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>543</v>
+        <v>507</v>
       </c>
       <c r="E48" s="85"/>
       <c r="F48" s="1"/>
@@ -31785,7 +31974,7 @@
       <c r="B49" s="53" t="s">
         <v>477</v>
       </c>
-      <c r="C49" s="169"/>
+      <c r="C49" s="150"/>
       <c r="D49" s="62"/>
       <c r="E49" s="83"/>
       <c r="F49" s="64"/>
@@ -31799,13 +31988,13 @@
         <v>29</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="C50" s="173" t="s">
-        <v>548</v>
+        <v>643</v>
+      </c>
+      <c r="C50" s="154" t="s">
+        <v>508</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>551</v>
+        <v>511</v>
       </c>
       <c r="E50" s="84"/>
       <c r="F50" s="1"/>
@@ -31819,13 +32008,13 @@
         <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="C51" s="173" t="s">
-        <v>518</v>
+        <v>644</v>
+      </c>
+      <c r="C51" s="154" t="s">
+        <v>659</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>549</v>
+        <v>509</v>
       </c>
       <c r="E51" s="84"/>
       <c r="F51" s="1"/>
@@ -31839,10 +32028,10 @@
         <v>31</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C52" s="173" t="s">
-        <v>539</v>
+        <v>646</v>
+      </c>
+      <c r="C52" s="154" t="s">
+        <v>660</v>
       </c>
       <c r="D52" s="70" t="s">
         <v>253</v>
@@ -31859,13 +32048,13 @@
         <v>32</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C53" s="173" t="s">
+        <v>647</v>
+      </c>
+      <c r="C53" s="154" t="s">
+        <v>661</v>
+      </c>
+      <c r="D53" s="24" t="s">
         <v>552</v>
-      </c>
-      <c r="D53" s="24" t="s">
-        <v>619</v>
       </c>
       <c r="E53" s="84"/>
       <c r="F53" s="1"/>
@@ -31873,22 +32062,22 @@
       <c r="H53" s="1"/>
       <c r="I53" s="26"/>
     </row>
-    <row r="54" spans="1:9" s="27" customFormat="1" ht="127.5">
+    <row r="54" spans="1:9" s="27" customFormat="1" ht="153">
       <c r="A54" s="65">
         <f t="shared" ca="1" si="4"/>
         <v>33</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C54" s="173" t="s">
-        <v>522</v>
+        <v>648</v>
+      </c>
+      <c r="C54" s="154" t="s">
+        <v>662</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>553</v>
+        <v>586</v>
       </c>
       <c r="E54" s="84" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -31901,13 +32090,13 @@
         <v>34</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C55" s="173" t="s">
-        <v>524</v>
+        <v>649</v>
+      </c>
+      <c r="C55" s="154" t="s">
+        <v>663</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E55" s="84"/>
       <c r="F55" s="1"/>
@@ -31921,13 +32110,13 @@
         <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C56" s="173" t="s">
-        <v>525</v>
+        <v>650</v>
+      </c>
+      <c r="C56" s="154" t="s">
+        <v>664</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E56" s="84"/>
       <c r="F56" s="1"/>
@@ -31941,13 +32130,13 @@
         <v>36</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C57" s="173" t="s">
-        <v>526</v>
+        <v>651</v>
+      </c>
+      <c r="C57" s="154" t="s">
+        <v>665</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>553</v>
+        <v>512</v>
       </c>
       <c r="E57" s="84"/>
       <c r="F57" s="1"/>
@@ -31961,13 +32150,13 @@
         <v>37</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C58" s="173" t="s">
-        <v>527</v>
+        <v>652</v>
+      </c>
+      <c r="C58" s="154" t="s">
+        <v>666</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>553</v>
+        <v>512</v>
       </c>
       <c r="E58" s="84"/>
       <c r="F58" s="1"/>
@@ -31981,13 +32170,13 @@
         <v>38</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C59" s="173" t="s">
-        <v>528</v>
+        <v>653</v>
+      </c>
+      <c r="C59" s="154" t="s">
+        <v>667</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>553</v>
+        <v>512</v>
       </c>
       <c r="E59" s="84"/>
       <c r="F59" s="1"/>
@@ -32001,13 +32190,13 @@
         <v>39</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="C60" s="173" t="s">
-        <v>591</v>
+        <v>482</v>
+      </c>
+      <c r="C60" s="154" t="s">
+        <v>668</v>
       </c>
       <c r="D60" s="107" t="s">
-        <v>550</v>
+        <v>510</v>
       </c>
       <c r="E60" s="84"/>
       <c r="F60" s="1"/>
@@ -32021,13 +32210,13 @@
         <v>40</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C61" s="173" t="s">
+        <v>645</v>
+      </c>
+      <c r="C61" s="154" t="s">
+        <v>669</v>
+      </c>
+      <c r="D61" s="24" t="s">
         <v>554</v>
-      </c>
-      <c r="D61" s="24" t="s">
-        <v>621</v>
       </c>
       <c r="E61" s="84"/>
       <c r="F61" s="1"/>
@@ -32041,13 +32230,13 @@
         <v>41</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="C62" s="173" t="s">
-        <v>560</v>
+        <v>654</v>
+      </c>
+      <c r="C62" s="154" t="s">
+        <v>670</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>555</v>
+        <v>513</v>
       </c>
       <c r="E62" s="84"/>
       <c r="F62" s="1"/>
@@ -32061,13 +32250,13 @@
         <v>42</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="C63" s="173" t="s">
-        <v>557</v>
+        <v>655</v>
+      </c>
+      <c r="C63" s="154" t="s">
+        <v>671</v>
       </c>
       <c r="D63" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E63" s="84"/>
       <c r="F63" s="1"/>
@@ -32081,13 +32270,13 @@
         <v>43</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="C64" s="173" t="s">
-        <v>558</v>
+        <v>656</v>
+      </c>
+      <c r="C64" s="154" t="s">
+        <v>672</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E64" s="84"/>
       <c r="F64" s="1"/>
@@ -32101,13 +32290,13 @@
         <v>44</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="C65" s="173" t="s">
-        <v>559</v>
+        <v>657</v>
+      </c>
+      <c r="C65" s="154" t="s">
+        <v>673</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E65" s="84"/>
       <c r="F65" s="1"/>
@@ -32121,13 +32310,13 @@
         <v>45</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="C66" s="173" t="s">
-        <v>561</v>
+        <v>658</v>
+      </c>
+      <c r="C66" s="154" t="s">
+        <v>674</v>
       </c>
       <c r="D66" s="24" t="s">
-        <v>556</v>
+        <v>514</v>
       </c>
       <c r="E66" s="84"/>
       <c r="F66" s="1"/>
@@ -32140,7 +32329,7 @@
       <c r="B67" s="53" t="s">
         <v>478</v>
       </c>
-      <c r="C67" s="169"/>
+      <c r="C67" s="150"/>
       <c r="D67" s="62"/>
       <c r="E67" s="83"/>
       <c r="F67" s="64"/>
@@ -32154,13 +32343,13 @@
         <v>46</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="C68" s="173" t="s">
-        <v>580</v>
+        <v>675</v>
+      </c>
+      <c r="C68" s="154" t="s">
+        <v>524</v>
       </c>
       <c r="D68" s="24" t="s">
-        <v>565</v>
+        <v>516</v>
       </c>
       <c r="E68" s="84"/>
       <c r="F68" s="1"/>
@@ -32168,60 +32357,59 @@
       <c r="H68" s="1"/>
       <c r="I68" s="26"/>
     </row>
-    <row r="69" spans="1:9" s="27" customFormat="1" ht="25.5">
+    <row r="69" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A69" s="65">
         <f ca="1">IF(OFFSET(A69,-1,0) ="",OFFSET(A69,-2,0)+1,OFFSET(A69,-1,0)+1 )</f>
         <v>47</v>
       </c>
-      <c r="B69" s="101" t="s">
-        <v>198</v>
-      </c>
-      <c r="C69" s="173" t="s">
-        <v>571</v>
-      </c>
-      <c r="D69" s="102" t="s">
-        <v>568</v>
-      </c>
-      <c r="E69" s="84" t="s">
-        <v>566</v>
-      </c>
+      <c r="B69" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="C69" s="154" t="s">
+        <v>678</v>
+      </c>
+      <c r="D69" s="24" t="s">
+        <v>515</v>
+      </c>
+      <c r="E69" s="84"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="26"/>
     </row>
-    <row r="70" spans="1:9" s="27" customFormat="1" ht="25.5">
+    <row r="70" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A70" s="65">
-        <f t="shared" ref="A70:A71" ca="1" si="5">IF(OFFSET(A70,-1,0) ="",OFFSET(A70,-2,0)+1,OFFSET(A70,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A70,-1,0) ="",OFFSET(A70,-2,0)+1,OFFSET(A70,-1,0)+1 )</f>
         <v>48</v>
       </c>
-      <c r="B70" s="54" t="s">
-        <v>493</v>
-      </c>
-      <c r="C70" s="173" t="s">
-        <v>570</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>567</v>
-      </c>
+      <c r="B70" s="101" t="s">
+        <v>689</v>
+      </c>
+      <c r="C70" s="154" t="s">
+        <v>518</v>
+      </c>
+      <c r="D70" s="102" t="s">
+        <v>679</v>
+      </c>
+      <c r="E70" s="84"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="26"/>
     </row>
-    <row r="71" spans="1:9" s="27" customFormat="1" ht="38.25">
+    <row r="71" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A71" s="65">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="2"/>
         <v>49</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="C71" s="173" t="s">
-        <v>573</v>
+      <c r="B71" s="101" t="s">
+        <v>483</v>
+      </c>
+      <c r="C71" s="154" t="s">
+        <v>520</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>564</v>
+        <v>552</v>
       </c>
       <c r="E71" s="84"/>
       <c r="F71" s="1"/>
@@ -32229,19 +32417,19 @@
       <c r="H71" s="1"/>
       <c r="I71" s="26"/>
     </row>
-    <row r="72" spans="1:9" s="27" customFormat="1" ht="51">
+    <row r="72" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A72" s="65">
         <f t="shared" ca="1" si="2"/>
         <v>50</v>
       </c>
-      <c r="B72" s="101" t="s">
-        <v>492</v>
-      </c>
-      <c r="C72" s="173" t="s">
-        <v>574</v>
-      </c>
-      <c r="D72" s="24" t="s">
-        <v>619</v>
+      <c r="B72" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C72" s="154" t="s">
+        <v>680</v>
+      </c>
+      <c r="D72" s="101" t="s">
+        <v>517</v>
       </c>
       <c r="E72" s="84"/>
       <c r="F72" s="1"/>
@@ -32249,19 +32437,19 @@
       <c r="H72" s="1"/>
       <c r="I72" s="26"/>
     </row>
-    <row r="73" spans="1:9" s="27" customFormat="1" ht="63.75">
+    <row r="73" spans="1:9" s="27" customFormat="1" ht="12.75">
       <c r="A73" s="65">
         <f t="shared" ca="1" si="2"/>
         <v>51</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="C73" s="173" t="s">
-        <v>578</v>
+      <c r="B73" s="112" t="s">
+        <v>677</v>
+      </c>
+      <c r="C73" s="154" t="s">
+        <v>681</v>
       </c>
       <c r="D73" s="101" t="s">
-        <v>569</v>
+        <v>312</v>
       </c>
       <c r="E73" s="84"/>
       <c r="F73" s="1"/>
@@ -32269,52 +32457,52 @@
       <c r="H73" s="1"/>
       <c r="I73" s="26"/>
     </row>
-    <row r="74" spans="1:9" s="27" customFormat="1" ht="12.75">
-      <c r="A74" s="65">
+    <row r="74" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A74" s="43"/>
+      <c r="B74" s="53" t="s">
+        <v>479</v>
+      </c>
+      <c r="C74" s="150"/>
+      <c r="D74" s="62"/>
+      <c r="E74" s="83"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="64"/>
+      <c r="H74" s="64"/>
+      <c r="I74" s="63"/>
+    </row>
+    <row r="75" spans="1:9" s="27" customFormat="1" ht="51">
+      <c r="A75" s="65">
         <f t="shared" ca="1" si="2"/>
         <v>52</v>
       </c>
-      <c r="B74" s="112" t="s">
-        <v>195</v>
-      </c>
-      <c r="C74" s="173" t="s">
-        <v>579</v>
-      </c>
-      <c r="D74" s="101" t="s">
-        <v>312</v>
-      </c>
-      <c r="E74" s="84"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="26"/>
-    </row>
-    <row r="75" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A75" s="43"/>
-      <c r="B75" s="53" t="s">
-        <v>479</v>
-      </c>
-      <c r="C75" s="169"/>
-      <c r="D75" s="62"/>
-      <c r="E75" s="83"/>
-      <c r="F75" s="64"/>
-      <c r="G75" s="64"/>
-      <c r="H75" s="64"/>
-      <c r="I75" s="63"/>
-    </row>
-    <row r="76" spans="1:9" s="27" customFormat="1" ht="51">
+      <c r="B75" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="C75" s="154" t="s">
+        <v>588</v>
+      </c>
+      <c r="D75" s="24" t="s">
+        <v>526</v>
+      </c>
+      <c r="E75" s="84"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="26"/>
+    </row>
+    <row r="76" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A76" s="65">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">IF(OFFSET(A76,-1,0) ="",OFFSET(A76,-2,0)+1,OFFSET(A76,-1,0)+1 )</f>
         <v>53</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="C76" s="173" t="s">
-        <v>581</v>
+        <v>683</v>
+      </c>
+      <c r="C76" s="154" t="s">
+        <v>519</v>
       </c>
       <c r="D76" s="24" t="s">
-        <v>583</v>
+        <v>528</v>
       </c>
       <c r="E76" s="84"/>
       <c r="F76" s="1"/>
@@ -32328,13 +32516,13 @@
         <v>54</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="C77" s="173" t="s">
-        <v>582</v>
+        <v>490</v>
+      </c>
+      <c r="C77" s="154" t="s">
+        <v>525</v>
       </c>
       <c r="D77" s="102" t="s">
-        <v>584</v>
+        <v>527</v>
       </c>
       <c r="E77" s="84"/>
       <c r="F77" s="1"/>
@@ -32342,38 +32530,38 @@
       <c r="H77" s="1"/>
       <c r="I77" s="26"/>
     </row>
-    <row r="78" spans="1:9" s="27" customFormat="1" ht="25.5">
+    <row r="78" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A78" s="65">
         <f ca="1">IF(OFFSET(A78,-1,0) ="",OFFSET(A78,-2,0)+1,OFFSET(A78,-1,0)+1 )</f>
         <v>55</v>
       </c>
       <c r="B78" s="101" t="s">
-        <v>198</v>
-      </c>
-      <c r="C78" s="173" t="s">
-        <v>590</v>
+        <v>690</v>
+      </c>
+      <c r="C78" s="154" t="s">
+        <v>531</v>
       </c>
       <c r="D78" s="84" t="s">
-        <v>604</v>
+        <v>684</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="26"/>
     </row>
-    <row r="79" spans="1:9" s="27" customFormat="1" ht="25.5">
+    <row r="79" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A79" s="65">
-        <f t="shared" ref="A79:A80" ca="1" si="6">IF(OFFSET(A79,-1,0) ="",OFFSET(A79,-2,0)+1,OFFSET(A79,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>56</v>
       </c>
-      <c r="B79" s="54" t="s">
-        <v>495</v>
-      </c>
-      <c r="C79" s="173" t="s">
-        <v>572</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>585</v>
+      <c r="B79" s="101" t="s">
+        <v>484</v>
+      </c>
+      <c r="C79" s="154" t="s">
+        <v>529</v>
+      </c>
+      <c r="D79" s="24" t="s">
+        <v>552</v>
       </c>
       <c r="E79" s="84"/>
       <c r="F79" s="1"/>
@@ -32381,19 +32569,19 @@
       <c r="H79" s="1"/>
       <c r="I79" s="26"/>
     </row>
-    <row r="80" spans="1:9" s="27" customFormat="1" ht="38.25">
+    <row r="80" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A80" s="65">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="2"/>
         <v>57</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="C80" s="173" t="s">
-        <v>573</v>
-      </c>
-      <c r="D80" s="24" t="s">
-        <v>586</v>
+        <v>523</v>
+      </c>
+      <c r="C80" s="154" t="s">
+        <v>685</v>
+      </c>
+      <c r="D80" s="101" t="s">
+        <v>530</v>
       </c>
       <c r="E80" s="84"/>
       <c r="F80" s="1"/>
@@ -32401,19 +32589,19 @@
       <c r="H80" s="1"/>
       <c r="I80" s="26"/>
     </row>
-    <row r="81" spans="1:9" s="27" customFormat="1" ht="51">
+    <row r="81" spans="1:9" s="27" customFormat="1" ht="12.75">
       <c r="A81" s="65">
         <f t="shared" ca="1" si="2"/>
         <v>58</v>
       </c>
-      <c r="B81" s="101" t="s">
-        <v>494</v>
-      </c>
-      <c r="C81" s="173" t="s">
-        <v>587</v>
-      </c>
-      <c r="D81" s="24" t="s">
-        <v>619</v>
+      <c r="B81" s="112" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" s="154" t="s">
+        <v>681</v>
+      </c>
+      <c r="D81" s="101" t="s">
+        <v>312</v>
       </c>
       <c r="E81" s="84"/>
       <c r="F81" s="1"/>
@@ -32421,39 +32609,32 @@
       <c r="H81" s="1"/>
       <c r="I81" s="26"/>
     </row>
-    <row r="82" spans="1:9" s="27" customFormat="1" ht="63.75">
-      <c r="A82" s="65">
+    <row r="82" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A82" s="43"/>
+      <c r="B82" s="53" t="s">
+        <v>480</v>
+      </c>
+      <c r="C82" s="150"/>
+      <c r="D82" s="62"/>
+      <c r="E82" s="83"/>
+      <c r="F82" s="64"/>
+      <c r="G82" s="64"/>
+      <c r="H82" s="64"/>
+      <c r="I82" s="63"/>
+    </row>
+    <row r="83" spans="1:9" s="27" customFormat="1" ht="51">
+      <c r="A83" s="65">
         <f t="shared" ca="1" si="2"/>
         <v>59</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C82" s="173" t="s">
-        <v>589</v>
-      </c>
-      <c r="D82" s="101" t="s">
-        <v>588</v>
-      </c>
-      <c r="E82" s="84"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="26"/>
-    </row>
-    <row r="83" spans="1:9" s="27" customFormat="1" ht="12.75">
-      <c r="A83" s="65">
-        <f t="shared" ca="1" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="B83" s="112" t="s">
-        <v>195</v>
-      </c>
-      <c r="C83" s="173" t="s">
-        <v>579</v>
-      </c>
-      <c r="D83" s="101" t="s">
-        <v>312</v>
+      <c r="B83" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="C83" s="154" t="s">
+        <v>587</v>
+      </c>
+      <c r="D83" s="24" t="s">
+        <v>532</v>
       </c>
       <c r="E83" s="84"/>
       <c r="F83" s="1"/>
@@ -32461,32 +32642,39 @@
       <c r="H83" s="1"/>
       <c r="I83" s="26"/>
     </row>
-    <row r="84" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A84" s="43"/>
-      <c r="B84" s="53" t="s">
-        <v>480</v>
-      </c>
-      <c r="C84" s="169"/>
-      <c r="D84" s="62"/>
-      <c r="E84" s="83"/>
-      <c r="F84" s="64"/>
-      <c r="G84" s="64"/>
-      <c r="H84" s="64"/>
-      <c r="I84" s="63"/>
-    </row>
-    <row r="85" spans="1:9" s="27" customFormat="1" ht="51">
+    <row r="84" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A84" s="65">
+        <f ca="1">IF(OFFSET(A84,-1,0) ="",OFFSET(A84,-2,0)+1,OFFSET(A84,-1,0)+1 )</f>
+        <v>60</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="C84" s="154" t="s">
+        <v>519</v>
+      </c>
+      <c r="D84" s="24" t="s">
+        <v>535</v>
+      </c>
+      <c r="E84" s="84"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="26"/>
+    </row>
+    <row r="85" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A85" s="65">
         <f t="shared" ca="1" si="2"/>
         <v>61</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="C85" s="173" t="s">
-        <v>593</v>
-      </c>
-      <c r="D85" s="24" t="s">
-        <v>594</v>
+        <v>489</v>
+      </c>
+      <c r="C85" s="154" t="s">
+        <v>538</v>
+      </c>
+      <c r="D85" s="102" t="s">
+        <v>533</v>
       </c>
       <c r="E85" s="84"/>
       <c r="F85" s="1"/>
@@ -32494,19 +32682,19 @@
       <c r="H85" s="1"/>
       <c r="I85" s="26"/>
     </row>
-    <row r="86" spans="1:9" s="27" customFormat="1" ht="25.5">
+    <row r="86" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A86" s="65">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">IF(OFFSET(A86,-1,0) ="",OFFSET(A86,-2,0)+1,OFFSET(A86,-1,0)+1 )</f>
         <v>62</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="C86" s="173" t="s">
-        <v>603</v>
-      </c>
-      <c r="D86" s="102" t="s">
-        <v>595</v>
+      <c r="B86" s="101" t="s">
+        <v>691</v>
+      </c>
+      <c r="C86" s="154" t="s">
+        <v>534</v>
+      </c>
+      <c r="D86" s="84" t="s">
+        <v>688</v>
       </c>
       <c r="E86" s="84"/>
       <c r="F86" s="1"/>
@@ -32514,19 +32702,19 @@
       <c r="H86" s="1"/>
       <c r="I86" s="26"/>
     </row>
-    <row r="87" spans="1:9" s="27" customFormat="1" ht="25.5">
+    <row r="87" spans="1:9" s="27" customFormat="1" ht="51">
       <c r="A87" s="65">
-        <f ca="1">IF(OFFSET(A87,-1,0) ="",OFFSET(A87,-2,0)+1,OFFSET(A87,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>63</v>
       </c>
       <c r="B87" s="101" t="s">
-        <v>198</v>
-      </c>
-      <c r="C87" s="173" t="s">
-        <v>596</v>
-      </c>
-      <c r="D87" s="84" t="s">
-        <v>605</v>
+        <v>485</v>
+      </c>
+      <c r="C87" s="154" t="s">
+        <v>536</v>
+      </c>
+      <c r="D87" s="24" t="s">
+        <v>552</v>
       </c>
       <c r="E87" s="84"/>
       <c r="F87" s="1"/>
@@ -32534,19 +32722,19 @@
       <c r="H87" s="1"/>
       <c r="I87" s="26"/>
     </row>
-    <row r="88" spans="1:9" s="27" customFormat="1" ht="25.5">
+    <row r="88" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A88" s="65">
-        <f t="shared" ref="A88:A89" ca="1" si="7">IF(OFFSET(A88,-1,0) ="",OFFSET(A88,-2,0)+1,OFFSET(A88,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>64</v>
       </c>
-      <c r="B88" s="54" t="s">
-        <v>496</v>
-      </c>
-      <c r="C88" s="173" t="s">
-        <v>597</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>598</v>
+      <c r="B88" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C88" s="154" t="s">
+        <v>692</v>
+      </c>
+      <c r="D88" s="101" t="s">
+        <v>537</v>
       </c>
       <c r="E88" s="84"/>
       <c r="F88" s="1"/>
@@ -32554,19 +32742,19 @@
       <c r="H88" s="1"/>
       <c r="I88" s="26"/>
     </row>
-    <row r="89" spans="1:9" s="27" customFormat="1" ht="38.25">
+    <row r="89" spans="1:9" s="27" customFormat="1" ht="12.75">
       <c r="A89" s="65">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="2"/>
         <v>65</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="C89" s="173" t="s">
-        <v>573</v>
-      </c>
-      <c r="D89" s="24" t="s">
-        <v>599</v>
+      <c r="B89" s="112" t="s">
+        <v>195</v>
+      </c>
+      <c r="C89" s="154" t="s">
+        <v>681</v>
+      </c>
+      <c r="D89" s="101" t="s">
+        <v>312</v>
       </c>
       <c r="E89" s="84"/>
       <c r="F89" s="1"/>
@@ -32574,92 +32762,92 @@
       <c r="H89" s="1"/>
       <c r="I89" s="26"/>
     </row>
-    <row r="90" spans="1:9" s="27" customFormat="1" ht="51">
-      <c r="A90" s="65">
-        <f t="shared" ca="1" si="2"/>
+    <row r="90" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A90" s="43"/>
+      <c r="B90" s="53" t="s">
+        <v>486</v>
+      </c>
+      <c r="C90" s="150"/>
+      <c r="D90" s="62"/>
+      <c r="E90" s="83"/>
+      <c r="F90" s="64"/>
+      <c r="G90" s="64"/>
+      <c r="H90" s="64"/>
+      <c r="I90" s="63"/>
+    </row>
+    <row r="91" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A91" s="65">
+        <f t="shared" ref="A91:A99" ca="1" si="5">IF(OFFSET(A91,-1,0) ="",OFFSET(A91,-2,0)+1,OFFSET(A91,-1,0)+1 )</f>
         <v>66</v>
       </c>
-      <c r="B90" s="101" t="s">
-        <v>497</v>
-      </c>
-      <c r="C90" s="173" t="s">
-        <v>600</v>
-      </c>
-      <c r="D90" s="24" t="s">
-        <v>619</v>
-      </c>
-      <c r="E90" s="84"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="26"/>
-    </row>
-    <row r="91" spans="1:9" s="27" customFormat="1" ht="63.75">
-      <c r="A91" s="65">
-        <f t="shared" ca="1" si="2"/>
-        <v>67</v>
-      </c>
       <c r="B91" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="C91" s="173" t="s">
-        <v>601</v>
-      </c>
-      <c r="D91" s="101" t="s">
-        <v>602</v>
+        <v>693</v>
+      </c>
+      <c r="C91" s="154" t="s">
+        <v>539</v>
+      </c>
+      <c r="D91" s="24" t="s">
+        <v>540</v>
       </c>
       <c r="E91" s="84"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
-      <c r="I91" s="26"/>
-    </row>
-    <row r="92" spans="1:9" s="27" customFormat="1" ht="12.75">
+      <c r="I91" s="67"/>
+    </row>
+    <row r="92" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A92" s="65">
-        <f t="shared" ca="1" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="B92" s="112" t="s">
-        <v>195</v>
-      </c>
-      <c r="C92" s="173" t="s">
-        <v>579</v>
-      </c>
-      <c r="D92" s="101" t="s">
-        <v>312</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>67</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C92" s="154" t="s">
+        <v>542</v>
+      </c>
+      <c r="D92" s="24" t="s">
+        <v>541</v>
       </c>
       <c r="E92" s="84"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
-      <c r="I92" s="26"/>
-    </row>
-    <row r="93" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A93" s="43"/>
-      <c r="B93" s="53" t="s">
-        <v>504</v>
-      </c>
-      <c r="C93" s="169"/>
-      <c r="D93" s="62"/>
-      <c r="E93" s="83"/>
-      <c r="F93" s="64"/>
-      <c r="G93" s="64"/>
-      <c r="H93" s="64"/>
-      <c r="I93" s="63"/>
-    </row>
-    <row r="94" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="I92" s="67"/>
+    </row>
+    <row r="93" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A93" s="65">
+        <f t="shared" ca="1" si="5"/>
+        <v>68</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="C93" s="154" t="s">
+        <v>543</v>
+      </c>
+      <c r="D93" s="24" t="s">
+        <v>544</v>
+      </c>
+      <c r="E93" s="84"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="67"/>
+    </row>
+    <row r="94" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A94" s="65">
-        <f t="shared" ref="A94:A100" ca="1" si="8">IF(OFFSET(A94,-1,0) ="",OFFSET(A94,-2,0)+1,OFFSET(A94,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="5"/>
         <v>69</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="C94" s="173" t="s">
-        <v>606</v>
+        <v>699</v>
+      </c>
+      <c r="C94" s="154" t="s">
+        <v>701</v>
       </c>
       <c r="D94" s="24" t="s">
-        <v>607</v>
+        <v>702</v>
       </c>
       <c r="E94" s="84"/>
       <c r="F94" s="1"/>
@@ -32667,39 +32855,32 @@
       <c r="H94" s="1"/>
       <c r="I94" s="67"/>
     </row>
-    <row r="95" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A95" s="65">
-        <f t="shared" ca="1" si="8"/>
+    <row r="95" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A95" s="43"/>
+      <c r="B95" s="53" t="s">
+        <v>487</v>
+      </c>
+      <c r="C95" s="150"/>
+      <c r="D95" s="62"/>
+      <c r="E95" s="83"/>
+      <c r="F95" s="64"/>
+      <c r="G95" s="64"/>
+      <c r="H95" s="64"/>
+      <c r="I95" s="63"/>
+    </row>
+    <row r="96" spans="1:9" s="29" customFormat="1" ht="14.25">
+      <c r="A96" s="65">
+        <f t="shared" ca="1" si="5"/>
         <v>70</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="C95" s="173" t="s">
-        <v>609</v>
-      </c>
-      <c r="D95" s="24" t="s">
-        <v>608</v>
-      </c>
-      <c r="E95" s="84"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="67"/>
-    </row>
-    <row r="96" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A96" s="65">
-        <f t="shared" ca="1" si="8"/>
-        <v>71</v>
-      </c>
       <c r="B96" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="C96" s="173" t="s">
-        <v>610</v>
+        <v>696</v>
+      </c>
+      <c r="C96" s="154" t="s">
+        <v>545</v>
       </c>
       <c r="D96" s="24" t="s">
-        <v>611</v>
+        <v>546</v>
       </c>
       <c r="E96" s="84"/>
       <c r="F96" s="1"/>
@@ -32707,32 +32888,39 @@
       <c r="H96" s="1"/>
       <c r="I96" s="67"/>
     </row>
-    <row r="97" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A97" s="43"/>
-      <c r="B97" s="53" t="s">
-        <v>505</v>
-      </c>
-      <c r="C97" s="169"/>
-      <c r="D97" s="62"/>
-      <c r="E97" s="83"/>
-      <c r="F97" s="64"/>
-      <c r="G97" s="64"/>
-      <c r="H97" s="64"/>
-      <c r="I97" s="63"/>
-    </row>
-    <row r="98" spans="1:9" s="29" customFormat="1" ht="14.25">
+    <row r="97" spans="1:9" s="29" customFormat="1" ht="25.5">
+      <c r="A97" s="65">
+        <f t="shared" ca="1" si="5"/>
+        <v>71</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="C97" s="154" t="s">
+        <v>547</v>
+      </c>
+      <c r="D97" s="24" t="s">
+        <v>548</v>
+      </c>
+      <c r="E97" s="84"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="67"/>
+    </row>
+    <row r="98" spans="1:9" s="29" customFormat="1" ht="25.5">
       <c r="A98" s="65">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="5"/>
         <v>72</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="C98" s="173" t="s">
-        <v>612</v>
+        <v>698</v>
+      </c>
+      <c r="C98" s="154" t="s">
+        <v>549</v>
       </c>
       <c r="D98" s="24" t="s">
-        <v>613</v>
+        <v>550</v>
       </c>
       <c r="E98" s="84"/>
       <c r="F98" s="1"/>
@@ -32740,19 +32928,19 @@
       <c r="H98" s="1"/>
       <c r="I98" s="67"/>
     </row>
-    <row r="99" spans="1:9" s="29" customFormat="1" ht="25.5">
+    <row r="99" spans="1:9" s="29" customFormat="1" ht="38.25">
       <c r="A99" s="65">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="5"/>
         <v>73</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="C99" s="173" t="s">
-        <v>614</v>
+        <v>700</v>
+      </c>
+      <c r="C99" s="154" t="s">
+        <v>704</v>
       </c>
       <c r="D99" s="24" t="s">
-        <v>615</v>
+        <v>703</v>
       </c>
       <c r="E99" s="84"/>
       <c r="F99" s="1"/>
@@ -32760,52 +32948,52 @@
       <c r="H99" s="1"/>
       <c r="I99" s="67"/>
     </row>
-    <row r="100" spans="1:9" s="29" customFormat="1" ht="25.5">
-      <c r="A100" s="65">
-        <f t="shared" ca="1" si="8"/>
+    <row r="100" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A100" s="68"/>
+      <c r="B100" s="169" t="s">
+        <v>210</v>
+      </c>
+      <c r="C100" s="170"/>
+      <c r="D100" s="171"/>
+      <c r="E100" s="86"/>
+      <c r="F100" s="32"/>
+      <c r="G100" s="32"/>
+      <c r="H100" s="32"/>
+      <c r="I100" s="69"/>
+    </row>
+    <row r="101" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A101" s="71">
+        <f t="shared" ref="A101:A108" ca="1" si="6">IF(OFFSET(A101,-1,0) ="",OFFSET(A101,-2,0)+1,OFFSET(A101,-1,0)+1 )</f>
         <v>74</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C100" s="173" t="s">
-        <v>616</v>
-      </c>
-      <c r="D100" s="24" t="s">
-        <v>617</v>
-      </c>
-      <c r="E100" s="84"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="67"/>
-    </row>
-    <row r="101" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A101" s="68"/>
-      <c r="B101" s="160" t="s">
-        <v>210</v>
-      </c>
-      <c r="C101" s="161"/>
-      <c r="D101" s="162"/>
-      <c r="E101" s="86"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="32"/>
-      <c r="H101" s="32"/>
-      <c r="I101" s="69"/>
+      <c r="B101" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C101" s="154" t="s">
+        <v>551</v>
+      </c>
+      <c r="D101" s="24" t="s">
+        <v>555</v>
+      </c>
+      <c r="E101" s="84"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="26"/>
     </row>
     <row r="102" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A102" s="71">
-        <f t="shared" ref="A102:A109" ca="1" si="9">IF(OFFSET(A102,-1,0) ="",OFFSET(A102,-2,0)+1,OFFSET(A102,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="6"/>
         <v>75</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="C102" s="173" t="s">
-        <v>618</v>
+        <v>494</v>
+      </c>
+      <c r="C102" s="154" t="s">
+        <v>557</v>
       </c>
       <c r="D102" s="24" t="s">
-        <v>622</v>
+        <v>556</v>
       </c>
       <c r="E102" s="84"/>
       <c r="F102" s="1"/>
@@ -32813,19 +33001,19 @@
       <c r="H102" s="1"/>
       <c r="I102" s="26"/>
     </row>
-    <row r="103" spans="1:9" s="27" customFormat="1" ht="38.25">
+    <row r="103" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A103" s="71">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v>76</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="C103" s="173" t="s">
-        <v>624</v>
+        <v>495</v>
+      </c>
+      <c r="C103" s="154" t="s">
+        <v>558</v>
       </c>
       <c r="D103" s="24" t="s">
-        <v>623</v>
+        <v>559</v>
       </c>
       <c r="E103" s="84"/>
       <c r="F103" s="1"/>
@@ -32833,19 +33021,19 @@
       <c r="H103" s="1"/>
       <c r="I103" s="26"/>
     </row>
-    <row r="104" spans="1:9" s="27" customFormat="1" ht="63.75">
+    <row r="104" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A104" s="71">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v>77</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="C104" s="173" t="s">
-        <v>625</v>
+        <v>488</v>
+      </c>
+      <c r="C104" s="154" t="s">
+        <v>560</v>
       </c>
       <c r="D104" s="24" t="s">
-        <v>626</v>
+        <v>561</v>
       </c>
       <c r="E104" s="84"/>
       <c r="F104" s="1"/>
@@ -32855,17 +33043,17 @@
     </row>
     <row r="105" spans="1:9" s="27" customFormat="1" ht="25.5">
       <c r="A105" s="71">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v>78</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="C105" s="173" t="s">
-        <v>627</v>
+      <c r="B105" s="54" t="s">
+        <v>491</v>
+      </c>
+      <c r="C105" s="154" t="s">
+        <v>562</v>
       </c>
       <c r="D105" s="24" t="s">
-        <v>628</v>
+        <v>564</v>
       </c>
       <c r="E105" s="84"/>
       <c r="F105" s="1"/>
@@ -32873,19 +33061,19 @@
       <c r="H105" s="1"/>
       <c r="I105" s="26"/>
     </row>
-    <row r="106" spans="1:9" s="27" customFormat="1" ht="25.5">
+    <row r="106" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A106" s="71">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v>79</v>
       </c>
       <c r="B106" s="54" t="s">
-        <v>509</v>
-      </c>
-      <c r="C106" s="173" t="s">
-        <v>629</v>
+        <v>565</v>
+      </c>
+      <c r="C106" s="154" t="s">
+        <v>563</v>
       </c>
       <c r="D106" s="24" t="s">
-        <v>631</v>
+        <v>552</v>
       </c>
       <c r="E106" s="84"/>
       <c r="F106" s="1"/>
@@ -32895,17 +33083,17 @@
     </row>
     <row r="107" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A107" s="71">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v>80</v>
       </c>
       <c r="B107" s="54" t="s">
-        <v>632</v>
-      </c>
-      <c r="C107" s="173" t="s">
-        <v>630</v>
+        <v>567</v>
+      </c>
+      <c r="C107" s="154" t="s">
+        <v>569</v>
       </c>
       <c r="D107" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E107" s="84"/>
       <c r="F107" s="1"/>
@@ -32913,19 +33101,19 @@
       <c r="H107" s="1"/>
       <c r="I107" s="26"/>
     </row>
-    <row r="108" spans="1:9" s="27" customFormat="1" ht="38.25">
+    <row r="108" spans="1:9" s="27" customFormat="1" ht="63.75">
       <c r="A108" s="71">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v>81</v>
       </c>
       <c r="B108" s="54" t="s">
-        <v>634</v>
-      </c>
-      <c r="C108" s="173" t="s">
-        <v>636</v>
+        <v>568</v>
+      </c>
+      <c r="C108" s="154" t="s">
+        <v>566</v>
       </c>
       <c r="D108" s="24" t="s">
-        <v>619</v>
+        <v>552</v>
       </c>
       <c r="E108" s="84"/>
       <c r="F108" s="1"/>
@@ -32933,25 +33121,8 @@
       <c r="H108" s="1"/>
       <c r="I108" s="26"/>
     </row>
-    <row r="109" spans="1:9" s="27" customFormat="1" ht="63.75">
-      <c r="A109" s="71">
-        <f t="shared" ca="1" si="9"/>
-        <v>82</v>
-      </c>
-      <c r="B109" s="54" t="s">
-        <v>635</v>
-      </c>
-      <c r="C109" s="173" t="s">
-        <v>633</v>
-      </c>
-      <c r="D109" s="24" t="s">
-        <v>619</v>
-      </c>
-      <c r="E109" s="84"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="I109" s="26"/>
+    <row r="109" spans="1:9" ht="12.75">
+      <c r="E109" s="87"/>
     </row>
     <row r="110" spans="1:9" ht="12.75">
       <c r="E110" s="87"/>
@@ -35569,15 +35740,12 @@
     <row r="981" spans="5:5" ht="12.75">
       <c r="E981" s="87"/>
     </row>
-    <row r="982" spans="5:5" ht="12.75">
-      <c r="E982" s="87"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A20:I109"/>
+  <autoFilter ref="A20:I108"/>
   <mergeCells count="12">
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B100:D100"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:E3"/>
@@ -35588,12 +35756,12 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="F38 F41:F42 F20:H36 F44 F94:H96 F77:H83 F68:H74 F85:H92 F98:H109 F50:H66 G38:H39 G41:H48 F40:H40 F46:F48">
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation type="list" allowBlank="1" sqref="F38 F41:F42 F20:H36 F44 F83:H89 F46:F48 F96:H108 F50:H66 G38:H39 G41:H48 F40:H40 F68:H73 F76:H81 F91:H94">
       <formula1>$A$11:$A$15</formula1>
     </dataValidation>
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F75:H76 F93:H93 F84:H84 F37:H37 F67:H67 F18:H19 F49:H49 F97:H97"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F95:H95 F90:H90 F82:H82 F37:H37 F67:H67 F18:H19 F49:H49 F74:H75"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -35603,10 +35771,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -35621,10 +35789,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" ht="14.25">
-      <c r="A1" s="152"/>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
+      <c r="A1" s="161"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -35633,13 +35801,13 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:24" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="154"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="163"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -35648,9 +35816,9 @@
     </row>
     <row r="3" spans="1:24" s="4" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="154"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="163"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -35661,11 +35829,11 @@
       <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="165"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -35679,9 +35847,9 @@
       <c r="A5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="157"/>
-      <c r="C5" s="158"/>
-      <c r="D5" s="158"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -35695,9 +35863,9 @@
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="157"/>
-      <c r="C6" s="158"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="166"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -35708,11 +35876,11 @@
       <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="158" t="s">
+      <c r="B7" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="167"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -35724,9 +35892,9 @@
       <c r="A8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="159"/>
-      <c r="C8" s="159"/>
-      <c r="D8" s="159"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="168"/>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:24" s="12" customFormat="1">
@@ -35869,11 +36037,11 @@
       <c r="C16" s="17"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
-      <c r="F16" s="148" t="s">
+      <c r="F16" s="157" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="148"/>
-      <c r="H16" s="148"/>
+      <c r="G16" s="157"/>
+      <c r="H16" s="157"/>
       <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" s="21" customFormat="1" ht="38.25">
@@ -35907,11 +36075,11 @@
     </row>
     <row r="18" spans="1:9" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="22"/>
-      <c r="B18" s="149" t="s">
-        <v>637</v>
-      </c>
-      <c r="C18" s="150"/>
-      <c r="D18" s="151"/>
+      <c r="B18" s="158" t="s">
+        <v>570</v>
+      </c>
+      <c r="C18" s="159"/>
+      <c r="D18" s="160"/>
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
@@ -35923,13 +36091,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>638</v>
+        <v>571</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>644</v>
+        <v>577</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>651</v>
+        <v>584</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="1"/>
@@ -35939,17 +36107,17 @@
     </row>
     <row r="20" spans="1:9" s="27" customFormat="1" ht="38.25">
       <c r="A20" s="2">
-        <f t="shared" ref="A20:A23" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
+        <f t="shared" ref="A20:A24" ca="1" si="0">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>641</v>
+        <v>574</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>647</v>
+        <v>580</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>642</v>
+        <v>575</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="1"/>
@@ -35963,13 +36131,13 @@
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>639</v>
+        <v>572</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>645</v>
+        <v>578</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>643</v>
+        <v>576</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="1"/>
@@ -35983,13 +36151,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>640</v>
+        <v>573</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>648</v>
+        <v>581</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>649</v>
+        <v>582</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="1"/>
@@ -36003,19 +36171,39 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>650</v>
+        <v>583</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>646</v>
+        <v>579</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>649</v>
+        <v>582</v>
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="1:9" s="27" customFormat="1" ht="38.25">
+      <c r="A24" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>582</v>
+      </c>
+      <c r="E24" s="25"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -36024,17 +36212,17 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:H18"/>
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
-    <dataValidation type="list" allowBlank="1" sqref="F19:H23">
+    <dataValidation type="list" allowBlank="1" sqref="F19:H24">
       <formula1>$A$11:$A$15</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>